<commit_message>
Change "Class" to "Item Class" in Weapons, Armaments, Potions cause class is keyword in java
</commit_message>
<xml_diff>
--- a/RDG/config/RDG.xlsx
+++ b/RDG/config/RDG.xlsx
@@ -36,88 +36,97 @@
   <connection id="5" name="D_Armaments4" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="C:\Users\Flo\git\RDG\RDG\config\Drafts\D_Armaments.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="6" name="D_Attacks" type="4" refreshedVersion="0" background="1">
+  <connection id="6" name="D_Armaments5" type="4" refreshedVersion="0" background="1">
+    <webPr xml="1" sourceData="1" url="C:\Users\Flo\git\RDG\RDG\config\Drafts\D_Armaments.xml" htmlTables="1" htmlFormat="all"/>
+  </connection>
+  <connection id="7" name="D_Attacks" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="D:\Dokumente\fh\bif\3\ITP3\Config\Drafts\D_Attacks.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="7" name="D_Attacks1" type="4" refreshedVersion="0" background="1">
+  <connection id="8" name="D_Attacks1" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="C:\Users\Flo\git\RDG\RDG\config\Drafts\D_Attacks.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="8" name="D_Monsters" type="4" refreshedVersion="0" background="1">
+  <connection id="9" name="D_Monsters" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="D:\Dokumente\fh\bif\3\ITP3\Config\Drafts\D_Monsters.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="9" name="D_Monsters1" type="4" refreshedVersion="0" background="1">
+  <connection id="10" name="D_Monsters1" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="D:\Dokumente\fh\bif\3\ITP3\Config\Drafts\D_Monsters.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="10" name="D_Monsters2" type="4" refreshedVersion="0" background="1">
+  <connection id="11" name="D_Monsters2" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="D:\Dokumente\fh\bif\3\ITP3\Config\Drafts\D_Monsters.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="11" name="D_Monsters3" type="4" refreshedVersion="0" background="1">
+  <connection id="12" name="D_Monsters3" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="D:\Dokumente\fh\bif\3\ITP3\Config\Drafts\D_Monsters.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="12" name="D_Monsters4" type="4" refreshedVersion="0" background="1">
+  <connection id="13" name="D_Monsters4" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="C:\Users\Flo\git\RDG\RDG\config\Drafts\D_Monsters.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="13" name="D_Potions" type="4" refreshedVersion="0" background="1">
+  <connection id="14" name="D_Potions" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="D:\Dokumente\fh\bif\3\ITP3\Config\Drafts\D_Potions.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="14" name="D_Potions1" type="4" refreshedVersion="0" background="1">
+  <connection id="15" name="D_Potions1" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="D:\Dokumente\fh\bif\3\ITP3\Config\Drafts\D_Potions.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="15" name="D_Potions2" type="4" refreshedVersion="0" background="1">
+  <connection id="16" name="D_Potions2" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="D:\Dokumente\fh\bif\3\ITP3\Config\Drafts\D_Potions.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="16" name="D_Potions3" type="4" refreshedVersion="0" background="1">
+  <connection id="17" name="D_Potions3" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="D:\Dokumente\fh\bif\3\ITP3\Config\Drafts\D_Potions.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="17" name="D_Potions4" type="4" refreshedVersion="0" background="1">
+  <connection id="18" name="D_Potions4" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="C:\Users\Flo\git\RDG\RDG\config\Drafts\D_Potions.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="18" name="D_Rooms" type="4" refreshedVersion="0" background="1">
+  <connection id="19" name="D_Potions5" type="4" refreshedVersion="0" background="1">
+    <webPr xml="1" sourceData="1" url="C:\Users\Flo\git\RDG\RDG\config\Drafts\D_Potions.xml" htmlTables="1" htmlFormat="all"/>
+  </connection>
+  <connection id="20" name="D_Rooms" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="D:\Dokumente\fh\bif\3\ITP3\Config\Drafts\D_Rooms.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="19" name="D_Rooms_test" type="4" refreshedVersion="0" background="1">
+  <connection id="21" name="D_Rooms_test" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="D:\Dokumente\fh\bif\3\ITP3\Config\Drafts\D_Rooms_test.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="20" name="D_Rooms1" type="4" refreshedVersion="0" background="1">
+  <connection id="22" name="D_Rooms1" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="D:\Dokumente\fh\bif\3\ITP3\Config\Drafts\D_Rooms.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="21" name="D_Rooms2" type="4" refreshedVersion="0" background="1">
+  <connection id="23" name="D_Rooms2" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="D:\Dokumente\fh\bif\3\ITP3\Config\Drafts\D_Rooms.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="22" name="D_Rooms3" type="4" refreshedVersion="0" background="1">
+  <connection id="24" name="D_Rooms3" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="D:\Dokumente\fh\bif\3\ITP3\Config\Drafts\D_Rooms.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="23" name="D_Rooms4" type="4" refreshedVersion="0" background="1">
+  <connection id="25" name="D_Rooms4" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="C:\Users\Flo\git\RDG\RDG\config\Drafts\D_Rooms.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="24" name="D_text" type="4" refreshedVersion="0" background="1">
+  <connection id="26" name="D_text" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="D:\Dokumente\fh\bif\3\ITP3\Config\Drafts\D_text.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="25" name="D_text1" type="4" refreshedVersion="0" background="1">
+  <connection id="27" name="D_text1" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="D:\Dokumente\fh\bif\3\ITP3\Config\Drafts\D_text.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="26" name="D_text2" type="4" refreshedVersion="0" background="1">
+  <connection id="28" name="D_text2" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="D:\Dokumente\fh\bif\3\ITP3\Config\Drafts\D_text.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="27" name="D_Weapons" type="4" refreshedVersion="0" background="1">
+  <connection id="29" name="D_Weapons" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="D:\Dokumente\fh\bif\3\ITP3\Config\Drafts\D_Weapons.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="28" name="D_Weapons1" type="4" refreshedVersion="0" background="1">
+  <connection id="30" name="D_Weapons1" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="D:\Dokumente\fh\bif\3\ITP3\Config\Drafts\D_Weapons.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="29" name="D_Weapons2" type="4" refreshedVersion="0" background="1">
+  <connection id="31" name="D_Weapons2" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="D:\Dokumente\fh\bif\3\ITP3\Config\Drafts\D_Weapons.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="30" name="D_Weapons3" type="4" refreshedVersion="0" background="1">
+  <connection id="32" name="D_Weapons3" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="D:\Dokumente\fh\bif\3\ITP3\Config\Drafts\D_Weapons.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="31" name="D_Weapons4" type="4" refreshedVersion="0" background="1">
+  <connection id="33" name="D_Weapons4" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="D:\Dokumente\fh\bif\3\ITP3\Config\Drafts\D_Weapons.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="32" name="D_Weapons5" type="4" refreshedVersion="0" background="1">
+  <connection id="34" name="D_Weapons5" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="C:\Users\Flo\git\RDG\RDG\config\Drafts\D_Weapons.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="33" name="Schema_Potions" type="4" refreshedVersion="0" background="1">
+  <connection id="35" name="D_Weapons6" type="4" refreshedVersion="0" background="1">
+    <webPr xml="1" sourceData="1" url="C:\Users\Flo\git\RDG\RDG\config\Drafts\D_Weapons.xml" htmlTables="1" htmlFormat="all"/>
+  </connection>
+  <connection id="36" name="Schema_Potions" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="D:\Dokumente\fh\bif\3\ITP3\Config\Schema_Potions.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
 </connections>
@@ -579,9 +588,6 @@
     <t>Treasure Chamber: hard opponents, &lt;= strong items</t>
   </si>
   <si>
-    <t>Class</t>
-  </si>
-  <si>
     <t>weak</t>
   </si>
   <si>
@@ -916,6 +922,9 @@
   </si>
   <si>
     <t>1,2</t>
+  </si>
+  <si>
+    <t>Item Class</t>
   </si>
 </sst>
 </file>
@@ -1324,6 +1333,9 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1333,336 +1345,11 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="82">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Verdana"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Verdana"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Verdana"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Verdana"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Verdana"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Verdana"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Verdana"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Verdana"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Verdana"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Verdana"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1914,6 +1601,68 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Verdana"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Verdana"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -2360,7 +2109,44 @@
         <name val="Verdana"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="30" formatCode="@"/>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Verdana"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -2434,6 +2220,7 @@
         <name val="Verdana"/>
         <scheme val="none"/>
       </font>
+      <numFmt numFmtId="30" formatCode="@"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -2441,7 +2228,7 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right/>
         <top style="thin">
@@ -2450,29 +2237,8 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -2498,6 +2264,63 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Verdana"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <border outline="0">
@@ -2725,6 +2548,68 @@
         <name val="Verdana"/>
         <scheme val="none"/>
       </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Verdana"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Verdana"/>
+        <scheme val="none"/>
+      </font>
       <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
@@ -3150,6 +3035,68 @@
         <name val="Verdana"/>
         <scheme val="none"/>
       </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Verdana"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Verdana"/>
+        <scheme val="none"/>
+      </font>
       <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
@@ -3401,6 +3348,68 @@
         <name val="Verdana"/>
         <scheme val="none"/>
       </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Verdana"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Verdana"/>
+        <scheme val="none"/>
+      </font>
       <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
@@ -3526,33 +3535,6 @@
 
 <file path=xl/xmlMaps.xml><?xml version="1.0" encoding="utf-8"?>
 <MapInfo xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" SelectionNamespaces="">
-  <Schema ID="Schema7">
-    <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns="">
-      <xsd:element nillable="true" name="Armaments">
-        <xsd:complexType>
-          <xsd:sequence minOccurs="0">
-            <xsd:element minOccurs="0" maxOccurs="unbounded" nillable="true" name="Armament" form="unqualified">
-              <xsd:complexType>
-                <xsd:sequence minOccurs="0">
-                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Name" form="unqualified"/>
-                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Class" form="unqualified"/>
-                  <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="Class_Multiplier" form="unqualified"/>
-                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Stats_Low_Multiplier" form="unqualified"/>
-                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Stats_High_Multiplier" form="unqualified"/>
-                  <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="Armor" form="unqualified"/>
-                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Speed" form="unqualified"/>
-                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Type" form="unqualified"/>
-                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Bonus" form="unqualified"/>
-                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Image_Big" form="unqualified"/>
-                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Image_Small" form="unqualified"/>
-                </xsd:sequence>
-              </xsd:complexType>
-            </xsd:element>
-          </xsd:sequence>
-        </xsd:complexType>
-      </xsd:element>
-    </xsd:schema>
-  </Schema>
   <Schema ID="Schema9">
     <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns="">
       <xsd:element nillable="true" name="Attacks">
@@ -3595,35 +3577,6 @@
                   <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Kill_Bonus_Type" form="unqualified"/>
                   <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="Kill_Bonus_Low" form="unqualified"/>
                   <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="Kill_Bonus_High" form="unqualified"/>
-                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Image_Big" form="unqualified"/>
-                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Image_Small" form="unqualified"/>
-                </xsd:sequence>
-              </xsd:complexType>
-            </xsd:element>
-          </xsd:sequence>
-        </xsd:complexType>
-      </xsd:element>
-    </xsd:schema>
-  </Schema>
-  <Schema ID="Schema11">
-    <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns="">
-      <xsd:element nillable="true" name="Potions">
-        <xsd:complexType>
-          <xsd:sequence minOccurs="0">
-            <xsd:element minOccurs="0" maxOccurs="unbounded" nillable="true" name="Potion" form="unqualified">
-              <xsd:complexType>
-                <xsd:sequence minOccurs="0">
-                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Name" form="unqualified"/>
-                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Class" form="unqualified"/>
-                  <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="Class_Multiplier" form="unqualified"/>
-                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Stats_Low_Multiplier" form="unqualified"/>
-                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Stats_High_Multiplier" form="unqualified"/>
-                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Description" form="unqualified"/>
-                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Target" form="unqualified"/>
-                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Effect" form="unqualified"/>
-                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Mode" form="unqualified"/>
-                  <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="x" form="unqualified"/>
-                  <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="n" form="unqualified"/>
                   <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Image_Big" form="unqualified"/>
                   <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Image_Small" form="unqualified"/>
                 </xsd:sequence>
@@ -3684,7 +3637,63 @@
       </xsd:element>
     </xsd:schema>
   </Schema>
-  <Schema ID="Schema15">
+  <Schema ID="Schema8">
+    <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns="">
+      <xsd:element nillable="true" name="Armaments">
+        <xsd:complexType>
+          <xsd:sequence minOccurs="0">
+            <xsd:element minOccurs="0" maxOccurs="unbounded" nillable="true" name="Armament" form="unqualified">
+              <xsd:complexType>
+                <xsd:sequence minOccurs="0">
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Name" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Item_Class" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="Class_Multiplier" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Stats_Low_Multiplier" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Stats_High_Multiplier" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="Armor" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Speed" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Type" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Bonus" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Image_Big" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Image_Small" form="unqualified"/>
+                </xsd:sequence>
+              </xsd:complexType>
+            </xsd:element>
+          </xsd:sequence>
+        </xsd:complexType>
+      </xsd:element>
+    </xsd:schema>
+  </Schema>
+  <Schema ID="Schema12">
+    <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns="">
+      <xsd:element nillable="true" name="Potions">
+        <xsd:complexType>
+          <xsd:sequence minOccurs="0">
+            <xsd:element minOccurs="0" maxOccurs="unbounded" nillable="true" name="Potion" form="unqualified">
+              <xsd:complexType>
+                <xsd:sequence minOccurs="0">
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Name" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Item_Class" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="Class_Multiplier" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Stats_Low_Multiplier" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Stats_High_Multiplier" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Description" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Target" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Effect" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Mode" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="x" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="n" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Image_Big" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Image_Small" form="unqualified"/>
+                </xsd:sequence>
+              </xsd:complexType>
+            </xsd:element>
+          </xsd:sequence>
+        </xsd:complexType>
+      </xsd:element>
+    </xsd:schema>
+  </Schema>
+  <Schema ID="Schema14">
     <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns="">
       <xsd:element nillable="true" name="Weapons">
         <xsd:complexType>
@@ -3693,7 +3702,7 @@
               <xsd:complexType>
                 <xsd:sequence minOccurs="0">
                   <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Name" form="unqualified"/>
-                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Class" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Item_Class" form="unqualified"/>
                   <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="Class_Multiplier" form="unqualified"/>
                   <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Stats_Low_Multiplier" form="unqualified"/>
                   <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Stats_High_Multiplier" form="unqualified"/>
@@ -3714,29 +3723,29 @@
       </xsd:element>
     </xsd:schema>
   </Schema>
-  <Map ID="30" Name="Armaments_Map" RootElement="Armaments" SchemaID="Schema7" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true">
-    <DataBinding FileBinding="true" ConnectionID="5" DataBindingLoadMode="1"/>
+  <Map ID="36" Name="Armaments_Map" RootElement="Armaments" SchemaID="Schema8" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true">
+    <DataBinding FileBinding="true" ConnectionID="6" DataBindingLoadMode="1"/>
   </Map>
   <Map ID="31" Name="Attacks_Map" RootElement="Attacks" SchemaID="Schema9" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true">
-    <DataBinding FileBinding="true" ConnectionID="7" DataBindingLoadMode="1"/>
+    <DataBinding FileBinding="true" ConnectionID="8" DataBindingLoadMode="1"/>
   </Map>
   <Map ID="32" Name="Monsters_Map" RootElement="Monsters" SchemaID="Schema10" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true">
-    <DataBinding FileBinding="true" ConnectionID="12" DataBindingLoadMode="1"/>
+    <DataBinding FileBinding="true" ConnectionID="13" DataBindingLoadMode="1"/>
   </Map>
-  <Map ID="33" Name="Potions_Map" RootElement="Potions" SchemaID="Schema11" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true">
-    <DataBinding FileBinding="true" ConnectionID="17" DataBindingLoadMode="1"/>
+  <Map ID="37" Name="Potions_Map" RootElement="Potions" SchemaID="Schema12" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true">
+    <DataBinding FileBinding="true" ConnectionID="19" DataBindingLoadMode="1"/>
   </Map>
   <Map ID="34" Name="Rooms_Map" RootElement="Rooms" SchemaID="Schema13" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true">
-    <DataBinding FileBinding="true" ConnectionID="23" DataBindingLoadMode="1"/>
+    <DataBinding FileBinding="true" ConnectionID="25" DataBindingLoadMode="1"/>
   </Map>
-  <Map ID="35" Name="Weapons_Map" RootElement="Weapons" SchemaID="Schema15" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true">
-    <DataBinding FileBinding="true" ConnectionID="32" DataBindingLoadMode="1"/>
+  <Map ID="38" Name="Weapons_Map" RootElement="Weapons" SchemaID="Schema14" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true">
+    <DataBinding FileBinding="true" ConnectionID="35" DataBindingLoadMode="1"/>
   </Map>
 </MapInfo>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table9" displayName="Table9" ref="A2:P8" tableType="xml" totalsRowShown="0" headerRowDxfId="81" headerRowBorderDxfId="80" connectionId="23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table9" displayName="Table9" ref="A2:P8" tableType="xml" totalsRowShown="0" headerRowDxfId="81" headerRowBorderDxfId="80" connectionId="25">
   <autoFilter ref="A2:P8"/>
   <tableColumns count="16">
     <tableColumn id="1" uniqueName="Name" name="Name">
@@ -3793,28 +3802,28 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table8" displayName="Table8" ref="A1:G5" tableType="xml" totalsRowShown="0" headerRowDxfId="79" dataDxfId="77" headerRowBorderDxfId="78" tableBorderDxfId="76" connectionId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table8" displayName="Table8" ref="A1:G5" tableType="xml" totalsRowShown="0" headerRowDxfId="79" dataDxfId="77" headerRowBorderDxfId="78" tableBorderDxfId="76" connectionId="8">
   <autoFilter ref="A1:G5"/>
   <tableColumns count="7">
     <tableColumn id="1" uniqueName="Name" name="Name" dataDxfId="75">
       <xmlColumnPr mapId="31" xpath="/Attacks/Attack/Name" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="6" uniqueName="Stats_Low_Multiplier" name="Stats Low Multiplier" dataDxfId="1">
+    <tableColumn id="6" uniqueName="Stats_Low_Multiplier" name="Stats Low Multiplier" dataDxfId="74">
       <xmlColumnPr mapId="31" xpath="/Attacks/Attack/Stats_Low_Multiplier" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="7" uniqueName="Stats_High_Multiplier" name="Stats High Multiplier" dataDxfId="0">
+    <tableColumn id="7" uniqueName="Stats_High_Multiplier" name="Stats High Multiplier" dataDxfId="73">
       <xmlColumnPr mapId="31" xpath="/Attacks/Attack/Stats_High_Multiplier" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="2" uniqueName="HP_Damage" name="HP Damage" dataDxfId="74">
+    <tableColumn id="2" uniqueName="HP_Damage" name="HP Damage" dataDxfId="72">
       <xmlColumnPr mapId="31" xpath="/Attacks/Attack/HP_Damage" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="3" uniqueName="Hit_Probability" name="Hit Probability" dataDxfId="73">
+    <tableColumn id="3" uniqueName="Hit_Probability" name="Hit Probability" dataDxfId="71">
       <xmlColumnPr mapId="31" xpath="/Attacks/Attack/Hit_Probability" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="4" uniqueName="Effect" name="Effect" dataDxfId="72">
+    <tableColumn id="4" uniqueName="Effect" name="Effect" dataDxfId="70">
       <xmlColumnPr mapId="31" xpath="/Attacks/Attack/Effect" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="5" uniqueName="x" name="x" dataDxfId="71">
+    <tableColumn id="5" uniqueName="x" name="x" dataDxfId="69">
       <xmlColumnPr mapId="31" xpath="/Attacks/Attack/x" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
@@ -3823,46 +3832,46 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="A1:M13" tableType="xml" totalsRowShown="0" headerRowDxfId="70" dataDxfId="68" headerRowBorderDxfId="69" tableBorderDxfId="67" connectionId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="A1:M13" tableType="xml" totalsRowShown="0" headerRowDxfId="68" dataDxfId="66" headerRowBorderDxfId="67" tableBorderDxfId="65" connectionId="13">
   <autoFilter ref="A1:M13"/>
   <tableColumns count="13">
-    <tableColumn id="1" uniqueName="Name" name="Name" dataDxfId="66">
+    <tableColumn id="1" uniqueName="Name" name="Name" dataDxfId="64">
       <xmlColumnPr mapId="32" xpath="/Monsters/Monster/Name" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="2" uniqueName="Level" name="Level" dataDxfId="65">
+    <tableColumn id="2" uniqueName="Level" name="Level" dataDxfId="63">
       <xmlColumnPr mapId="32" xpath="/Monsters/Monster/Level" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="10" uniqueName="Stats_Low_Multiplier" name="Stats Low Multiplier" dataDxfId="3">
+    <tableColumn id="10" uniqueName="Stats_Low_Multiplier" name="Stats Low Multiplier" dataDxfId="62">
       <xmlColumnPr mapId="32" xpath="/Monsters/Monster/Stats_Low_Multiplier" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="13" uniqueName="Stats_High_Multiplier" name="Stats High Multiplier" dataDxfId="2">
+    <tableColumn id="13" uniqueName="Stats_High_Multiplier" name="Stats High Multiplier" dataDxfId="61">
       <xmlColumnPr mapId="32" xpath="/Monsters/Monster/Stats_High_Multiplier" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="3" uniqueName="HP" name="HP" dataDxfId="64">
+    <tableColumn id="3" uniqueName="HP" name="HP" dataDxfId="60">
       <xmlColumnPr mapId="32" xpath="/Monsters/Monster/HP" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="4" uniqueName="Strength" name="Strength" dataDxfId="63">
+    <tableColumn id="4" uniqueName="Strength" name="Strength" dataDxfId="59">
       <xmlColumnPr mapId="32" xpath="/Monsters/Monster/Strength" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="5" uniqueName="Speed" name="Speed" dataDxfId="62">
+    <tableColumn id="5" uniqueName="Speed" name="Speed" dataDxfId="58">
       <xmlColumnPr mapId="32" xpath="/Monsters/Monster/Speed" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="6" uniqueName="Accuracy" name="Accuracy" dataDxfId="61">
+    <tableColumn id="6" uniqueName="Accuracy" name="Accuracy" dataDxfId="57">
       <xmlColumnPr mapId="32" xpath="/Monsters/Monster/Accuracy" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="7" uniqueName="Kill_Bonus_Type" name="Kill Bonus Type" dataDxfId="60">
+    <tableColumn id="7" uniqueName="Kill_Bonus_Type" name="Kill Bonus Type" dataDxfId="56">
       <xmlColumnPr mapId="32" xpath="/Monsters/Monster/Kill_Bonus_Type" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="8" uniqueName="Kill_Bonus_Low" name="Kill Bonus Low" dataDxfId="59">
+    <tableColumn id="8" uniqueName="Kill_Bonus_Low" name="Kill Bonus Low" dataDxfId="55">
       <xmlColumnPr mapId="32" xpath="/Monsters/Monster/Kill_Bonus_Low" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="9" uniqueName="Kill_Bonus_High" name="Kill Bonus High" dataDxfId="58">
+    <tableColumn id="9" uniqueName="Kill_Bonus_High" name="Kill Bonus High" dataDxfId="54">
       <xmlColumnPr mapId="32" xpath="/Monsters/Monster/Kill_Bonus_High" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="11" uniqueName="Image_Big" name="Image Big" dataDxfId="57">
+    <tableColumn id="11" uniqueName="Image_Big" name="Image Big" dataDxfId="53">
       <xmlColumnPr mapId="32" xpath="/Monsters/Monster/Image_Big" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="12" uniqueName="Image_Small" name="Image Small" dataDxfId="56">
+    <tableColumn id="12" uniqueName="Image_Small" name="Image Small" dataDxfId="52">
       <xmlColumnPr mapId="32" xpath="/Monsters/Monster/Image_Small" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
@@ -3871,41 +3880,41 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:K16" tableType="xml" totalsRowShown="0" headerRowDxfId="55" dataDxfId="53" headerRowBorderDxfId="54" tableBorderDxfId="52" totalsRowBorderDxfId="51" connectionId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:K16" tableType="xml" totalsRowShown="0" headerRowDxfId="51" dataDxfId="49" headerRowBorderDxfId="50" tableBorderDxfId="48" totalsRowBorderDxfId="47" connectionId="6">
   <autoFilter ref="A1:K16"/>
   <tableColumns count="11">
-    <tableColumn id="1" uniqueName="Name" name="Name" dataDxfId="50">
-      <xmlColumnPr mapId="30" xpath="/Armaments/Armament/Name" xmlDataType="string"/>
-    </tableColumn>
-    <tableColumn id="9" uniqueName="Class" name="Class" dataDxfId="49">
-      <xmlColumnPr mapId="30" xpath="/Armaments/Armament/Class" xmlDataType="string"/>
-    </tableColumn>
-    <tableColumn id="10" uniqueName="Class_Multiplier" name="Class Multiplier" dataDxfId="48">
-      <xmlColumnPr mapId="30" xpath="/Armaments/Armament/Class_Multiplier" xmlDataType="integer"/>
-    </tableColumn>
-    <tableColumn id="6" uniqueName="Stats_Low_Multiplier" name="Stats Low Multiplier" dataDxfId="5">
-      <xmlColumnPr mapId="30" xpath="/Armaments/Armament/Stats_Low_Multiplier" xmlDataType="string"/>
-    </tableColumn>
-    <tableColumn id="11" uniqueName="Stats_High_Multiplier" name="Stats High Multiplier" dataDxfId="4">
-      <xmlColumnPr mapId="30" xpath="/Armaments/Armament/Stats_High_Multiplier" xmlDataType="string"/>
-    </tableColumn>
-    <tableColumn id="2" uniqueName="Armor" name="Armor" dataDxfId="47">
-      <xmlColumnPr mapId="30" xpath="/Armaments/Armament/Armor" xmlDataType="integer"/>
-    </tableColumn>
-    <tableColumn id="3" uniqueName="Speed" name="Speed" dataDxfId="46">
-      <xmlColumnPr mapId="30" xpath="/Armaments/Armament/Speed" xmlDataType="string"/>
-    </tableColumn>
-    <tableColumn id="4" uniqueName="Type" name="Type" dataDxfId="45">
-      <xmlColumnPr mapId="30" xpath="/Armaments/Armament/Type" xmlDataType="string"/>
-    </tableColumn>
-    <tableColumn id="5" uniqueName="Bonus" name="Bonus" dataDxfId="44">
-      <xmlColumnPr mapId="30" xpath="/Armaments/Armament/Bonus" xmlDataType="string"/>
-    </tableColumn>
-    <tableColumn id="7" uniqueName="Image_Big" name="Image Big" dataDxfId="43">
-      <xmlColumnPr mapId="30" xpath="/Armaments/Armament/Image_Big" xmlDataType="string"/>
-    </tableColumn>
-    <tableColumn id="8" uniqueName="Image_Small" name="Image Small" dataDxfId="42">
-      <xmlColumnPr mapId="30" xpath="/Armaments/Armament/Image_Small" xmlDataType="string"/>
+    <tableColumn id="1" uniqueName="Name" name="Name" dataDxfId="46">
+      <xmlColumnPr mapId="36" xpath="/Armaments/Armament/Name" xmlDataType="string"/>
+    </tableColumn>
+    <tableColumn id="9" uniqueName="Item_Class" name="Item Class" dataDxfId="45">
+      <xmlColumnPr mapId="36" xpath="/Armaments/Armament/Item_Class" xmlDataType="string"/>
+    </tableColumn>
+    <tableColumn id="10" uniqueName="Class_Multiplier" name="Class Multiplier" dataDxfId="44">
+      <xmlColumnPr mapId="36" xpath="/Armaments/Armament/Class_Multiplier" xmlDataType="integer"/>
+    </tableColumn>
+    <tableColumn id="6" uniqueName="Stats_Low_Multiplier" name="Stats Low Multiplier" dataDxfId="43">
+      <xmlColumnPr mapId="36" xpath="/Armaments/Armament/Stats_Low_Multiplier" xmlDataType="string"/>
+    </tableColumn>
+    <tableColumn id="11" uniqueName="Stats_High_Multiplier" name="Stats High Multiplier" dataDxfId="42">
+      <xmlColumnPr mapId="36" xpath="/Armaments/Armament/Stats_High_Multiplier" xmlDataType="string"/>
+    </tableColumn>
+    <tableColumn id="2" uniqueName="Armor" name="Armor" dataDxfId="41">
+      <xmlColumnPr mapId="36" xpath="/Armaments/Armament/Armor" xmlDataType="integer"/>
+    </tableColumn>
+    <tableColumn id="3" uniqueName="Speed" name="Speed" dataDxfId="40">
+      <xmlColumnPr mapId="36" xpath="/Armaments/Armament/Speed" xmlDataType="string"/>
+    </tableColumn>
+    <tableColumn id="4" uniqueName="Type" name="Type" dataDxfId="39">
+      <xmlColumnPr mapId="36" xpath="/Armaments/Armament/Type" xmlDataType="string"/>
+    </tableColumn>
+    <tableColumn id="5" uniqueName="Bonus" name="Bonus" dataDxfId="38">
+      <xmlColumnPr mapId="36" xpath="/Armaments/Armament/Bonus" xmlDataType="string"/>
+    </tableColumn>
+    <tableColumn id="7" uniqueName="Image_Big" name="Image Big" dataDxfId="37">
+      <xmlColumnPr mapId="36" xpath="/Armaments/Armament/Image_Big" xmlDataType="string"/>
+    </tableColumn>
+    <tableColumn id="8" uniqueName="Image_Small" name="Image Small" dataDxfId="36">
+      <xmlColumnPr mapId="36" xpath="/Armaments/Armament/Image_Small" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -3913,47 +3922,47 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:M11" tableType="xml" totalsRowShown="0" headerRowDxfId="41" dataDxfId="39" headerRowBorderDxfId="40" tableBorderDxfId="38" totalsRowBorderDxfId="37" connectionId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:M11" tableType="xml" totalsRowShown="0" headerRowDxfId="35" dataDxfId="33" headerRowBorderDxfId="34" tableBorderDxfId="32" totalsRowBorderDxfId="31" connectionId="19">
   <autoFilter ref="A1:M11"/>
   <tableColumns count="13">
-    <tableColumn id="1" uniqueName="Name" name="Name" dataDxfId="36">
-      <xmlColumnPr mapId="33" xpath="/Potions/Potion/Name" xmlDataType="string"/>
-    </tableColumn>
-    <tableColumn id="10" uniqueName="Class" name="Class" dataDxfId="35">
-      <xmlColumnPr mapId="33" xpath="/Potions/Potion/Class" xmlDataType="string"/>
-    </tableColumn>
-    <tableColumn id="11" uniqueName="Class_Multiplier" name="Class Multiplier" dataDxfId="34">
-      <xmlColumnPr mapId="33" xpath="/Potions/Potion/Class_Multiplier" xmlDataType="integer"/>
-    </tableColumn>
-    <tableColumn id="12" uniqueName="Stats_Low_Multiplier" name="Stats Low Multiplier" dataDxfId="7">
-      <xmlColumnPr mapId="33" xpath="/Potions/Potion/Stats_Low_Multiplier" xmlDataType="string"/>
-    </tableColumn>
-    <tableColumn id="13" uniqueName="Stats_High_Multiplier" name="Stats High Multiplier" dataDxfId="6">
-      <xmlColumnPr mapId="33" xpath="/Potions/Potion/Stats_High_Multiplier" xmlDataType="string"/>
-    </tableColumn>
-    <tableColumn id="2" uniqueName="Description" name="Description" dataDxfId="33">
-      <xmlColumnPr mapId="33" xpath="/Potions/Potion/Description" xmlDataType="string"/>
-    </tableColumn>
-    <tableColumn id="3" uniqueName="Target" name="Target" dataDxfId="32">
-      <xmlColumnPr mapId="33" xpath="/Potions/Potion/Target" xmlDataType="string"/>
-    </tableColumn>
-    <tableColumn id="4" uniqueName="Effect" name="Effect" dataDxfId="31">
-      <xmlColumnPr mapId="33" xpath="/Potions/Potion/Effect" xmlDataType="string"/>
-    </tableColumn>
-    <tableColumn id="5" uniqueName="Mode" name="Mode" dataDxfId="30">
-      <xmlColumnPr mapId="33" xpath="/Potions/Potion/Mode" xmlDataType="string"/>
-    </tableColumn>
-    <tableColumn id="6" uniqueName="x" name="x" dataDxfId="29">
-      <xmlColumnPr mapId="33" xpath="/Potions/Potion/x" xmlDataType="integer"/>
-    </tableColumn>
-    <tableColumn id="7" uniqueName="n" name="n" dataDxfId="28">
-      <xmlColumnPr mapId="33" xpath="/Potions/Potion/n" xmlDataType="integer"/>
-    </tableColumn>
-    <tableColumn id="8" uniqueName="Image_Big" name="Image Big" dataDxfId="27">
-      <xmlColumnPr mapId="33" xpath="/Potions/Potion/Image_Big" xmlDataType="string"/>
-    </tableColumn>
-    <tableColumn id="9" uniqueName="Image_Small" name="Image Small" dataDxfId="26">
-      <xmlColumnPr mapId="33" xpath="/Potions/Potion/Image_Small" xmlDataType="string"/>
+    <tableColumn id="1" uniqueName="Name" name="Name" dataDxfId="30">
+      <xmlColumnPr mapId="37" xpath="/Potions/Potion/Name" xmlDataType="string"/>
+    </tableColumn>
+    <tableColumn id="10" uniqueName="Item_Class" name="Item Class" dataDxfId="29">
+      <xmlColumnPr mapId="37" xpath="/Potions/Potion/Item_Class" xmlDataType="string"/>
+    </tableColumn>
+    <tableColumn id="11" uniqueName="Class_Multiplier" name="Class Multiplier" dataDxfId="28">
+      <xmlColumnPr mapId="37" xpath="/Potions/Potion/Class_Multiplier" xmlDataType="integer"/>
+    </tableColumn>
+    <tableColumn id="12" uniqueName="Stats_Low_Multiplier" name="Stats Low Multiplier" dataDxfId="27">
+      <xmlColumnPr mapId="37" xpath="/Potions/Potion/Stats_Low_Multiplier" xmlDataType="string"/>
+    </tableColumn>
+    <tableColumn id="13" uniqueName="Stats_High_Multiplier" name="Stats High Multiplier" dataDxfId="26">
+      <xmlColumnPr mapId="37" xpath="/Potions/Potion/Stats_High_Multiplier" xmlDataType="string"/>
+    </tableColumn>
+    <tableColumn id="2" uniqueName="Description" name="Description" dataDxfId="25">
+      <xmlColumnPr mapId="37" xpath="/Potions/Potion/Description" xmlDataType="string"/>
+    </tableColumn>
+    <tableColumn id="3" uniqueName="Target" name="Target" dataDxfId="24">
+      <xmlColumnPr mapId="37" xpath="/Potions/Potion/Target" xmlDataType="string"/>
+    </tableColumn>
+    <tableColumn id="4" uniqueName="Effect" name="Effect" dataDxfId="23">
+      <xmlColumnPr mapId="37" xpath="/Potions/Potion/Effect" xmlDataType="string"/>
+    </tableColumn>
+    <tableColumn id="5" uniqueName="Mode" name="Mode" dataDxfId="22">
+      <xmlColumnPr mapId="37" xpath="/Potions/Potion/Mode" xmlDataType="string"/>
+    </tableColumn>
+    <tableColumn id="6" uniqueName="x" name="x" dataDxfId="21">
+      <xmlColumnPr mapId="37" xpath="/Potions/Potion/x" xmlDataType="integer"/>
+    </tableColumn>
+    <tableColumn id="7" uniqueName="n" name="n" dataDxfId="20">
+      <xmlColumnPr mapId="37" xpath="/Potions/Potion/n" xmlDataType="integer"/>
+    </tableColumn>
+    <tableColumn id="8" uniqueName="Image_Big" name="Image Big" dataDxfId="19">
+      <xmlColumnPr mapId="37" xpath="/Potions/Potion/Image_Big" xmlDataType="string"/>
+    </tableColumn>
+    <tableColumn id="9" uniqueName="Image_Small" name="Image Small" dataDxfId="18">
+      <xmlColumnPr mapId="37" xpath="/Potions/Potion/Image_Small" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -3961,51 +3970,51 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:N9" tableType="xml" totalsRowShown="0" headerRowDxfId="25" dataDxfId="23" headerRowBorderDxfId="24" tableBorderDxfId="22" connectionId="32">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:N9" tableType="xml" totalsRowShown="0" headerRowDxfId="17" dataDxfId="15" headerRowBorderDxfId="16" tableBorderDxfId="14" connectionId="35">
   <autoFilter ref="A1:N9"/>
   <tableColumns count="14">
-    <tableColumn id="1" uniqueName="Name" name="Name" dataDxfId="21">
-      <xmlColumnPr mapId="35" xpath="/Weapons/Weapon/Name" xmlDataType="string"/>
-    </tableColumn>
-    <tableColumn id="11" uniqueName="Class" name="Class" dataDxfId="20">
-      <xmlColumnPr mapId="35" xpath="/Weapons/Weapon/Class" xmlDataType="string"/>
-    </tableColumn>
-    <tableColumn id="12" uniqueName="Class_Multiplier" name="Class Multiplier" dataDxfId="19">
-      <xmlColumnPr mapId="35" xpath="/Weapons/Weapon/Class_Multiplier" xmlDataType="integer"/>
-    </tableColumn>
-    <tableColumn id="13" uniqueName="Stats_Low_Multiplier" name="Stats Low Multiplier" dataDxfId="9">
-      <xmlColumnPr mapId="35" xpath="/Weapons/Weapon/Stats_Low_Multiplier" xmlDataType="string"/>
-    </tableColumn>
-    <tableColumn id="14" uniqueName="Stats_High_Multiplier" name="Stats High Multiplier" dataDxfId="8">
-      <xmlColumnPr mapId="35" xpath="/Weapons/Weapon/Stats_High_Multiplier" xmlDataType="string"/>
-    </tableColumn>
-    <tableColumn id="2" uniqueName="Attack" name="Attack" dataDxfId="18">
-      <xmlColumnPr mapId="35" xpath="/Weapons/Weapon/Attack" xmlDataType="integer"/>
-    </tableColumn>
-    <tableColumn id="3" uniqueName="Speed" name="Speed" dataDxfId="17">
-      <xmlColumnPr mapId="35" xpath="/Weapons/Weapon/Speed" xmlDataType="integer"/>
-    </tableColumn>
-    <tableColumn id="4" uniqueName="Accuracy" name="Accuracy" dataDxfId="16">
-      <xmlColumnPr mapId="35" xpath="/Weapons/Weapon/Accuracy" xmlDataType="integer"/>
-    </tableColumn>
-    <tableColumn id="5" uniqueName="Defence" name="Defence" dataDxfId="15">
+    <tableColumn id="1" uniqueName="Name" name="Name" dataDxfId="13">
+      <xmlColumnPr mapId="38" xpath="/Weapons/Weapon/Name" xmlDataType="string"/>
+    </tableColumn>
+    <tableColumn id="11" uniqueName="Item_Class" name="Item Class" dataDxfId="12">
+      <xmlColumnPr mapId="38" xpath="/Weapons/Weapon/Item_Class" xmlDataType="string"/>
+    </tableColumn>
+    <tableColumn id="12" uniqueName="Class_Multiplier" name="Class Multiplier" dataDxfId="11">
+      <xmlColumnPr mapId="38" xpath="/Weapons/Weapon/Class_Multiplier" xmlDataType="integer"/>
+    </tableColumn>
+    <tableColumn id="13" uniqueName="Stats_Low_Multiplier" name="Stats Low Multiplier" dataDxfId="10">
+      <xmlColumnPr mapId="38" xpath="/Weapons/Weapon/Stats_Low_Multiplier" xmlDataType="string"/>
+    </tableColumn>
+    <tableColumn id="14" uniqueName="Stats_High_Multiplier" name="Stats High Multiplier" dataDxfId="9">
+      <xmlColumnPr mapId="38" xpath="/Weapons/Weapon/Stats_High_Multiplier" xmlDataType="string"/>
+    </tableColumn>
+    <tableColumn id="2" uniqueName="Attack" name="Attack" dataDxfId="8">
+      <xmlColumnPr mapId="38" xpath="/Weapons/Weapon/Attack" xmlDataType="integer"/>
+    </tableColumn>
+    <tableColumn id="3" uniqueName="Speed" name="Speed" dataDxfId="7">
+      <xmlColumnPr mapId="38" xpath="/Weapons/Weapon/Speed" xmlDataType="integer"/>
+    </tableColumn>
+    <tableColumn id="4" uniqueName="Accuracy" name="Accuracy" dataDxfId="6">
+      <xmlColumnPr mapId="38" xpath="/Weapons/Weapon/Accuracy" xmlDataType="integer"/>
+    </tableColumn>
+    <tableColumn id="5" uniqueName="Defence" name="Defence" dataDxfId="5">
       <calculatedColumnFormula>"-"</calculatedColumnFormula>
-      <xmlColumnPr mapId="35" xpath="/Weapons/Weapon/Defence" xmlDataType="string"/>
-    </tableColumn>
-    <tableColumn id="6" uniqueName="Slots" name="Slots" dataDxfId="14">
-      <xmlColumnPr mapId="35" xpath="/Weapons/Weapon/Slots" xmlDataType="integer"/>
-    </tableColumn>
-    <tableColumn id="7" uniqueName="Max" name="Max" dataDxfId="13">
-      <xmlColumnPr mapId="35" xpath="/Weapons/Weapon/Max" xmlDataType="integer"/>
-    </tableColumn>
-    <tableColumn id="8" uniqueName="Type" name="Type" dataDxfId="12">
-      <xmlColumnPr mapId="35" xpath="/Weapons/Weapon/Type" xmlDataType="string"/>
-    </tableColumn>
-    <tableColumn id="9" uniqueName="Image_Big" name="Image Big" dataDxfId="11">
-      <xmlColumnPr mapId="35" xpath="/Weapons/Weapon/Image_Big" xmlDataType="string"/>
-    </tableColumn>
-    <tableColumn id="10" uniqueName="Image_Small" name="Image Small" dataDxfId="10">
-      <xmlColumnPr mapId="35" xpath="/Weapons/Weapon/Image_Small" xmlDataType="string"/>
+      <xmlColumnPr mapId="38" xpath="/Weapons/Weapon/Defence" xmlDataType="string"/>
+    </tableColumn>
+    <tableColumn id="6" uniqueName="Slots" name="Slots" dataDxfId="4">
+      <xmlColumnPr mapId="38" xpath="/Weapons/Weapon/Slots" xmlDataType="integer"/>
+    </tableColumn>
+    <tableColumn id="7" uniqueName="Max" name="Max" dataDxfId="3">
+      <xmlColumnPr mapId="38" xpath="/Weapons/Weapon/Max" xmlDataType="integer"/>
+    </tableColumn>
+    <tableColumn id="8" uniqueName="Type" name="Type" dataDxfId="2">
+      <xmlColumnPr mapId="38" xpath="/Weapons/Weapon/Type" xmlDataType="string"/>
+    </tableColumn>
+    <tableColumn id="9" uniqueName="Image_Big" name="Image Big" dataDxfId="1">
+      <xmlColumnPr mapId="38" xpath="/Weapons/Weapon/Image_Big" xmlDataType="string"/>
+    </tableColumn>
+    <tableColumn id="10" uniqueName="Image_Small" name="Image Small" dataDxfId="0">
+      <xmlColumnPr mapId="38" xpath="/Weapons/Weapon/Image_Small" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -4354,24 +4363,24 @@
     <row r="1" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
       <c r="B1" s="6"/>
-      <c r="C1" s="59" t="s">
+      <c r="C1" s="60" t="s">
         <v>127</v>
       </c>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="59" t="s">
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="60" t="s">
         <v>122</v>
       </c>
-      <c r="H1" s="60"/>
-      <c r="I1" s="60"/>
-      <c r="J1" s="61"/>
+      <c r="H1" s="61"/>
+      <c r="I1" s="61"/>
+      <c r="J1" s="62"/>
       <c r="K1" s="56"/>
-      <c r="L1" s="59" t="s">
-        <v>158</v>
-      </c>
-      <c r="M1" s="60"/>
-      <c r="N1" s="61"/>
+      <c r="L1" s="60" t="s">
+        <v>157</v>
+      </c>
+      <c r="M1" s="61"/>
+      <c r="N1" s="62"/>
       <c r="O1" s="56"/>
       <c r="P1" s="56"/>
     </row>
@@ -4407,19 +4416,19 @@
         <v>83</v>
       </c>
       <c r="K2" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="L2" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="M2" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="N2" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="O2" s="7" t="s">
         <v>162</v>
-      </c>
-      <c r="L2" s="8" t="s">
-        <v>152</v>
-      </c>
-      <c r="M2" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="N2" s="8" t="s">
-        <v>154</v>
-      </c>
-      <c r="O2" s="7" t="s">
-        <v>163</v>
       </c>
       <c r="P2" s="7" t="s">
         <v>124</v>
@@ -4472,7 +4481,7 @@
         <v>3</v>
       </c>
       <c r="P3" s="57" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
@@ -4522,7 +4531,7 @@
         <v>2</v>
       </c>
       <c r="P4" s="57" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
@@ -4572,7 +4581,7 @@
         <v>2</v>
       </c>
       <c r="P5" s="57" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
@@ -4622,7 +4631,7 @@
         <v>1</v>
       </c>
       <c r="P6" s="57" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
@@ -4672,7 +4681,7 @@
         <v>1</v>
       </c>
       <c r="P7" s="57" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
@@ -4722,31 +4731,31 @@
         <v>5</v>
       </c>
       <c r="P8" s="57" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>148</v>
       </c>
-      <c r="C10" s="62" t="s">
+      <c r="C10" s="59" t="s">
         <v>133</v>
       </c>
-      <c r="D10" s="62"/>
-      <c r="E10" s="62"/>
-      <c r="F10" s="62"/>
-      <c r="G10" s="62" t="s">
+      <c r="D10" s="59"/>
+      <c r="E10" s="59"/>
+      <c r="F10" s="59"/>
+      <c r="G10" s="59" t="s">
         <v>132</v>
       </c>
-      <c r="H10" s="62"/>
-      <c r="I10" s="62"/>
-      <c r="J10" s="62"/>
+      <c r="H10" s="59"/>
+      <c r="I10" s="59"/>
+      <c r="J10" s="59"/>
       <c r="K10" s="38"/>
-      <c r="L10" s="62" t="s">
-        <v>159</v>
-      </c>
-      <c r="M10" s="62"/>
-      <c r="N10" s="62"/>
+      <c r="L10" s="59" t="s">
+        <v>158</v>
+      </c>
+      <c r="M10" s="59"/>
+      <c r="N10" s="59"/>
       <c r="O10" s="38"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
@@ -4775,7 +4784,7 @@
       <c r="J12" s="39"/>
       <c r="K12" s="39"/>
       <c r="L12" s="39" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="M12" s="39"/>
       <c r="N12" s="39"/>
@@ -4791,19 +4800,19 @@
       <c r="J13" s="39"/>
       <c r="K13" s="39"/>
       <c r="L13" s="39" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="M13" s="39"/>
       <c r="N13" s="39"/>
       <c r="O13" s="39"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="G14" s="62" t="s">
+      <c r="G14" s="59" t="s">
         <v>134</v>
       </c>
-      <c r="H14" s="62"/>
-      <c r="I14" s="62"/>
-      <c r="J14" s="62"/>
+      <c r="H14" s="59"/>
+      <c r="I14" s="59"/>
+      <c r="J14" s="59"/>
       <c r="K14" s="38"/>
       <c r="L14" s="38"/>
       <c r="M14" s="38"/>
@@ -4814,12 +4823,12 @@
       <c r="A15" t="s">
         <v>147</v>
       </c>
-      <c r="G15" s="62" t="s">
+      <c r="G15" s="59" t="s">
         <v>135</v>
       </c>
-      <c r="H15" s="62"/>
-      <c r="I15" s="62"/>
-      <c r="J15" s="62"/>
+      <c r="H15" s="59"/>
+      <c r="I15" s="59"/>
+      <c r="J15" s="59"/>
       <c r="K15" s="38"/>
       <c r="L15" s="38"/>
       <c r="M15" s="38"/>
@@ -4827,12 +4836,12 @@
       <c r="O15" s="38"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="G16" s="62" t="s">
+      <c r="G16" s="59" t="s">
         <v>136</v>
       </c>
-      <c r="H16" s="62"/>
-      <c r="I16" s="62"/>
-      <c r="J16" s="62"/>
+      <c r="H16" s="59"/>
+      <c r="I16" s="59"/>
+      <c r="J16" s="59"/>
       <c r="K16" s="38"/>
       <c r="L16" s="38"/>
       <c r="M16" s="38"/>
@@ -4840,12 +4849,12 @@
       <c r="O16" s="38"/>
     </row>
     <row r="17" spans="7:15" x14ac:dyDescent="0.25">
-      <c r="G17" s="62" t="s">
+      <c r="G17" s="59" t="s">
         <v>137</v>
       </c>
-      <c r="H17" s="62"/>
-      <c r="I17" s="62"/>
-      <c r="J17" s="62"/>
+      <c r="H17" s="59"/>
+      <c r="I17" s="59"/>
+      <c r="J17" s="59"/>
       <c r="K17" s="38"/>
       <c r="L17" s="38"/>
       <c r="M17" s="38"/>
@@ -4853,12 +4862,12 @@
       <c r="O17" s="38"/>
     </row>
     <row r="18" spans="7:15" x14ac:dyDescent="0.25">
-      <c r="G18" s="62" t="s">
+      <c r="G18" s="59" t="s">
         <v>138</v>
       </c>
-      <c r="H18" s="62"/>
-      <c r="I18" s="62"/>
-      <c r="J18" s="62"/>
+      <c r="H18" s="59"/>
+      <c r="I18" s="59"/>
+      <c r="J18" s="59"/>
       <c r="K18" s="38"/>
       <c r="L18" s="38"/>
       <c r="M18" s="38"/>
@@ -4866,12 +4875,12 @@
       <c r="O18" s="38"/>
     </row>
     <row r="20" spans="7:15" x14ac:dyDescent="0.25">
-      <c r="G20" s="62" t="s">
+      <c r="G20" s="59" t="s">
         <v>139</v>
       </c>
-      <c r="H20" s="62"/>
-      <c r="I20" s="62"/>
-      <c r="J20" s="62"/>
+      <c r="H20" s="59"/>
+      <c r="I20" s="59"/>
+      <c r="J20" s="59"/>
       <c r="K20" s="38"/>
       <c r="L20" s="38"/>
       <c r="M20" s="38"/>
@@ -4879,12 +4888,12 @@
       <c r="O20" s="38"/>
     </row>
     <row r="21" spans="7:15" x14ac:dyDescent="0.25">
-      <c r="G21" s="62" t="s">
+      <c r="G21" s="59" t="s">
         <v>140</v>
       </c>
-      <c r="H21" s="62"/>
-      <c r="I21" s="62"/>
-      <c r="J21" s="62"/>
+      <c r="H21" s="59"/>
+      <c r="I21" s="59"/>
+      <c r="J21" s="59"/>
       <c r="K21" s="38"/>
       <c r="L21" s="38"/>
       <c r="M21" s="38"/>
@@ -4897,12 +4906,12 @@
       </c>
     </row>
     <row r="24" spans="7:15" x14ac:dyDescent="0.25">
-      <c r="G24" s="62" t="s">
+      <c r="G24" s="59" t="s">
         <v>141</v>
       </c>
-      <c r="H24" s="62"/>
-      <c r="I24" s="62"/>
-      <c r="J24" s="62"/>
+      <c r="H24" s="59"/>
+      <c r="I24" s="59"/>
+      <c r="J24" s="59"/>
       <c r="K24" s="38"/>
       <c r="L24" s="38"/>
       <c r="M24" s="38"/>
@@ -4910,12 +4919,12 @@
       <c r="O24" s="38"/>
     </row>
     <row r="25" spans="7:15" x14ac:dyDescent="0.25">
-      <c r="G25" s="62" t="s">
+      <c r="G25" s="59" t="s">
         <v>142</v>
       </c>
-      <c r="H25" s="62"/>
-      <c r="I25" s="62"/>
-      <c r="J25" s="62"/>
+      <c r="H25" s="59"/>
+      <c r="I25" s="59"/>
+      <c r="J25" s="59"/>
       <c r="K25" s="38"/>
       <c r="L25" s="38"/>
       <c r="M25" s="38"/>
@@ -4923,12 +4932,12 @@
       <c r="O25" s="38"/>
     </row>
     <row r="26" spans="7:15" x14ac:dyDescent="0.25">
-      <c r="G26" s="62" t="s">
+      <c r="G26" s="59" t="s">
         <v>144</v>
       </c>
-      <c r="H26" s="62"/>
-      <c r="I26" s="62"/>
-      <c r="J26" s="62"/>
+      <c r="H26" s="59"/>
+      <c r="I26" s="59"/>
+      <c r="J26" s="59"/>
       <c r="K26" s="38"/>
       <c r="L26" s="38"/>
       <c r="M26" s="38"/>
@@ -4937,6 +4946,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="G1:J1"/>
+    <mergeCell ref="L1:N1"/>
+    <mergeCell ref="L10:N10"/>
+    <mergeCell ref="G25:J25"/>
     <mergeCell ref="G26:J26"/>
     <mergeCell ref="C10:F10"/>
     <mergeCell ref="G10:J10"/>
@@ -4948,11 +4962,6 @@
     <mergeCell ref="G17:J17"/>
     <mergeCell ref="G18:J18"/>
     <mergeCell ref="G21:J21"/>
-    <mergeCell ref="C1:F1"/>
-    <mergeCell ref="G1:J1"/>
-    <mergeCell ref="L1:N1"/>
-    <mergeCell ref="L10:N10"/>
-    <mergeCell ref="G25:J25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -4986,10 +4995,10 @@
         <v>41</v>
       </c>
       <c r="B1" s="40" t="s">
+        <v>259</v>
+      </c>
+      <c r="C1" s="40" t="s">
         <v>260</v>
-      </c>
-      <c r="C1" s="40" t="s">
-        <v>261</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>106</v>
@@ -5009,10 +5018,10 @@
         <v>102</v>
       </c>
       <c r="B2" s="44" t="s">
+        <v>261</v>
+      </c>
+      <c r="C2" s="44" t="s">
         <v>262</v>
-      </c>
-      <c r="C2" s="44" t="s">
-        <v>263</v>
       </c>
       <c r="D2" s="44">
         <v>0.5</v>
@@ -5033,10 +5042,10 @@
         <v>103</v>
       </c>
       <c r="B3" s="44" t="s">
+        <v>261</v>
+      </c>
+      <c r="C3" s="42" t="s">
         <v>262</v>
-      </c>
-      <c r="C3" s="42" t="s">
-        <v>263</v>
       </c>
       <c r="D3" s="42">
         <v>0.7</v>
@@ -5056,10 +5065,10 @@
         <v>104</v>
       </c>
       <c r="B4" s="44" t="s">
+        <v>261</v>
+      </c>
+      <c r="C4" s="44" t="s">
         <v>262</v>
-      </c>
-      <c r="C4" s="44" t="s">
-        <v>263</v>
       </c>
       <c r="D4" s="42">
         <v>0.3</v>
@@ -5079,10 +5088,10 @@
         <v>105</v>
       </c>
       <c r="B5" s="44" t="s">
+        <v>261</v>
+      </c>
+      <c r="C5" s="42" t="s">
         <v>262</v>
-      </c>
-      <c r="C5" s="42" t="s">
-        <v>263</v>
       </c>
       <c r="D5" s="43">
         <v>0.4</v>
@@ -5158,10 +5167,10 @@
         <v>98</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>260</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>261</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>80</v>
@@ -5199,10 +5208,10 @@
         <v>81</v>
       </c>
       <c r="C2" s="33" t="s">
+        <v>261</v>
+      </c>
+      <c r="D2" s="33" t="s">
         <v>262</v>
-      </c>
-      <c r="D2" s="33" t="s">
-        <v>263</v>
       </c>
       <c r="E2" s="29">
         <v>20</v>
@@ -5226,10 +5235,10 @@
         <v>4</v>
       </c>
       <c r="L2" s="17" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="M2" s="17" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5240,10 +5249,10 @@
         <v>81</v>
       </c>
       <c r="C3" s="34" t="s">
+        <v>261</v>
+      </c>
+      <c r="D3" s="34" t="s">
         <v>262</v>
-      </c>
-      <c r="D3" s="34" t="s">
-        <v>263</v>
       </c>
       <c r="E3" s="30">
         <v>25</v>
@@ -5267,10 +5276,10 @@
         <v>2</v>
       </c>
       <c r="L3" s="17" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="M3" s="17" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5281,10 +5290,10 @@
         <v>81</v>
       </c>
       <c r="C4" s="33" t="s">
+        <v>261</v>
+      </c>
+      <c r="D4" s="33" t="s">
         <v>262</v>
-      </c>
-      <c r="D4" s="33" t="s">
-        <v>263</v>
       </c>
       <c r="E4" s="30">
         <v>15</v>
@@ -5308,10 +5317,10 @@
         <v>2</v>
       </c>
       <c r="L4" s="17" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="M4" s="17" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5322,10 +5331,10 @@
         <v>81</v>
       </c>
       <c r="C5" s="34" t="s">
+        <v>261</v>
+      </c>
+      <c r="D5" s="34" t="s">
         <v>262</v>
-      </c>
-      <c r="D5" s="34" t="s">
-        <v>263</v>
       </c>
       <c r="E5" s="30">
         <v>25</v>
@@ -5349,10 +5358,10 @@
         <v>2</v>
       </c>
       <c r="L5" s="17" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="M5" s="17" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5363,10 +5372,10 @@
         <v>81</v>
       </c>
       <c r="C6" s="33" t="s">
+        <v>261</v>
+      </c>
+      <c r="D6" s="33" t="s">
         <v>262</v>
-      </c>
-      <c r="D6" s="33" t="s">
-        <v>263</v>
       </c>
       <c r="E6" s="30">
         <v>15</v>
@@ -5390,10 +5399,10 @@
         <v>2</v>
       </c>
       <c r="L6" s="17" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="M6" s="17" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5404,10 +5413,10 @@
         <v>82</v>
       </c>
       <c r="C7" s="34" t="s">
+        <v>261</v>
+      </c>
+      <c r="D7" s="34" t="s">
         <v>262</v>
-      </c>
-      <c r="D7" s="34" t="s">
-        <v>263</v>
       </c>
       <c r="E7" s="30">
         <v>35</v>
@@ -5431,10 +5440,10 @@
         <v>5</v>
       </c>
       <c r="L7" s="17" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="M7" s="17" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5445,10 +5454,10 @@
         <v>82</v>
       </c>
       <c r="C8" s="33" t="s">
+        <v>261</v>
+      </c>
+      <c r="D8" s="33" t="s">
         <v>262</v>
-      </c>
-      <c r="D8" s="33" t="s">
-        <v>263</v>
       </c>
       <c r="E8" s="30">
         <v>40</v>
@@ -5472,10 +5481,10 @@
         <v>7</v>
       </c>
       <c r="L8" s="17" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="M8" s="17" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5486,10 +5495,10 @@
         <v>82</v>
       </c>
       <c r="C9" s="34" t="s">
+        <v>261</v>
+      </c>
+      <c r="D9" s="34" t="s">
         <v>262</v>
-      </c>
-      <c r="D9" s="34" t="s">
-        <v>263</v>
       </c>
       <c r="E9" s="30">
         <v>45</v>
@@ -5513,10 +5522,10 @@
         <v>5</v>
       </c>
       <c r="L9" s="17" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="M9" s="17" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5527,10 +5536,10 @@
         <v>82</v>
       </c>
       <c r="C10" s="33" t="s">
+        <v>261</v>
+      </c>
+      <c r="D10" s="33" t="s">
         <v>262</v>
-      </c>
-      <c r="D10" s="33" t="s">
-        <v>263</v>
       </c>
       <c r="E10" s="30">
         <v>55</v>
@@ -5554,10 +5563,10 @@
         <v>10</v>
       </c>
       <c r="L10" s="17" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M10" s="17" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5568,10 +5577,10 @@
         <v>83</v>
       </c>
       <c r="C11" s="34" t="s">
+        <v>261</v>
+      </c>
+      <c r="D11" s="34" t="s">
         <v>262</v>
-      </c>
-      <c r="D11" s="34" t="s">
-        <v>263</v>
       </c>
       <c r="E11" s="30">
         <v>60</v>
@@ -5595,10 +5604,10 @@
         <v>30</v>
       </c>
       <c r="L11" s="17" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M11" s="17" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5609,10 +5618,10 @@
         <v>83</v>
       </c>
       <c r="C12" s="33" t="s">
+        <v>261</v>
+      </c>
+      <c r="D12" s="33" t="s">
         <v>262</v>
-      </c>
-      <c r="D12" s="33" t="s">
-        <v>263</v>
       </c>
       <c r="E12" s="30">
         <v>80</v>
@@ -5636,10 +5645,10 @@
         <v>30</v>
       </c>
       <c r="L12" s="17" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="M12" s="17" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5650,10 +5659,10 @@
         <v>83</v>
       </c>
       <c r="C13" s="34" t="s">
+        <v>261</v>
+      </c>
+      <c r="D13" s="34" t="s">
         <v>262</v>
-      </c>
-      <c r="D13" s="34" t="s">
-        <v>263</v>
       </c>
       <c r="E13" s="31">
         <v>70</v>
@@ -5677,10 +5686,10 @@
         <v>30</v>
       </c>
       <c r="L13" s="17" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="M13" s="17" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
@@ -5726,14 +5735,14 @@
   <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="L26" sqref="L26"/>
+      <pane xSplit="1" topLeftCell="I1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.7109375" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" customWidth="1"/>
     <col min="3" max="3" width="18.28515625" customWidth="1"/>
     <col min="4" max="4" width="23.85546875" customWidth="1"/>
     <col min="5" max="5" width="23.7109375" customWidth="1"/>
@@ -5750,16 +5759,16 @@
         <v>41</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>151</v>
+        <v>263</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D1" s="10" t="s">
+        <v>259</v>
+      </c>
+      <c r="E1" s="10" t="s">
         <v>260</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>261</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>78</v>
@@ -5785,10 +5794,10 @@
         <v>61</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C2" s="51" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D2" s="17">
         <v>0.8</v>
@@ -5811,10 +5820,10 @@
         <v>0.1</v>
       </c>
       <c r="J2" s="17" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="K2" s="17" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5822,10 +5831,10 @@
         <v>62</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C3" s="52" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D3" s="13">
         <v>0.8</v>
@@ -5846,10 +5855,10 @@
         <v>0.1</v>
       </c>
       <c r="J3" s="17" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="K3" s="17" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5857,10 +5866,10 @@
         <v>63</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C4" s="52" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D4" s="17">
         <v>0.8</v>
@@ -5883,10 +5892,10 @@
         <v>0.1</v>
       </c>
       <c r="J4" s="17" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="K4" s="17" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5894,10 +5903,10 @@
         <v>64</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C5" s="52" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D5" s="13">
         <v>0.8</v>
@@ -5920,10 +5929,10 @@
         <v>0.1</v>
       </c>
       <c r="J5" s="17" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="K5" s="17" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5931,10 +5940,10 @@
         <v>65</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C6" s="52" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D6" s="17">
         <v>0.8</v>
@@ -5957,10 +5966,10 @@
         <v>0.1</v>
       </c>
       <c r="J6" s="17" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K6" s="17" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5968,10 +5977,10 @@
         <v>66</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C7" s="52" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D7" s="13">
         <v>0.8</v>
@@ -5994,10 +6003,10 @@
         <v>0.15</v>
       </c>
       <c r="J7" s="17" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="K7" s="17" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6005,10 +6014,10 @@
         <v>67</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C8" s="52" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D8" s="17">
         <v>0.8</v>
@@ -6029,10 +6038,10 @@
         <v>0.15</v>
       </c>
       <c r="J8" s="17" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="K8" s="17" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6040,10 +6049,10 @@
         <v>68</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C9" s="52" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D9" s="13">
         <v>0.8</v>
@@ -6066,10 +6075,10 @@
         <v>0.15</v>
       </c>
       <c r="J9" s="17" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K9" s="17" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6077,10 +6086,10 @@
         <v>69</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C10" s="52" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D10" s="17">
         <v>0.8</v>
@@ -6103,10 +6112,10 @@
         <v>0.15</v>
       </c>
       <c r="J10" s="17" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="K10" s="17" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6114,10 +6123,10 @@
         <v>70</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C11" s="52" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D11" s="13">
         <v>0.8</v>
@@ -6140,10 +6149,10 @@
         <v>0.15</v>
       </c>
       <c r="J11" s="17" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="K11" s="17" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6151,10 +6160,10 @@
         <v>72</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C12" s="52" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D12" s="17">
         <v>0.8</v>
@@ -6177,10 +6186,10 @@
         <v>0.2</v>
       </c>
       <c r="J12" s="17" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="K12" s="17" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6188,10 +6197,10 @@
         <v>73</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C13" s="52" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D13" s="13">
         <v>0.8</v>
@@ -6212,10 +6221,10 @@
         <v>0.2</v>
       </c>
       <c r="J13" s="17" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="K13" s="17" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6223,10 +6232,10 @@
         <v>74</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C14" s="52" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D14" s="17">
         <v>0.8</v>
@@ -6249,10 +6258,10 @@
         <v>0.2</v>
       </c>
       <c r="J14" s="17" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K14" s="17" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6260,10 +6269,10 @@
         <v>75</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C15" s="52" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D15" s="13">
         <v>0.8</v>
@@ -6286,10 +6295,10 @@
         <v>0.2</v>
       </c>
       <c r="J15" s="17" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="K15" s="17" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6297,10 +6306,10 @@
         <v>76</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C16" s="53" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D16" s="17">
         <v>0.8</v>
@@ -6323,15 +6332,15 @@
         <v>0.2</v>
       </c>
       <c r="J16" s="17" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="K16" s="17" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="18" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G18" t="s">
         <v>79</v>
@@ -6351,14 +6360,14 @@
   <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="P15" sqref="P15"/>
+      <pane xSplit="1" topLeftCell="J1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.7109375" customWidth="1"/>
-    <col min="2" max="2" width="12" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" customWidth="1"/>
     <col min="3" max="3" width="17.28515625" customWidth="1"/>
     <col min="4" max="4" width="21.28515625" customWidth="1"/>
     <col min="5" max="5" width="24.42578125" customWidth="1"/>
@@ -6377,16 +6386,16 @@
         <v>41</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>151</v>
+        <v>263</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D1" s="10" t="s">
+        <v>259</v>
+      </c>
+      <c r="E1" s="10" t="s">
         <v>260</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>261</v>
       </c>
       <c r="F1" s="14" t="s">
         <v>40</v>
@@ -6418,10 +6427,10 @@
         <v>20</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C2" s="51" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D2" s="17">
         <v>0.8</v>
@@ -6449,10 +6458,10 @@
         <v>1</v>
       </c>
       <c r="L2" s="17" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="M2" s="17" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -6460,10 +6469,10 @@
         <v>21</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C3" s="52" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D3" s="13">
         <v>0.8</v>
@@ -6491,10 +6500,10 @@
         <v>5</v>
       </c>
       <c r="L3" s="17" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="M3" s="17" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -6502,10 +6511,10 @@
         <v>22</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C4" s="52" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D4" s="17">
         <v>0.8</v>
@@ -6532,10 +6541,10 @@
         <v>1</v>
       </c>
       <c r="L4" s="17" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="M4" s="17" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -6543,10 +6552,10 @@
         <v>23</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C5" s="52" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D5" s="13">
         <v>0.8</v>
@@ -6573,10 +6582,10 @@
         <v>5</v>
       </c>
       <c r="L5" s="17" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="M5" s="17" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -6584,10 +6593,10 @@
         <v>24</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C6" s="52" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D6" s="17">
         <v>0.8</v>
@@ -6614,10 +6623,10 @@
         <v>5</v>
       </c>
       <c r="L6" s="17" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="M6" s="17" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -6625,10 +6634,10 @@
         <v>25</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C7" s="52" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D7" s="13">
         <v>0.8</v>
@@ -6655,10 +6664,10 @@
         <v>5</v>
       </c>
       <c r="L7" s="17" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="M7" s="17" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -6666,10 +6675,10 @@
         <v>26</v>
       </c>
       <c r="B8" s="24" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C8" s="54" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D8" s="17">
         <v>0.8</v>
@@ -6696,10 +6705,10 @@
         <v>5</v>
       </c>
       <c r="L8" s="17" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="M8" s="17" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -6707,10 +6716,10 @@
         <v>29</v>
       </c>
       <c r="B9" s="24" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C9" s="54" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D9" s="13">
         <v>0.8</v>
@@ -6737,10 +6746,10 @@
         <v>5</v>
       </c>
       <c r="L9" s="17" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="M9" s="17" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -6748,10 +6757,10 @@
         <v>28</v>
       </c>
       <c r="B10" s="24" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C10" s="54" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D10" s="17">
         <v>0.8</v>
@@ -6779,10 +6788,10 @@
         <v>5</v>
       </c>
       <c r="L10" s="17" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="M10" s="17" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
@@ -6790,10 +6799,10 @@
         <v>27</v>
       </c>
       <c r="B11" s="25" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C11" s="55" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D11" s="13">
         <v>0.8</v>
@@ -6820,15 +6829,15 @@
         <v>5</v>
       </c>
       <c r="L11" s="17" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="M11" s="17" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
   </sheetData>
@@ -6844,13 +6853,14 @@
   <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E22" sqref="E22"/>
+      <pane xSplit="1" topLeftCell="M1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="11.85546875" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" customWidth="1"/>
     <col min="3" max="5" width="23.140625" customWidth="1"/>
     <col min="6" max="6" width="7.7109375" customWidth="1"/>
     <col min="7" max="7" width="7.85546875" customWidth="1"/>
@@ -6868,16 +6878,16 @@
         <v>41</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>151</v>
+        <v>263</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D1" s="58" t="s">
+        <v>259</v>
+      </c>
+      <c r="E1" s="58" t="s">
         <v>260</v>
-      </c>
-      <c r="E1" s="58" t="s">
-        <v>261</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>51</v>
@@ -6915,7 +6925,7 @@
         <v>7</v>
       </c>
       <c r="C2" s="51" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D2" s="17">
         <v>0.8</v>
@@ -6946,10 +6956,10 @@
         <v>56</v>
       </c>
       <c r="M2" s="17" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="N2" s="17" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -6957,10 +6967,10 @@
         <v>45</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C3" s="52" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D3" s="17">
         <v>0.8</v>
@@ -6991,10 +7001,10 @@
         <v>56</v>
       </c>
       <c r="M3" s="17" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="N3" s="17" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -7002,10 +7012,10 @@
         <v>0</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C4" s="52" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D4" s="17">
         <v>0.8</v>
@@ -7036,10 +7046,10 @@
         <v>56</v>
       </c>
       <c r="M4" s="17" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="N4" s="17" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -7047,10 +7057,10 @@
         <v>46</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C5" s="52" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D5" s="17">
         <v>0.8</v>
@@ -7081,10 +7091,10 @@
         <v>56</v>
       </c>
       <c r="M5" s="17" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N5" s="17" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -7092,10 +7102,10 @@
         <v>47</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C6" s="52" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D6" s="17">
         <v>0.8</v>
@@ -7128,10 +7138,10 @@
         <v>58</v>
       </c>
       <c r="M6" s="17" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N6" s="17" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
@@ -7139,10 +7149,10 @@
         <v>48</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C7" s="52" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D7" s="17">
         <v>0.8</v>
@@ -7173,10 +7183,10 @@
         <v>56</v>
       </c>
       <c r="M7" s="17" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="N7" s="17" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -7184,10 +7194,10 @@
         <v>49</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C8" s="52" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D8" s="17">
         <v>0.8</v>
@@ -7218,10 +7228,10 @@
         <v>57</v>
       </c>
       <c r="M8" s="17" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="N8" s="17" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -7229,10 +7239,10 @@
         <v>50</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C9" s="53" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D9" s="17">
         <v>0.8</v>
@@ -7263,15 +7273,15 @@
         <v>57</v>
       </c>
       <c r="M9" s="17" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="N9" s="17" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- finished Configloader - added Configprinter for testing - added Enums.java - finished parsed xml value validation - finished error handling in configloaders -> 	errors are passed to main function and program exited since errors in 	config will lead to severe problems later on
</commit_message>
<xml_diff>
--- a/RDG/config/RDG.xlsx
+++ b/RDG/config/RDG.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="8565" windowHeight="9420" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="8565" windowHeight="9420" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="6" r:id="rId1"/>
@@ -202,7 +202,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="261">
   <si>
     <t>Axt</t>
   </si>
@@ -373,9 +373,6 @@
   </si>
   <si>
     <t>two-hand</t>
-  </si>
-  <si>
-    <t>single-hand, max. 1</t>
   </si>
   <si>
     <t>leather</t>
@@ -1460,17 +1457,17 @@
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="1" fontId="2" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="2" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -4495,7 +4492,7 @@
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
   </sheetData>
@@ -4536,21 +4533,21 @@
     <row r="1" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="22"/>
       <c r="B1" s="22"/>
-      <c r="C1" s="78" t="s">
-        <v>126</v>
-      </c>
-      <c r="D1" s="79"/>
-      <c r="E1" s="79"/>
-      <c r="F1" s="80"/>
-      <c r="G1" s="78" t="s">
-        <v>121</v>
-      </c>
-      <c r="H1" s="79"/>
-      <c r="I1" s="79"/>
-      <c r="J1" s="80"/>
+      <c r="C1" s="77" t="s">
+        <v>125</v>
+      </c>
+      <c r="D1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="79"/>
+      <c r="G1" s="77" t="s">
+        <v>120</v>
+      </c>
+      <c r="H1" s="78"/>
+      <c r="I1" s="78"/>
+      <c r="J1" s="79"/>
       <c r="K1" s="29"/>
       <c r="L1" s="81" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="M1" s="82"/>
       <c r="N1" s="82"/>
@@ -4566,57 +4563,57 @@
         <v>39</v>
       </c>
       <c r="C2" s="25" t="s">
+        <v>127</v>
+      </c>
+      <c r="D2" s="25" t="s">
+        <v>126</v>
+      </c>
+      <c r="E2" s="25" t="s">
         <v>128</v>
       </c>
-      <c r="D2" s="25" t="s">
-        <v>127</v>
-      </c>
-      <c r="E2" s="25" t="s">
+      <c r="F2" s="25" t="s">
         <v>129</v>
       </c>
-      <c r="F2" s="25" t="s">
-        <v>130</v>
-      </c>
       <c r="G2" s="25" t="s">
+        <v>121</v>
+      </c>
+      <c r="H2" s="35" t="s">
+        <v>79</v>
+      </c>
+      <c r="I2" s="35" t="s">
+        <v>80</v>
+      </c>
+      <c r="J2" s="35" t="s">
+        <v>81</v>
+      </c>
+      <c r="K2" s="30" t="s">
+        <v>158</v>
+      </c>
+      <c r="L2" s="32" t="s">
+        <v>259</v>
+      </c>
+      <c r="M2" s="32" t="s">
+        <v>149</v>
+      </c>
+      <c r="N2" s="32" t="s">
+        <v>150</v>
+      </c>
+      <c r="O2" s="32" t="s">
+        <v>151</v>
+      </c>
+      <c r="P2" s="37" t="s">
+        <v>159</v>
+      </c>
+      <c r="Q2" s="39" t="s">
         <v>122</v>
-      </c>
-      <c r="H2" s="35" t="s">
-        <v>80</v>
-      </c>
-      <c r="I2" s="35" t="s">
-        <v>81</v>
-      </c>
-      <c r="J2" s="35" t="s">
-        <v>82</v>
-      </c>
-      <c r="K2" s="30" t="s">
-        <v>159</v>
-      </c>
-      <c r="L2" s="32" t="s">
-        <v>260</v>
-      </c>
-      <c r="M2" s="32" t="s">
-        <v>150</v>
-      </c>
-      <c r="N2" s="32" t="s">
-        <v>151</v>
-      </c>
-      <c r="O2" s="32" t="s">
-        <v>152</v>
-      </c>
-      <c r="P2" s="37" t="s">
-        <v>160</v>
-      </c>
-      <c r="Q2" s="39" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C3" s="26">
         <v>1</v>
@@ -4661,15 +4658,15 @@
         <v>3</v>
       </c>
       <c r="Q3" s="21" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C4" s="26">
         <v>1</v>
@@ -4714,15 +4711,15 @@
         <v>2</v>
       </c>
       <c r="Q4" s="21" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C5" s="26">
         <v>1</v>
@@ -4767,15 +4764,15 @@
         <v>2</v>
       </c>
       <c r="Q5" s="21" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="21" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C6" s="26">
         <v>1</v>
@@ -4820,15 +4817,15 @@
         <v>1</v>
       </c>
       <c r="Q6" s="21" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="21" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C7" s="26">
         <v>1</v>
@@ -4873,15 +4870,15 @@
         <v>1</v>
       </c>
       <c r="Q7" s="21" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="21" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B8" s="21" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C8" s="26">
         <v>1</v>
@@ -4926,37 +4923,37 @@
         <v>5</v>
       </c>
       <c r="Q8" s="21" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="21" t="s">
-        <v>147</v>
-      </c>
-      <c r="C10" s="77" t="s">
-        <v>132</v>
-      </c>
-      <c r="D10" s="77"/>
-      <c r="E10" s="77"/>
-      <c r="F10" s="77"/>
-      <c r="G10" s="77" t="s">
+        <v>146</v>
+      </c>
+      <c r="C10" s="80" t="s">
         <v>131</v>
       </c>
-      <c r="H10" s="77"/>
-      <c r="I10" s="77"/>
-      <c r="J10" s="77"/>
+      <c r="D10" s="80"/>
+      <c r="E10" s="80"/>
+      <c r="F10" s="80"/>
+      <c r="G10" s="80" t="s">
+        <v>130</v>
+      </c>
+      <c r="H10" s="80"/>
+      <c r="I10" s="80"/>
+      <c r="J10" s="80"/>
       <c r="K10" s="31"/>
       <c r="L10" s="33"/>
-      <c r="M10" s="77" t="s">
-        <v>156</v>
-      </c>
-      <c r="N10" s="77"/>
-      <c r="O10" s="77"/>
+      <c r="M10" s="80" t="s">
+        <v>155</v>
+      </c>
+      <c r="N10" s="80"/>
+      <c r="O10" s="80"/>
       <c r="P10" s="33"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="21" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G11" s="34"/>
       <c r="H11" s="34"/>
@@ -4971,10 +4968,10 @@
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="21" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G12" s="34" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H12" s="34"/>
       <c r="I12" s="34"/>
@@ -4982,7 +4979,7 @@
       <c r="K12" s="28"/>
       <c r="L12" s="34"/>
       <c r="M12" s="34" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="N12" s="34"/>
       <c r="O12" s="34"/>
@@ -4990,7 +4987,7 @@
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G13" s="34"/>
       <c r="H13" s="34"/>
@@ -4999,19 +4996,19 @@
       <c r="K13" s="28"/>
       <c r="L13" s="34"/>
       <c r="M13" s="34" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="N13" s="34"/>
       <c r="O13" s="34"/>
       <c r="P13" s="34"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="G14" s="77" t="s">
-        <v>133</v>
-      </c>
-      <c r="H14" s="77"/>
-      <c r="I14" s="77"/>
-      <c r="J14" s="77"/>
+      <c r="G14" s="80" t="s">
+        <v>132</v>
+      </c>
+      <c r="H14" s="80"/>
+      <c r="I14" s="80"/>
+      <c r="J14" s="80"/>
       <c r="K14" s="31"/>
       <c r="L14" s="33"/>
       <c r="M14" s="33"/>
@@ -5021,14 +5018,14 @@
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="21" t="s">
-        <v>146</v>
-      </c>
-      <c r="G15" s="77" t="s">
-        <v>134</v>
-      </c>
-      <c r="H15" s="77"/>
-      <c r="I15" s="77"/>
-      <c r="J15" s="77"/>
+        <v>145</v>
+      </c>
+      <c r="G15" s="80" t="s">
+        <v>133</v>
+      </c>
+      <c r="H15" s="80"/>
+      <c r="I15" s="80"/>
+      <c r="J15" s="80"/>
       <c r="K15" s="31"/>
       <c r="L15" s="33"/>
       <c r="M15" s="33"/>
@@ -5037,12 +5034,12 @@
       <c r="P15" s="33"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="G16" s="77" t="s">
-        <v>135</v>
-      </c>
-      <c r="H16" s="77"/>
-      <c r="I16" s="77"/>
-      <c r="J16" s="77"/>
+      <c r="G16" s="80" t="s">
+        <v>134</v>
+      </c>
+      <c r="H16" s="80"/>
+      <c r="I16" s="80"/>
+      <c r="J16" s="80"/>
       <c r="K16" s="31"/>
       <c r="L16" s="33"/>
       <c r="M16" s="33"/>
@@ -5051,12 +5048,12 @@
       <c r="P16" s="33"/>
     </row>
     <row r="17" spans="7:16" x14ac:dyDescent="0.25">
-      <c r="G17" s="77" t="s">
-        <v>136</v>
-      </c>
-      <c r="H17" s="77"/>
-      <c r="I17" s="77"/>
-      <c r="J17" s="77"/>
+      <c r="G17" s="80" t="s">
+        <v>135</v>
+      </c>
+      <c r="H17" s="80"/>
+      <c r="I17" s="80"/>
+      <c r="J17" s="80"/>
       <c r="K17" s="31"/>
       <c r="L17" s="33"/>
       <c r="M17" s="33"/>
@@ -5065,12 +5062,12 @@
       <c r="P17" s="33"/>
     </row>
     <row r="18" spans="7:16" x14ac:dyDescent="0.25">
-      <c r="G18" s="77" t="s">
-        <v>137</v>
-      </c>
-      <c r="H18" s="77"/>
-      <c r="I18" s="77"/>
-      <c r="J18" s="77"/>
+      <c r="G18" s="80" t="s">
+        <v>136</v>
+      </c>
+      <c r="H18" s="80"/>
+      <c r="I18" s="80"/>
+      <c r="J18" s="80"/>
       <c r="K18" s="31"/>
       <c r="L18" s="33"/>
       <c r="M18" s="33"/>
@@ -5079,12 +5076,12 @@
       <c r="P18" s="33"/>
     </row>
     <row r="20" spans="7:16" x14ac:dyDescent="0.25">
-      <c r="G20" s="77" t="s">
-        <v>138</v>
-      </c>
-      <c r="H20" s="77"/>
-      <c r="I20" s="77"/>
-      <c r="J20" s="77"/>
+      <c r="G20" s="80" t="s">
+        <v>137</v>
+      </c>
+      <c r="H20" s="80"/>
+      <c r="I20" s="80"/>
+      <c r="J20" s="80"/>
       <c r="K20" s="31"/>
       <c r="L20" s="33"/>
       <c r="M20" s="33"/>
@@ -5093,12 +5090,12 @@
       <c r="P20" s="33"/>
     </row>
     <row r="21" spans="7:16" x14ac:dyDescent="0.25">
-      <c r="G21" s="77" t="s">
-        <v>139</v>
-      </c>
-      <c r="H21" s="77"/>
-      <c r="I21" s="77"/>
-      <c r="J21" s="77"/>
+      <c r="G21" s="80" t="s">
+        <v>138</v>
+      </c>
+      <c r="H21" s="80"/>
+      <c r="I21" s="80"/>
+      <c r="J21" s="80"/>
       <c r="K21" s="31"/>
       <c r="L21" s="33"/>
       <c r="M21" s="33"/>
@@ -5108,16 +5105,16 @@
     </row>
     <row r="23" spans="7:16" x14ac:dyDescent="0.25">
       <c r="G23" s="26" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="24" spans="7:16" x14ac:dyDescent="0.25">
-      <c r="G24" s="77" t="s">
-        <v>140</v>
-      </c>
-      <c r="H24" s="77"/>
-      <c r="I24" s="77"/>
-      <c r="J24" s="77"/>
+      <c r="G24" s="80" t="s">
+        <v>139</v>
+      </c>
+      <c r="H24" s="80"/>
+      <c r="I24" s="80"/>
+      <c r="J24" s="80"/>
       <c r="K24" s="31"/>
       <c r="L24" s="33"/>
       <c r="M24" s="33"/>
@@ -5126,12 +5123,12 @@
       <c r="P24" s="33"/>
     </row>
     <row r="25" spans="7:16" x14ac:dyDescent="0.25">
-      <c r="G25" s="77" t="s">
-        <v>141</v>
-      </c>
-      <c r="H25" s="77"/>
-      <c r="I25" s="77"/>
-      <c r="J25" s="77"/>
+      <c r="G25" s="80" t="s">
+        <v>140</v>
+      </c>
+      <c r="H25" s="80"/>
+      <c r="I25" s="80"/>
+      <c r="J25" s="80"/>
       <c r="K25" s="31"/>
       <c r="L25" s="33"/>
       <c r="M25" s="33"/>
@@ -5140,12 +5137,12 @@
       <c r="P25" s="33"/>
     </row>
     <row r="26" spans="7:16" x14ac:dyDescent="0.25">
-      <c r="G26" s="77" t="s">
-        <v>143</v>
-      </c>
-      <c r="H26" s="77"/>
-      <c r="I26" s="77"/>
-      <c r="J26" s="77"/>
+      <c r="G26" s="80" t="s">
+        <v>142</v>
+      </c>
+      <c r="H26" s="80"/>
+      <c r="I26" s="80"/>
+      <c r="J26" s="80"/>
       <c r="K26" s="31"/>
       <c r="L26" s="33"/>
       <c r="M26" s="33"/>
@@ -5155,11 +5152,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="C1:F1"/>
-    <mergeCell ref="G1:J1"/>
-    <mergeCell ref="M10:O10"/>
-    <mergeCell ref="G25:J25"/>
-    <mergeCell ref="L1:O1"/>
     <mergeCell ref="G26:J26"/>
     <mergeCell ref="C10:F10"/>
     <mergeCell ref="G10:J10"/>
@@ -5171,6 +5163,11 @@
     <mergeCell ref="G17:J17"/>
     <mergeCell ref="G18:J18"/>
     <mergeCell ref="G21:J21"/>
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="G1:J1"/>
+    <mergeCell ref="M10:O10"/>
+    <mergeCell ref="G25:J25"/>
+    <mergeCell ref="L1:O1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5205,16 +5202,16 @@
         <v>40</v>
       </c>
       <c r="B1" s="42" t="s">
+        <v>256</v>
+      </c>
+      <c r="C1" s="42" t="s">
         <v>257</v>
       </c>
-      <c r="C1" s="42" t="s">
-        <v>258</v>
-      </c>
       <c r="D1" s="43" t="s">
+        <v>104</v>
+      </c>
+      <c r="E1" s="43" t="s">
         <v>105</v>
-      </c>
-      <c r="E1" s="43" t="s">
-        <v>106</v>
       </c>
       <c r="F1" s="48" t="s">
         <v>16</v>
@@ -5225,7 +5222,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B2" s="44">
         <v>0.8</v>
@@ -5248,7 +5245,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B3" s="44">
         <v>0.8</v>
@@ -5271,7 +5268,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B4" s="44">
         <v>0.8</v>
@@ -5294,7 +5291,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B5" s="44">
         <v>0.8</v>
@@ -5317,7 +5314,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="41" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B7" s="28"/>
       <c r="C7" s="28"/>
@@ -5327,7 +5324,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="41" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B8" s="28"/>
       <c r="C8" s="28"/>
@@ -5373,16 +5370,16 @@
         <v>40</v>
       </c>
       <c r="B1" s="51" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C1" s="54" t="s">
+        <v>256</v>
+      </c>
+      <c r="D1" s="54" t="s">
         <v>257</v>
       </c>
-      <c r="D1" s="54" t="s">
-        <v>258</v>
-      </c>
       <c r="E1" s="57" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F1" s="57" t="s">
         <v>22</v>
@@ -5394,27 +5391,27 @@
         <v>24</v>
       </c>
       <c r="I1" s="53" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J1" s="61" t="s">
+        <v>97</v>
+      </c>
+      <c r="K1" s="61" t="s">
         <v>98</v>
       </c>
-      <c r="K1" s="61" t="s">
-        <v>99</v>
-      </c>
       <c r="L1" s="50" t="s">
+        <v>123</v>
+      </c>
+      <c r="M1" s="50" t="s">
         <v>124</v>
-      </c>
-      <c r="M1" s="50" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C2" s="55">
         <v>0.8</v>
@@ -5444,18 +5441,18 @@
         <v>4</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C3" s="55">
         <v>0.8</v>
@@ -5485,18 +5482,18 @@
         <v>2</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C4" s="55">
         <v>0.8</v>
@@ -5526,18 +5523,18 @@
         <v>2</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C5" s="55">
         <v>0.8</v>
@@ -5567,10 +5564,10 @@
         <v>2</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5578,7 +5575,7 @@
         <v>1</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C6" s="55">
         <v>0.8</v>
@@ -5608,10 +5605,10 @@
         <v>2</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5619,7 +5616,7 @@
         <v>2</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C7" s="55">
         <v>0.8</v>
@@ -5649,10 +5646,10 @@
         <v>5</v>
       </c>
       <c r="L7" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5660,7 +5657,7 @@
         <v>3</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C8" s="55">
         <v>0.8</v>
@@ -5690,18 +5687,18 @@
         <v>7</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="M8" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C9" s="55">
         <v>0.8</v>
@@ -5731,10 +5728,10 @@
         <v>5</v>
       </c>
       <c r="L9" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="M9" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5742,7 +5739,7 @@
         <v>4</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C10" s="55">
         <v>0.8</v>
@@ -5772,18 +5769,18 @@
         <v>10</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="M10" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C11" s="55">
         <v>0.8</v>
@@ -5813,18 +5810,18 @@
         <v>30</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="M11" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="19" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C12" s="55">
         <v>0.8</v>
@@ -5854,18 +5851,18 @@
         <v>30</v>
       </c>
       <c r="L12" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="M12" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C13" s="55">
         <v>0.8</v>
@@ -5895,38 +5892,38 @@
         <v>30</v>
       </c>
       <c r="L13" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M13" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="52" t="s">
+        <v>82</v>
+      </c>
+      <c r="B15" s="52" t="s">
         <v>83</v>
-      </c>
-      <c r="B15" s="52" t="s">
-        <v>84</v>
       </c>
       <c r="C15" s="56"/>
       <c r="D15" s="56"/>
     </row>
     <row r="16" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="52" t="s">
+        <v>84</v>
+      </c>
+      <c r="B16" s="52" t="s">
         <v>85</v>
-      </c>
-      <c r="B16" s="52" t="s">
-        <v>86</v>
       </c>
       <c r="C16" s="56"/>
       <c r="D16" s="56"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="52" t="s">
+        <v>86</v>
+      </c>
+      <c r="B17" s="52" t="s">
         <v>87</v>
-      </c>
-      <c r="B17" s="52" t="s">
-        <v>88</v>
       </c>
       <c r="C17" s="56"/>
       <c r="D17" s="56"/>
@@ -5968,19 +5965,19 @@
         <v>40</v>
       </c>
       <c r="B1" s="50" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C1" s="63" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D1" s="63" t="s">
+        <v>256</v>
+      </c>
+      <c r="E1" s="63" t="s">
         <v>257</v>
       </c>
-      <c r="E1" s="63" t="s">
-        <v>258</v>
-      </c>
       <c r="F1" s="57" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G1" s="57" t="s">
         <v>23</v>
@@ -5989,21 +5986,21 @@
         <v>52</v>
       </c>
       <c r="I1" s="54" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J1" s="50" t="s">
+        <v>123</v>
+      </c>
+      <c r="K1" s="50" t="s">
         <v>124</v>
-      </c>
-      <c r="K1" s="50" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C2" s="64">
         <v>1</v>
@@ -6023,24 +6020,24 @@
         <v>13.333333333333334</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I2" s="64">
         <v>0.1</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C3" s="65">
         <v>1</v>
@@ -6058,24 +6055,24 @@
         <v>20</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I3" s="65">
         <v>0.1</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C4" s="64">
         <v>1</v>
@@ -6095,24 +6092,24 @@
         <v>6.666666666666667</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I4" s="65">
         <v>0.1</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C5" s="65">
         <v>1</v>
@@ -6132,24 +6129,24 @@
         <v>10</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I5" s="65">
         <v>0.1</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C6" s="64">
         <v>1</v>
@@ -6169,24 +6166,24 @@
         <v>6.666666666666667</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I6" s="65">
         <v>0.1</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C7" s="65">
         <v>1</v>
@@ -6206,24 +6203,24 @@
         <v>16.666666666666668</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I7" s="65">
         <v>0.15</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C8" s="64">
         <v>1</v>
@@ -6241,24 +6238,24 @@
         <v>25</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I8" s="65">
         <v>0.15</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C9" s="65">
         <v>1</v>
@@ -6278,24 +6275,24 @@
         <v>8.3333333333333339</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I9" s="65">
         <v>0.15</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C10" s="64">
         <v>1</v>
@@ -6315,24 +6312,24 @@
         <v>12.5</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I10" s="65">
         <v>0.15</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C11" s="65">
         <v>1</v>
@@ -6352,24 +6349,24 @@
         <v>8.3333333333333339</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I11" s="65">
         <v>0.15</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C12" s="64">
         <v>1</v>
@@ -6389,24 +6386,24 @@
         <v>20</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I12" s="65">
         <v>0.2</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C13" s="65">
         <v>1</v>
@@ -6424,24 +6421,24 @@
         <v>30</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I13" s="65">
         <v>0.2</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C14" s="64">
         <v>1</v>
@@ -6461,24 +6458,24 @@
         <v>10</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I14" s="65">
         <v>0.2</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C15" s="65">
         <v>1</v>
@@ -6498,24 +6495,24 @@
         <v>15</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I15" s="65">
         <v>0.2</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C16" s="64">
         <v>1</v>
@@ -6535,24 +6532,24 @@
         <v>10</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I16" s="66">
         <v>0.2</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="18" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C18" s="27" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G18" s="26" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -6568,8 +6565,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
@@ -6595,16 +6592,16 @@
         <v>40</v>
       </c>
       <c r="B1" s="50" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C1" s="63" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D1" s="63" t="s">
+        <v>256</v>
+      </c>
+      <c r="E1" s="63" t="s">
         <v>257</v>
-      </c>
-      <c r="E1" s="63" t="s">
-        <v>258</v>
       </c>
       <c r="F1" s="70" t="s">
         <v>39</v>
@@ -6625,10 +6622,10 @@
         <v>6</v>
       </c>
       <c r="L1" s="50" t="s">
+        <v>123</v>
+      </c>
+      <c r="M1" s="50" t="s">
         <v>124</v>
-      </c>
-      <c r="M1" s="50" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -6636,7 +6633,7 @@
         <v>19</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C2" s="64">
         <v>1</v>
@@ -6667,10 +6664,10 @@
         <v>1</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -6678,7 +6675,7 @@
         <v>20</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C3" s="65">
         <v>1</v>
@@ -6709,10 +6706,10 @@
         <v>5</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -6720,7 +6717,7 @@
         <v>21</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C4" s="64">
         <v>1</v>
@@ -6750,10 +6747,10 @@
         <v>1</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -6761,7 +6758,7 @@
         <v>22</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C5" s="65">
         <v>1</v>
@@ -6791,10 +6788,10 @@
         <v>5</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -6802,7 +6799,7 @@
         <v>23</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C6" s="64">
         <v>1</v>
@@ -6832,10 +6829,10 @@
         <v>5</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -6843,7 +6840,7 @@
         <v>24</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C7" s="65">
         <v>1</v>
@@ -6873,10 +6870,10 @@
         <v>5</v>
       </c>
       <c r="L7" s="3" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -6884,7 +6881,7 @@
         <v>25</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C8" s="64">
         <v>1</v>
@@ -6914,10 +6911,10 @@
         <v>5</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="M8" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -6925,7 +6922,7 @@
         <v>28</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C9" s="65">
         <v>1</v>
@@ -6955,10 +6952,10 @@
         <v>5</v>
       </c>
       <c r="L9" s="3" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="M9" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -6966,7 +6963,7 @@
         <v>27</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C10" s="64">
         <v>1</v>
@@ -6997,10 +6994,10 @@
         <v>5</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="M10" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
@@ -7008,7 +7005,7 @@
         <v>26</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C11" s="65">
         <v>1</v>
@@ -7038,15 +7035,15 @@
         <v>5</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="M11" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C13" s="27" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
   </sheetData>
@@ -7061,9 +7058,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="P9" sqref="P9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7087,16 +7084,16 @@
         <v>40</v>
       </c>
       <c r="B1" s="23" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C1" s="30" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D1" s="30" t="s">
+        <v>256</v>
+      </c>
+      <c r="E1" s="30" t="s">
         <v>257</v>
-      </c>
-      <c r="E1" s="30" t="s">
-        <v>258</v>
       </c>
       <c r="F1" s="35" t="s">
         <v>50</v>
@@ -7120,10 +7117,10 @@
         <v>52</v>
       </c>
       <c r="M1" s="23" t="s">
+        <v>123</v>
+      </c>
+      <c r="N1" s="23" t="s">
         <v>124</v>
-      </c>
-      <c r="N1" s="23" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -7164,10 +7161,10 @@
         <v>55</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -7175,7 +7172,7 @@
         <v>44</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C3" s="64">
         <v>1</v>
@@ -7208,10 +7205,10 @@
         <v>55</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -7219,7 +7216,7 @@
         <v>0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C4" s="64">
         <v>1</v>
@@ -7252,10 +7249,10 @@
         <v>55</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -7263,7 +7260,7 @@
         <v>45</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C5" s="64">
         <v>1</v>
@@ -7296,10 +7293,10 @@
         <v>55</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="N5" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -7307,7 +7304,7 @@
         <v>46</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C6" s="64">
         <v>1</v>
@@ -7337,13 +7334,13 @@
         <v>1</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="N6" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
@@ -7351,7 +7348,7 @@
         <v>47</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C7" s="64">
         <v>1</v>
@@ -7384,10 +7381,10 @@
         <v>55</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="N7" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -7395,7 +7392,7 @@
         <v>48</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C8" s="64">
         <v>1</v>
@@ -7428,10 +7425,10 @@
         <v>56</v>
       </c>
       <c r="M8" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N8" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -7439,7 +7436,7 @@
         <v>49</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C9" s="64">
         <v>1</v>
@@ -7472,15 +7469,15 @@
         <v>56</v>
       </c>
       <c r="M9" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N9" s="3" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C11" s="27" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added javadocs to all config loaders and templates, view and game from worthy
</commit_message>
<xml_diff>
--- a/RDG/config/RDG.xlsx
+++ b/RDG/config/RDG.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="8565" windowHeight="9420" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="9975" windowHeight="7335" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="6" r:id="rId1"/>
@@ -16,6 +16,7 @@
     <sheet name="Weapons" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="145621"/>
+  <oleSize ref="A1:F22"/>
 </workbook>
 </file>
 
@@ -1457,6 +1458,9 @@
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="1" fontId="2" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1465,9 +1469,6 @@
     </xf>
     <xf numFmtId="1" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="2" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -4504,8 +4505,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="O1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="L1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="Q17" sqref="Q17"/>
     </sheetView>
   </sheetViews>
@@ -4533,18 +4534,18 @@
     <row r="1" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="22"/>
       <c r="B1" s="22"/>
-      <c r="C1" s="77" t="s">
+      <c r="C1" s="78" t="s">
         <v>125</v>
       </c>
-      <c r="D1" s="78"/>
-      <c r="E1" s="78"/>
-      <c r="F1" s="79"/>
-      <c r="G1" s="77" t="s">
+      <c r="D1" s="79"/>
+      <c r="E1" s="79"/>
+      <c r="F1" s="80"/>
+      <c r="G1" s="78" t="s">
         <v>120</v>
       </c>
-      <c r="H1" s="78"/>
-      <c r="I1" s="78"/>
-      <c r="J1" s="79"/>
+      <c r="H1" s="79"/>
+      <c r="I1" s="79"/>
+      <c r="J1" s="80"/>
       <c r="K1" s="29"/>
       <c r="L1" s="81" t="s">
         <v>154</v>
@@ -4930,25 +4931,25 @@
       <c r="A10" s="21" t="s">
         <v>146</v>
       </c>
-      <c r="C10" s="80" t="s">
+      <c r="C10" s="77" t="s">
         <v>131</v>
       </c>
-      <c r="D10" s="80"/>
-      <c r="E10" s="80"/>
-      <c r="F10" s="80"/>
-      <c r="G10" s="80" t="s">
+      <c r="D10" s="77"/>
+      <c r="E10" s="77"/>
+      <c r="F10" s="77"/>
+      <c r="G10" s="77" t="s">
         <v>130</v>
       </c>
-      <c r="H10" s="80"/>
-      <c r="I10" s="80"/>
-      <c r="J10" s="80"/>
+      <c r="H10" s="77"/>
+      <c r="I10" s="77"/>
+      <c r="J10" s="77"/>
       <c r="K10" s="31"/>
       <c r="L10" s="33"/>
-      <c r="M10" s="80" t="s">
+      <c r="M10" s="77" t="s">
         <v>155</v>
       </c>
-      <c r="N10" s="80"/>
-      <c r="O10" s="80"/>
+      <c r="N10" s="77"/>
+      <c r="O10" s="77"/>
       <c r="P10" s="33"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
@@ -5003,12 +5004,12 @@
       <c r="P13" s="34"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="G14" s="80" t="s">
+      <c r="G14" s="77" t="s">
         <v>132</v>
       </c>
-      <c r="H14" s="80"/>
-      <c r="I14" s="80"/>
-      <c r="J14" s="80"/>
+      <c r="H14" s="77"/>
+      <c r="I14" s="77"/>
+      <c r="J14" s="77"/>
       <c r="K14" s="31"/>
       <c r="L14" s="33"/>
       <c r="M14" s="33"/>
@@ -5020,12 +5021,12 @@
       <c r="A15" s="21" t="s">
         <v>145</v>
       </c>
-      <c r="G15" s="80" t="s">
+      <c r="G15" s="77" t="s">
         <v>133</v>
       </c>
-      <c r="H15" s="80"/>
-      <c r="I15" s="80"/>
-      <c r="J15" s="80"/>
+      <c r="H15" s="77"/>
+      <c r="I15" s="77"/>
+      <c r="J15" s="77"/>
       <c r="K15" s="31"/>
       <c r="L15" s="33"/>
       <c r="M15" s="33"/>
@@ -5034,12 +5035,12 @@
       <c r="P15" s="33"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="G16" s="80" t="s">
+      <c r="G16" s="77" t="s">
         <v>134</v>
       </c>
-      <c r="H16" s="80"/>
-      <c r="I16" s="80"/>
-      <c r="J16" s="80"/>
+      <c r="H16" s="77"/>
+      <c r="I16" s="77"/>
+      <c r="J16" s="77"/>
       <c r="K16" s="31"/>
       <c r="L16" s="33"/>
       <c r="M16" s="33"/>
@@ -5048,12 +5049,12 @@
       <c r="P16" s="33"/>
     </row>
     <row r="17" spans="7:16" x14ac:dyDescent="0.25">
-      <c r="G17" s="80" t="s">
+      <c r="G17" s="77" t="s">
         <v>135</v>
       </c>
-      <c r="H17" s="80"/>
-      <c r="I17" s="80"/>
-      <c r="J17" s="80"/>
+      <c r="H17" s="77"/>
+      <c r="I17" s="77"/>
+      <c r="J17" s="77"/>
       <c r="K17" s="31"/>
       <c r="L17" s="33"/>
       <c r="M17" s="33"/>
@@ -5062,12 +5063,12 @@
       <c r="P17" s="33"/>
     </row>
     <row r="18" spans="7:16" x14ac:dyDescent="0.25">
-      <c r="G18" s="80" t="s">
+      <c r="G18" s="77" t="s">
         <v>136</v>
       </c>
-      <c r="H18" s="80"/>
-      <c r="I18" s="80"/>
-      <c r="J18" s="80"/>
+      <c r="H18" s="77"/>
+      <c r="I18" s="77"/>
+      <c r="J18" s="77"/>
       <c r="K18" s="31"/>
       <c r="L18" s="33"/>
       <c r="M18" s="33"/>
@@ -5076,12 +5077,12 @@
       <c r="P18" s="33"/>
     </row>
     <row r="20" spans="7:16" x14ac:dyDescent="0.25">
-      <c r="G20" s="80" t="s">
+      <c r="G20" s="77" t="s">
         <v>137</v>
       </c>
-      <c r="H20" s="80"/>
-      <c r="I20" s="80"/>
-      <c r="J20" s="80"/>
+      <c r="H20" s="77"/>
+      <c r="I20" s="77"/>
+      <c r="J20" s="77"/>
       <c r="K20" s="31"/>
       <c r="L20" s="33"/>
       <c r="M20" s="33"/>
@@ -5090,12 +5091,12 @@
       <c r="P20" s="33"/>
     </row>
     <row r="21" spans="7:16" x14ac:dyDescent="0.25">
-      <c r="G21" s="80" t="s">
+      <c r="G21" s="77" t="s">
         <v>138</v>
       </c>
-      <c r="H21" s="80"/>
-      <c r="I21" s="80"/>
-      <c r="J21" s="80"/>
+      <c r="H21" s="77"/>
+      <c r="I21" s="77"/>
+      <c r="J21" s="77"/>
       <c r="K21" s="31"/>
       <c r="L21" s="33"/>
       <c r="M21" s="33"/>
@@ -5109,12 +5110,12 @@
       </c>
     </row>
     <row r="24" spans="7:16" x14ac:dyDescent="0.25">
-      <c r="G24" s="80" t="s">
+      <c r="G24" s="77" t="s">
         <v>139</v>
       </c>
-      <c r="H24" s="80"/>
-      <c r="I24" s="80"/>
-      <c r="J24" s="80"/>
+      <c r="H24" s="77"/>
+      <c r="I24" s="77"/>
+      <c r="J24" s="77"/>
       <c r="K24" s="31"/>
       <c r="L24" s="33"/>
       <c r="M24" s="33"/>
@@ -5123,12 +5124,12 @@
       <c r="P24" s="33"/>
     </row>
     <row r="25" spans="7:16" x14ac:dyDescent="0.25">
-      <c r="G25" s="80" t="s">
+      <c r="G25" s="77" t="s">
         <v>140</v>
       </c>
-      <c r="H25" s="80"/>
-      <c r="I25" s="80"/>
-      <c r="J25" s="80"/>
+      <c r="H25" s="77"/>
+      <c r="I25" s="77"/>
+      <c r="J25" s="77"/>
       <c r="K25" s="31"/>
       <c r="L25" s="33"/>
       <c r="M25" s="33"/>
@@ -5137,12 +5138,12 @@
       <c r="P25" s="33"/>
     </row>
     <row r="26" spans="7:16" x14ac:dyDescent="0.25">
-      <c r="G26" s="80" t="s">
+      <c r="G26" s="77" t="s">
         <v>142</v>
       </c>
-      <c r="H26" s="80"/>
-      <c r="I26" s="80"/>
-      <c r="J26" s="80"/>
+      <c r="H26" s="77"/>
+      <c r="I26" s="77"/>
+      <c r="J26" s="77"/>
       <c r="K26" s="31"/>
       <c r="L26" s="33"/>
       <c r="M26" s="33"/>
@@ -5152,6 +5153,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="G1:J1"/>
+    <mergeCell ref="M10:O10"/>
+    <mergeCell ref="G25:J25"/>
+    <mergeCell ref="L1:O1"/>
     <mergeCell ref="G26:J26"/>
     <mergeCell ref="C10:F10"/>
     <mergeCell ref="G10:J10"/>
@@ -5163,11 +5169,6 @@
     <mergeCell ref="G17:J17"/>
     <mergeCell ref="G18:J18"/>
     <mergeCell ref="G21:J21"/>
-    <mergeCell ref="C1:F1"/>
-    <mergeCell ref="G1:J1"/>
-    <mergeCell ref="M10:O10"/>
-    <mergeCell ref="G25:J25"/>
-    <mergeCell ref="L1:O1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5182,8 +5183,8 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F7" sqref="F7"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5240,7 +5241,7 @@
         <v>10</v>
       </c>
       <c r="G2" s="44">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -5263,7 +5264,7 @@
         <v>13</v>
       </c>
       <c r="G3" s="45">
-        <v>0.2</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -5286,7 +5287,7 @@
         <v>11</v>
       </c>
       <c r="G4" s="45">
-        <v>0.2</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -5309,7 +5310,7 @@
         <v>12</v>
       </c>
       <c r="G5" s="46">
-        <v>0.2</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -5345,7 +5346,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I15" sqref="I15"/>
+      <selection pane="topRight" activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7058,8 +7059,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
finished Armament.java, Potion.java, Weapon.java
</commit_message>
<xml_diff>
--- a/RDG/config/RDG.xlsx
+++ b/RDG/config/RDG.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="9975" windowHeight="7335" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="10725" windowHeight="8580" firstSheet="3" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="6" r:id="rId1"/>
@@ -16,7 +16,7 @@
     <sheet name="Weapons" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="145621"/>
-  <oleSize ref="A1:F22"/>
+  <oleSize ref="A1:E27"/>
 </workbook>
 </file>
 
@@ -1458,17 +1458,17 @@
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="1" fontId="2" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="2" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -4505,8 +4505,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="L1" activePane="topRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="Q17" sqref="Q17"/>
     </sheetView>
   </sheetViews>
@@ -4534,18 +4534,18 @@
     <row r="1" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="22"/>
       <c r="B1" s="22"/>
-      <c r="C1" s="78" t="s">
+      <c r="C1" s="77" t="s">
         <v>125</v>
       </c>
-      <c r="D1" s="79"/>
-      <c r="E1" s="79"/>
-      <c r="F1" s="80"/>
-      <c r="G1" s="78" t="s">
+      <c r="D1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="79"/>
+      <c r="G1" s="77" t="s">
         <v>120</v>
       </c>
-      <c r="H1" s="79"/>
-      <c r="I1" s="79"/>
-      <c r="J1" s="80"/>
+      <c r="H1" s="78"/>
+      <c r="I1" s="78"/>
+      <c r="J1" s="79"/>
       <c r="K1" s="29"/>
       <c r="L1" s="81" t="s">
         <v>154</v>
@@ -4931,25 +4931,25 @@
       <c r="A10" s="21" t="s">
         <v>146</v>
       </c>
-      <c r="C10" s="77" t="s">
+      <c r="C10" s="80" t="s">
         <v>131</v>
       </c>
-      <c r="D10" s="77"/>
-      <c r="E10" s="77"/>
-      <c r="F10" s="77"/>
-      <c r="G10" s="77" t="s">
+      <c r="D10" s="80"/>
+      <c r="E10" s="80"/>
+      <c r="F10" s="80"/>
+      <c r="G10" s="80" t="s">
         <v>130</v>
       </c>
-      <c r="H10" s="77"/>
-      <c r="I10" s="77"/>
-      <c r="J10" s="77"/>
+      <c r="H10" s="80"/>
+      <c r="I10" s="80"/>
+      <c r="J10" s="80"/>
       <c r="K10" s="31"/>
       <c r="L10" s="33"/>
-      <c r="M10" s="77" t="s">
+      <c r="M10" s="80" t="s">
         <v>155</v>
       </c>
-      <c r="N10" s="77"/>
-      <c r="O10" s="77"/>
+      <c r="N10" s="80"/>
+      <c r="O10" s="80"/>
       <c r="P10" s="33"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
@@ -5004,12 +5004,12 @@
       <c r="P13" s="34"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="G14" s="77" t="s">
+      <c r="G14" s="80" t="s">
         <v>132</v>
       </c>
-      <c r="H14" s="77"/>
-      <c r="I14" s="77"/>
-      <c r="J14" s="77"/>
+      <c r="H14" s="80"/>
+      <c r="I14" s="80"/>
+      <c r="J14" s="80"/>
       <c r="K14" s="31"/>
       <c r="L14" s="33"/>
       <c r="M14" s="33"/>
@@ -5021,12 +5021,12 @@
       <c r="A15" s="21" t="s">
         <v>145</v>
       </c>
-      <c r="G15" s="77" t="s">
+      <c r="G15" s="80" t="s">
         <v>133</v>
       </c>
-      <c r="H15" s="77"/>
-      <c r="I15" s="77"/>
-      <c r="J15" s="77"/>
+      <c r="H15" s="80"/>
+      <c r="I15" s="80"/>
+      <c r="J15" s="80"/>
       <c r="K15" s="31"/>
       <c r="L15" s="33"/>
       <c r="M15" s="33"/>
@@ -5035,12 +5035,12 @@
       <c r="P15" s="33"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="G16" s="77" t="s">
+      <c r="G16" s="80" t="s">
         <v>134</v>
       </c>
-      <c r="H16" s="77"/>
-      <c r="I16" s="77"/>
-      <c r="J16" s="77"/>
+      <c r="H16" s="80"/>
+      <c r="I16" s="80"/>
+      <c r="J16" s="80"/>
       <c r="K16" s="31"/>
       <c r="L16" s="33"/>
       <c r="M16" s="33"/>
@@ -5049,12 +5049,12 @@
       <c r="P16" s="33"/>
     </row>
     <row r="17" spans="7:16" x14ac:dyDescent="0.25">
-      <c r="G17" s="77" t="s">
+      <c r="G17" s="80" t="s">
         <v>135</v>
       </c>
-      <c r="H17" s="77"/>
-      <c r="I17" s="77"/>
-      <c r="J17" s="77"/>
+      <c r="H17" s="80"/>
+      <c r="I17" s="80"/>
+      <c r="J17" s="80"/>
       <c r="K17" s="31"/>
       <c r="L17" s="33"/>
       <c r="M17" s="33"/>
@@ -5063,12 +5063,12 @@
       <c r="P17" s="33"/>
     </row>
     <row r="18" spans="7:16" x14ac:dyDescent="0.25">
-      <c r="G18" s="77" t="s">
+      <c r="G18" s="80" t="s">
         <v>136</v>
       </c>
-      <c r="H18" s="77"/>
-      <c r="I18" s="77"/>
-      <c r="J18" s="77"/>
+      <c r="H18" s="80"/>
+      <c r="I18" s="80"/>
+      <c r="J18" s="80"/>
       <c r="K18" s="31"/>
       <c r="L18" s="33"/>
       <c r="M18" s="33"/>
@@ -5077,12 +5077,12 @@
       <c r="P18" s="33"/>
     </row>
     <row r="20" spans="7:16" x14ac:dyDescent="0.25">
-      <c r="G20" s="77" t="s">
+      <c r="G20" s="80" t="s">
         <v>137</v>
       </c>
-      <c r="H20" s="77"/>
-      <c r="I20" s="77"/>
-      <c r="J20" s="77"/>
+      <c r="H20" s="80"/>
+      <c r="I20" s="80"/>
+      <c r="J20" s="80"/>
       <c r="K20" s="31"/>
       <c r="L20" s="33"/>
       <c r="M20" s="33"/>
@@ -5091,12 +5091,12 @@
       <c r="P20" s="33"/>
     </row>
     <row r="21" spans="7:16" x14ac:dyDescent="0.25">
-      <c r="G21" s="77" t="s">
+      <c r="G21" s="80" t="s">
         <v>138</v>
       </c>
-      <c r="H21" s="77"/>
-      <c r="I21" s="77"/>
-      <c r="J21" s="77"/>
+      <c r="H21" s="80"/>
+      <c r="I21" s="80"/>
+      <c r="J21" s="80"/>
       <c r="K21" s="31"/>
       <c r="L21" s="33"/>
       <c r="M21" s="33"/>
@@ -5110,12 +5110,12 @@
       </c>
     </row>
     <row r="24" spans="7:16" x14ac:dyDescent="0.25">
-      <c r="G24" s="77" t="s">
+      <c r="G24" s="80" t="s">
         <v>139</v>
       </c>
-      <c r="H24" s="77"/>
-      <c r="I24" s="77"/>
-      <c r="J24" s="77"/>
+      <c r="H24" s="80"/>
+      <c r="I24" s="80"/>
+      <c r="J24" s="80"/>
       <c r="K24" s="31"/>
       <c r="L24" s="33"/>
       <c r="M24" s="33"/>
@@ -5124,12 +5124,12 @@
       <c r="P24" s="33"/>
     </row>
     <row r="25" spans="7:16" x14ac:dyDescent="0.25">
-      <c r="G25" s="77" t="s">
+      <c r="G25" s="80" t="s">
         <v>140</v>
       </c>
-      <c r="H25" s="77"/>
-      <c r="I25" s="77"/>
-      <c r="J25" s="77"/>
+      <c r="H25" s="80"/>
+      <c r="I25" s="80"/>
+      <c r="J25" s="80"/>
       <c r="K25" s="31"/>
       <c r="L25" s="33"/>
       <c r="M25" s="33"/>
@@ -5138,12 +5138,12 @@
       <c r="P25" s="33"/>
     </row>
     <row r="26" spans="7:16" x14ac:dyDescent="0.25">
-      <c r="G26" s="77" t="s">
+      <c r="G26" s="80" t="s">
         <v>142</v>
       </c>
-      <c r="H26" s="77"/>
-      <c r="I26" s="77"/>
-      <c r="J26" s="77"/>
+      <c r="H26" s="80"/>
+      <c r="I26" s="80"/>
+      <c r="J26" s="80"/>
       <c r="K26" s="31"/>
       <c r="L26" s="33"/>
       <c r="M26" s="33"/>
@@ -5153,11 +5153,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="C1:F1"/>
-    <mergeCell ref="G1:J1"/>
-    <mergeCell ref="M10:O10"/>
-    <mergeCell ref="G25:J25"/>
-    <mergeCell ref="L1:O1"/>
     <mergeCell ref="G26:J26"/>
     <mergeCell ref="C10:F10"/>
     <mergeCell ref="G10:J10"/>
@@ -5169,6 +5164,11 @@
     <mergeCell ref="G17:J17"/>
     <mergeCell ref="G18:J18"/>
     <mergeCell ref="G21:J21"/>
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="G1:J1"/>
+    <mergeCell ref="M10:O10"/>
+    <mergeCell ref="G25:J25"/>
+    <mergeCell ref="L1:O1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5941,7 +5941,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="L18" sqref="L18"/>
     </sheetView>
@@ -7060,7 +7060,7 @@
   <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
finished Room.java and Attack.java
</commit_message>
<xml_diff>
--- a/RDG/config/RDG.xlsx
+++ b/RDG/config/RDG.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="10725" windowHeight="8580" firstSheet="3" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="10725" windowHeight="8580" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="6" r:id="rId1"/>
@@ -16,7 +16,6 @@
     <sheet name="Weapons" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="145621"/>
-  <oleSize ref="A1:E27"/>
 </workbook>
 </file>
 
@@ -203,7 +202,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="256">
   <si>
     <t>Axt</t>
   </si>
@@ -685,24 +684,6 @@
     <t>Item_Count</t>
   </si>
   <si>
-    <t>rooms/deadend.png</t>
-  </si>
-  <si>
-    <t>rooms/hallway.png</t>
-  </si>
-  <si>
-    <t>rooms/turn.png</t>
-  </si>
-  <si>
-    <t>rooms/t-junction.png</t>
-  </si>
-  <si>
-    <t>rooms/junction.png</t>
-  </si>
-  <si>
-    <t>rooms/treasure_chamber.png</t>
-  </si>
-  <si>
     <t>monsters/rat_big.png</t>
   </si>
   <si>
@@ -986,6 +967,9 @@
   </si>
   <si>
     <t>Bitte in Excel die Kommetrennzeichen auf "." stellen!!! (google)</t>
+  </si>
+  <si>
+    <t>rooms/tileset.png</t>
   </si>
 </sst>
 </file>
@@ -4493,7 +4477,7 @@
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
     </row>
   </sheetData>
@@ -4505,9 +4489,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="Q17" sqref="Q17"/>
+      <selection pane="topRight" activeCell="Q13" sqref="Q13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4591,7 +4575,7 @@
         <v>158</v>
       </c>
       <c r="L2" s="32" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="M2" s="32" t="s">
         <v>149</v>
@@ -4659,7 +4643,7 @@
         <v>3</v>
       </c>
       <c r="Q3" s="21" t="s">
-        <v>160</v>
+        <v>255</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
@@ -4712,7 +4696,7 @@
         <v>2</v>
       </c>
       <c r="Q4" s="21" t="s">
-        <v>161</v>
+        <v>255</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
@@ -4765,7 +4749,7 @@
         <v>2</v>
       </c>
       <c r="Q5" s="21" t="s">
-        <v>162</v>
+        <v>255</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
@@ -4818,7 +4802,7 @@
         <v>1</v>
       </c>
       <c r="Q6" s="21" t="s">
-        <v>163</v>
+        <v>255</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
@@ -4871,7 +4855,7 @@
         <v>1</v>
       </c>
       <c r="Q7" s="21" t="s">
-        <v>164</v>
+        <v>255</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
@@ -4924,7 +4908,7 @@
         <v>5</v>
       </c>
       <c r="Q8" s="21" t="s">
-        <v>165</v>
+        <v>255</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
@@ -5203,10 +5187,10 @@
         <v>40</v>
       </c>
       <c r="B1" s="42" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="C1" s="42" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="D1" s="43" t="s">
         <v>104</v>
@@ -5374,10 +5358,10 @@
         <v>96</v>
       </c>
       <c r="C1" s="54" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="D1" s="54" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="E1" s="57" t="s">
         <v>78</v>
@@ -5442,10 +5426,10 @@
         <v>4</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5483,10 +5467,10 @@
         <v>2</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5524,10 +5508,10 @@
         <v>2</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5565,10 +5549,10 @@
         <v>2</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5606,10 +5590,10 @@
         <v>2</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5647,10 +5631,10 @@
         <v>5</v>
       </c>
       <c r="L7" s="3" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5688,10 +5672,10 @@
         <v>7</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="M8" s="3" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5729,10 +5713,10 @@
         <v>5</v>
       </c>
       <c r="L9" s="3" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="M9" s="3" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5770,10 +5754,10 @@
         <v>10</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="M10" s="3" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5811,10 +5795,10 @@
         <v>30</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="M11" s="3" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5852,10 +5836,10 @@
         <v>30</v>
       </c>
       <c r="L12" s="3" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="M12" s="3" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5893,10 +5877,10 @@
         <v>30</v>
       </c>
       <c r="L13" s="3" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="M13" s="3" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
@@ -5941,8 +5925,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
@@ -5966,16 +5950,16 @@
         <v>40</v>
       </c>
       <c r="B1" s="50" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="C1" s="63" t="s">
         <v>152</v>
       </c>
       <c r="D1" s="63" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="E1" s="63" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="F1" s="57" t="s">
         <v>76</v>
@@ -6027,10 +6011,10 @@
         <v>0.1</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6062,10 +6046,10 @@
         <v>0.1</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6099,10 +6083,10 @@
         <v>0.1</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6136,10 +6120,10 @@
         <v>0.1</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6173,10 +6157,10 @@
         <v>0.1</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6210,10 +6194,10 @@
         <v>0.15</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6245,10 +6229,10 @@
         <v>0.15</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6282,10 +6266,10 @@
         <v>0.15</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6319,10 +6303,10 @@
         <v>0.15</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6356,10 +6340,10 @@
         <v>0.15</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6393,10 +6377,10 @@
         <v>0.2</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6428,10 +6412,10 @@
         <v>0.2</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6465,10 +6449,10 @@
         <v>0.2</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6502,10 +6486,10 @@
         <v>0.2</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6539,10 +6523,10 @@
         <v>0.2</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
     </row>
     <row r="18" spans="3:7" x14ac:dyDescent="0.25">
@@ -6593,16 +6577,16 @@
         <v>40</v>
       </c>
       <c r="B1" s="50" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="C1" s="63" t="s">
         <v>152</v>
       </c>
       <c r="D1" s="63" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="E1" s="63" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="F1" s="70" t="s">
         <v>39</v>
@@ -6665,10 +6649,10 @@
         <v>1</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -6707,10 +6691,10 @@
         <v>5</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -6748,10 +6732,10 @@
         <v>1</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -6789,10 +6773,10 @@
         <v>5</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -6830,10 +6814,10 @@
         <v>5</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -6871,10 +6855,10 @@
         <v>5</v>
       </c>
       <c r="L7" s="3" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -6912,10 +6896,10 @@
         <v>5</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="M8" s="3" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -6953,10 +6937,10 @@
         <v>5</v>
       </c>
       <c r="L9" s="3" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="M9" s="3" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -6995,10 +6979,10 @@
         <v>5</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="M10" s="3" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
@@ -7036,10 +7020,10 @@
         <v>5</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="M11" s="3" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
@@ -7085,16 +7069,16 @@
         <v>40</v>
       </c>
       <c r="B1" s="23" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="C1" s="30" t="s">
         <v>152</v>
       </c>
       <c r="D1" s="30" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="E1" s="30" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="F1" s="35" t="s">
         <v>50</v>
@@ -7162,10 +7146,10 @@
         <v>55</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -7206,10 +7190,10 @@
         <v>55</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -7250,10 +7234,10 @@
         <v>55</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -7294,10 +7278,10 @@
         <v>55</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="N5" s="3" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -7338,10 +7322,10 @@
         <v>55</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="N6" s="3" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
@@ -7382,10 +7366,10 @@
         <v>55</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="N7" s="3" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -7426,10 +7410,10 @@
         <v>56</v>
       </c>
       <c r="M8" s="3" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="N8" s="3" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -7470,10 +7454,10 @@
         <v>56</v>
       </c>
       <c r="M9" s="3" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="N9" s="3" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
adapted config Files -> added Class Multiplier to Attacks for balancing, changed all big and small images to singlesize Image
</commit_message>
<xml_diff>
--- a/RDG/config/RDG.xlsx
+++ b/RDG/config/RDG.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="10725" windowHeight="8580" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="10725" windowHeight="8580" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="6" r:id="rId1"/>
@@ -27,182 +27,203 @@
   <connection id="2" name="D_Armaments1" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="D:\Dokumente\fh\bif\3\ITP3\Config\Drafts\D_Armaments.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="3" name="D_Armaments2" type="4" refreshedVersion="0" background="1">
+  <connection id="3" name="D_Armaments10" type="4" refreshedVersion="0" background="1">
+    <webPr xml="1" sourceData="1" url="C:\Users\Flo\git\RDG\RDG\config\Drafts\D_Armaments.xml" htmlTables="1" htmlFormat="all"/>
+  </connection>
+  <connection id="4" name="D_Armaments2" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="D:\Dokumente\fh\bif\3\ITP3\Config\Drafts\D_Armaments.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="4" name="D_Armaments3" type="4" refreshedVersion="0" background="1">
+  <connection id="5" name="D_Armaments3" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="D:\Dokumente\fh\bif\3\ITP3\Config\Drafts\D_Armaments.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="5" name="D_Armaments4" type="4" refreshedVersion="0" background="1">
+  <connection id="6" name="D_Armaments4" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="C:\Users\Flo\git\RDG\RDG\config\Drafts\D_Armaments.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="6" name="D_Armaments5" type="4" refreshedVersion="0" background="1">
+  <connection id="7" name="D_Armaments5" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="C:\Users\Flo\git\RDG\RDG\config\Drafts\D_Armaments.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="7" name="D_Armaments6" type="4" refreshedVersion="0" background="1">
+  <connection id="8" name="D_Armaments6" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="C:\Users\Flo\git\RDG\RDG\config\Drafts\D_Armaments.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="8" name="D_Armaments7" type="4" refreshedVersion="0" background="1">
+  <connection id="9" name="D_Armaments7" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="C:\Users\Flo\git\RDG\RDG\config\Drafts\D_Armaments.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="9" name="D_Armaments8" type="4" refreshedVersion="0" background="1">
+  <connection id="10" name="D_Armaments8" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="C:\Users\Flo\git\RDG\RDG\config\Drafts\D_Armaments.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="10" name="D_Armaments9" type="4" refreshedVersion="0" background="1">
+  <connection id="11" name="D_Armaments9" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="C:\Users\Flo\git\RDG\RDG\config\Drafts\D_Armaments.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="11" name="D_Attacks" type="4" refreshedVersion="0" background="1">
+  <connection id="12" name="D_Attacks" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="D:\Dokumente\fh\bif\3\ITP3\Config\Drafts\D_Attacks.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="12" name="D_Attacks1" type="4" refreshedVersion="0" background="1">
+  <connection id="13" name="D_Attacks1" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="C:\Users\Flo\git\RDG\RDG\config\Drafts\D_Attacks.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="13" name="D_Attacks2" type="4" refreshedVersion="0" background="1">
+  <connection id="14" name="D_Attacks2" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="C:\Users\Flo\git\RDG\RDG\config\Drafts\D_Attacks.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="14" name="D_Attacks3" type="4" refreshedVersion="0" background="1">
+  <connection id="15" name="D_Attacks3" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="C:\Users\Flo\git\RDG\RDG\config\Drafts\D_Attacks.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="15" name="D_Attacks4" type="4" refreshedVersion="0" background="1">
+  <connection id="16" name="D_Attacks4" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="C:\Users\Flo\git\RDG\RDG\config\Drafts\D_Attacks.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="16" name="D_Attacks5" type="4" refreshedVersion="0" background="1">
+  <connection id="17" name="D_Attacks5" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="C:\Users\Flo\git\RDG\RDG\config\Drafts\D_Attacks.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="17" name="D_Monsters" type="4" refreshedVersion="0" background="1">
+  <connection id="18" name="D_Attacks6" type="4" refreshedVersion="0" background="1">
+    <webPr xml="1" sourceData="1" url="C:\Users\Flo\git\RDG\RDG\config\Drafts\D_Attacks.xml" htmlTables="1" htmlFormat="all"/>
+  </connection>
+  <connection id="19" name="D_Monsters" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="D:\Dokumente\fh\bif\3\ITP3\Config\Drafts\D_Monsters.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="18" name="D_Monsters1" type="4" refreshedVersion="0" background="1">
+  <connection id="20" name="D_Monsters1" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="D:\Dokumente\fh\bif\3\ITP3\Config\Drafts\D_Monsters.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="19" name="D_Monsters2" type="4" refreshedVersion="0" background="1">
+  <connection id="21" name="D_Monsters10" type="4" refreshedVersion="0" background="1">
+    <webPr xml="1" sourceData="1" url="C:\Users\Flo\git\RDG\RDG\config\Drafts\D_Monsters.xml" htmlTables="1" htmlFormat="all"/>
+  </connection>
+  <connection id="22" name="D_Monsters2" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="D:\Dokumente\fh\bif\3\ITP3\Config\Drafts\D_Monsters.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="20" name="D_Monsters3" type="4" refreshedVersion="0" background="1">
+  <connection id="23" name="D_Monsters3" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="D:\Dokumente\fh\bif\3\ITP3\Config\Drafts\D_Monsters.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="21" name="D_Monsters4" type="4" refreshedVersion="0" background="1">
+  <connection id="24" name="D_Monsters4" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="C:\Users\Flo\git\RDG\RDG\config\Drafts\D_Monsters.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="22" name="D_Monsters5" type="4" refreshedVersion="0" background="1">
+  <connection id="25" name="D_Monsters5" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="C:\Users\Flo\git\RDG\RDG\config\Drafts\D_Monsters.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="23" name="D_Monsters6" type="4" refreshedVersion="0" background="1">
+  <connection id="26" name="D_Monsters6" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="C:\Users\Flo\git\RDG\RDG\config\Drafts\D_Monsters.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="24" name="D_Monsters7" type="4" refreshedVersion="0" background="1">
+  <connection id="27" name="D_Monsters7" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="C:\Users\Flo\git\RDG\RDG\config\Drafts\D_Monsters.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="25" name="D_Monsters8" type="4" refreshedVersion="0" background="1">
+  <connection id="28" name="D_Monsters8" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="C:\Users\Flo\git\RDG\RDG\config\Drafts\D_Monsters.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="26" name="D_Potions" type="4" refreshedVersion="0" background="1">
+  <connection id="29" name="D_Monsters9" type="4" refreshedVersion="0" background="1">
+    <webPr xml="1" sourceData="1" url="C:\Users\Flo\git\RDG\RDG\config\Drafts\D_Monsters.xml" htmlTables="1" htmlFormat="all"/>
+  </connection>
+  <connection id="30" name="D_Potions" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="D:\Dokumente\fh\bif\3\ITP3\Config\Drafts\D_Potions.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="27" name="D_Potions1" type="4" refreshedVersion="0" background="1">
+  <connection id="31" name="D_Potions1" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="D:\Dokumente\fh\bif\3\ITP3\Config\Drafts\D_Potions.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="28" name="D_Potions2" type="4" refreshedVersion="0" background="1">
+  <connection id="32" name="D_Potions10" type="4" refreshedVersion="0" background="1">
+    <webPr xml="1" sourceData="1" url="C:\Users\Flo\git\RDG\RDG\config\Drafts\D_Potions.xml" htmlTables="1" htmlFormat="all"/>
+  </connection>
+  <connection id="33" name="D_Potions2" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="D:\Dokumente\fh\bif\3\ITP3\Config\Drafts\D_Potions.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="29" name="D_Potions3" type="4" refreshedVersion="0" background="1">
+  <connection id="34" name="D_Potions3" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="D:\Dokumente\fh\bif\3\ITP3\Config\Drafts\D_Potions.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="30" name="D_Potions4" type="4" refreshedVersion="0" background="1">
+  <connection id="35" name="D_Potions4" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="C:\Users\Flo\git\RDG\RDG\config\Drafts\D_Potions.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="31" name="D_Potions5" type="4" refreshedVersion="0" background="1">
+  <connection id="36" name="D_Potions5" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="C:\Users\Flo\git\RDG\RDG\config\Drafts\D_Potions.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="32" name="D_Potions6" type="4" refreshedVersion="0" background="1">
+  <connection id="37" name="D_Potions6" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="C:\Users\Flo\git\RDG\RDG\config\Drafts\D_Potions.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="33" name="D_Potions7" type="4" refreshedVersion="0" background="1">
+  <connection id="38" name="D_Potions7" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="C:\Users\Flo\git\RDG\RDG\config\Drafts\D_Potions.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="34" name="D_Potions8" type="4" refreshedVersion="0" background="1">
+  <connection id="39" name="D_Potions8" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="C:\Users\Flo\git\RDG\RDG\config\Drafts\D_Potions.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="35" name="D_Potions9" type="4" refreshedVersion="0" background="1">
+  <connection id="40" name="D_Potions9" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="C:\Users\Flo\git\RDG\RDG\config\Drafts\D_Potions.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="36" name="D_Rooms" type="4" refreshedVersion="0" background="1">
+  <connection id="41" name="D_Rooms" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="D:\Dokumente\fh\bif\3\ITP3\Config\Drafts\D_Rooms.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="37" name="D_Rooms_test" type="4" refreshedVersion="0" background="1">
+  <connection id="42" name="D_Rooms_test" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="D:\Dokumente\fh\bif\3\ITP3\Config\Drafts\D_Rooms_test.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="38" name="D_Rooms1" type="4" refreshedVersion="0" background="1">
+  <connection id="43" name="D_Rooms1" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="D:\Dokumente\fh\bif\3\ITP3\Config\Drafts\D_Rooms.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="39" name="D_Rooms2" type="4" refreshedVersion="0" background="1">
+  <connection id="44" name="D_Rooms2" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="D:\Dokumente\fh\bif\3\ITP3\Config\Drafts\D_Rooms.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="40" name="D_Rooms3" type="4" refreshedVersion="0" background="1">
+  <connection id="45" name="D_Rooms3" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="D:\Dokumente\fh\bif\3\ITP3\Config\Drafts\D_Rooms.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="41" name="D_Rooms4" type="4" refreshedVersion="0" background="1">
+  <connection id="46" name="D_Rooms4" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="C:\Users\Flo\git\RDG\RDG\config\Drafts\D_Rooms.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="42" name="D_Rooms5" type="4" refreshedVersion="0" background="1">
+  <connection id="47" name="D_Rooms5" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="C:\Users\Flo\git\RDG\RDG\config\Drafts\D_Rooms.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="43" name="D_Rooms6" type="4" refreshedVersion="0" background="1">
+  <connection id="48" name="D_Rooms6" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="C:\Users\Flo\git\RDG\RDG\config\Drafts\D_Rooms.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="44" name="D_Rooms7" type="4" refreshedVersion="0" background="1">
+  <connection id="49" name="D_Rooms7" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="C:\Users\Flo\git\RDG\RDG\config\Drafts\D_Rooms.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="45" name="D_text" type="4" refreshedVersion="0" background="1">
+  <connection id="50" name="D_text" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="D:\Dokumente\fh\bif\3\ITP3\Config\Drafts\D_text.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="46" name="D_text1" type="4" refreshedVersion="0" background="1">
+  <connection id="51" name="D_text1" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="D:\Dokumente\fh\bif\3\ITP3\Config\Drafts\D_text.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="47" name="D_text2" type="4" refreshedVersion="0" background="1">
+  <connection id="52" name="D_text2" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="D:\Dokumente\fh\bif\3\ITP3\Config\Drafts\D_text.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="48" name="D_Weapons" type="4" refreshedVersion="0" background="1">
+  <connection id="53" name="D_Weapons" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="D:\Dokumente\fh\bif\3\ITP3\Config\Drafts\D_Weapons.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="49" name="D_Weapons1" type="4" refreshedVersion="0" background="1">
+  <connection id="54" name="D_Weapons1" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="D:\Dokumente\fh\bif\3\ITP3\Config\Drafts\D_Weapons.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="50" name="D_Weapons10" type="4" refreshedVersion="0" background="1">
+  <connection id="55" name="D_Weapons10" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="C:\Users\Flo\git\RDG\RDG\config\Drafts\D_Weapons.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="51" name="D_Weapons2" type="4" refreshedVersion="0" background="1">
+  <connection id="56" name="D_Weapons11" type="4" refreshedVersion="0" background="1">
+    <webPr xml="1" sourceData="1" url="C:\Users\Flo\git\RDG\RDG\config\Drafts\D_Weapons.xml" htmlTables="1" htmlFormat="all"/>
+  </connection>
+  <connection id="57" name="D_Weapons2" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="D:\Dokumente\fh\bif\3\ITP3\Config\Drafts\D_Weapons.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="52" name="D_Weapons3" type="4" refreshedVersion="0" background="1">
+  <connection id="58" name="D_Weapons3" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="D:\Dokumente\fh\bif\3\ITP3\Config\Drafts\D_Weapons.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="53" name="D_Weapons4" type="4" refreshedVersion="0" background="1">
+  <connection id="59" name="D_Weapons4" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="D:\Dokumente\fh\bif\3\ITP3\Config\Drafts\D_Weapons.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="54" name="D_Weapons5" type="4" refreshedVersion="0" background="1">
+  <connection id="60" name="D_Weapons5" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="C:\Users\Flo\git\RDG\RDG\config\Drafts\D_Weapons.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="55" name="D_Weapons6" type="4" refreshedVersion="0" background="1">
+  <connection id="61" name="D_Weapons6" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="C:\Users\Flo\git\RDG\RDG\config\Drafts\D_Weapons.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="56" name="D_Weapons7" type="4" refreshedVersion="0" background="1">
+  <connection id="62" name="D_Weapons7" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="C:\Users\Flo\git\RDG\RDG\config\Drafts\D_Weapons.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="57" name="D_Weapons8" type="4" refreshedVersion="0" background="1">
+  <connection id="63" name="D_Weapons8" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="C:\Users\Flo\git\RDG\RDG\config\Drafts\D_Weapons.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="58" name="D_Weapons9" type="4" refreshedVersion="0" background="1">
+  <connection id="64" name="D_Weapons9" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="C:\Users\Flo\git\RDG\RDG\config\Drafts\D_Weapons.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="59" name="Schema_Potions" type="4" refreshedVersion="0" background="1">
+  <connection id="65" name="Monsters" type="4" refreshedVersion="0" background="1">
+    <webPr xml="1" sourceData="1" url="C:\Users\Flo\git\RDG\RDG\config\Results\Monsters.xml" htmlTables="1" htmlFormat="all"/>
+  </connection>
+  <connection id="66" name="Schema_Potions" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="D:\Dokumente\fh\bif\3\ITP3\Config\Schema_Potions.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="209">
   <si>
     <t>Axt</t>
   </si>
@@ -573,12 +594,6 @@
     <t>Image</t>
   </si>
   <si>
-    <t>Image Big</t>
-  </si>
-  <si>
-    <t>Image Small</t>
-  </si>
-  <si>
     <t>Door Positions</t>
   </si>
   <si>
@@ -684,276 +699,6 @@
     <t>Item_Count</t>
   </si>
   <si>
-    <t>monsters/rat_big.png</t>
-  </si>
-  <si>
-    <t>monsters/spider_big.png</t>
-  </si>
-  <si>
-    <t>monsters/frog_big.png</t>
-  </si>
-  <si>
-    <t>monsters/bat_big.png</t>
-  </si>
-  <si>
-    <t>monsters/salamander_big.png</t>
-  </si>
-  <si>
-    <t>monsters/goblin_big.png</t>
-  </si>
-  <si>
-    <t>monsters/gremlin_big.png</t>
-  </si>
-  <si>
-    <t>monsters/ghost_big.png</t>
-  </si>
-  <si>
-    <t>monsters/zombie_big.png</t>
-  </si>
-  <si>
-    <t>monsters/ogre_big.png</t>
-  </si>
-  <si>
-    <t>monsters/giant_big.png</t>
-  </si>
-  <si>
-    <t>monsters/cyclops_big.png</t>
-  </si>
-  <si>
-    <t>monsters/rat_small.png</t>
-  </si>
-  <si>
-    <t>monsters/spider_small.png</t>
-  </si>
-  <si>
-    <t>monsters/frog_small.png</t>
-  </si>
-  <si>
-    <t>monsters/bat_small.png</t>
-  </si>
-  <si>
-    <t>monsters/salamander_small.png</t>
-  </si>
-  <si>
-    <t>monsters/goblin_small.png</t>
-  </si>
-  <si>
-    <t>monsters/gremlin_small.png</t>
-  </si>
-  <si>
-    <t>monsters/ghost_small.png</t>
-  </si>
-  <si>
-    <t>monsters/zombie_small.png</t>
-  </si>
-  <si>
-    <t>monsters/ogre_small.png</t>
-  </si>
-  <si>
-    <t>monsters/giant_small.png</t>
-  </si>
-  <si>
-    <t>monsters/cyclops_small.png</t>
-  </si>
-  <si>
-    <t>armaments/leather_helmet_big.png</t>
-  </si>
-  <si>
-    <t>armaments/leather_harness_big.png</t>
-  </si>
-  <si>
-    <t>armaments/leather_gauntlets_big.png</t>
-  </si>
-  <si>
-    <t>armaments/leather_cuisse_big.png</t>
-  </si>
-  <si>
-    <t>armaments/leather_boots_big.png</t>
-  </si>
-  <si>
-    <t>armaments/habergeon_helmet_big.png</t>
-  </si>
-  <si>
-    <t>armaments/habergeon_harness_big.png</t>
-  </si>
-  <si>
-    <t>armaments/habergeon_gauntlets_big.png</t>
-  </si>
-  <si>
-    <t>armaments/habergeon_cuisse_big.png</t>
-  </si>
-  <si>
-    <t>armaments/habergeon_boots_big.png</t>
-  </si>
-  <si>
-    <t>armaments/plate_helmet_big.png</t>
-  </si>
-  <si>
-    <t>armaments/plate_harness_big.png</t>
-  </si>
-  <si>
-    <t>armaments/plate_gauntlets_big.png</t>
-  </si>
-  <si>
-    <t>armaments/plate_cuisse_big.png</t>
-  </si>
-  <si>
-    <t>armaments/plate_boots_big.png</t>
-  </si>
-  <si>
-    <t>armaments/leather_helmet_small.png</t>
-  </si>
-  <si>
-    <t>armaments/leather_harness_small.png</t>
-  </si>
-  <si>
-    <t>armaments/leather_gauntlets_small.png</t>
-  </si>
-  <si>
-    <t>armaments/leather_cuisse_small.png</t>
-  </si>
-  <si>
-    <t>armaments/leather_boots_small.png</t>
-  </si>
-  <si>
-    <t>armaments/habergeon_helmet_small.png</t>
-  </si>
-  <si>
-    <t>armaments/habergeon_harness_small.png</t>
-  </si>
-  <si>
-    <t>armaments/habergeon_gauntlets_small.png</t>
-  </si>
-  <si>
-    <t>armaments/habergeon_cuisse_small.png</t>
-  </si>
-  <si>
-    <t>armaments/habergeon_boots_small.png</t>
-  </si>
-  <si>
-    <t>armaments/plate_helmet_small.png</t>
-  </si>
-  <si>
-    <t>armaments/plate_harness_small.png</t>
-  </si>
-  <si>
-    <t>armaments/plate_gauntlets_small.png</t>
-  </si>
-  <si>
-    <t>armaments/plate_cuisse_small.png</t>
-  </si>
-  <si>
-    <t>armaments/plate_boots_small.png</t>
-  </si>
-  <si>
-    <t>potions/instant_cure_big.png</t>
-  </si>
-  <si>
-    <t>potions/regeneration_big.png</t>
-  </si>
-  <si>
-    <t>potions/antidote_big.png</t>
-  </si>
-  <si>
-    <t>potions/strength_big.png</t>
-  </si>
-  <si>
-    <t>potions/speed_big.png</t>
-  </si>
-  <si>
-    <t>potions/accuracy_big.png</t>
-  </si>
-  <si>
-    <t>potions/blindness_big.png</t>
-  </si>
-  <si>
-    <t>potions/slowness_big.png</t>
-  </si>
-  <si>
-    <t>potions/poison_big.png</t>
-  </si>
-  <si>
-    <t>potions/weakness_big.png</t>
-  </si>
-  <si>
-    <t>potions/instant_cure_small.png</t>
-  </si>
-  <si>
-    <t>potions/regeneration_small.png</t>
-  </si>
-  <si>
-    <t>potions/antidote_small.png</t>
-  </si>
-  <si>
-    <t>potions/strength_small.png</t>
-  </si>
-  <si>
-    <t>potions/speed_small.png</t>
-  </si>
-  <si>
-    <t>potions/accuracy_small.png</t>
-  </si>
-  <si>
-    <t>potions/blindness_small.png</t>
-  </si>
-  <si>
-    <t>potions/slowness_small.png</t>
-  </si>
-  <si>
-    <t>potions/poison_small.png</t>
-  </si>
-  <si>
-    <t>potions/weakness_small.png</t>
-  </si>
-  <si>
-    <t>weapons/fists_big.png</t>
-  </si>
-  <si>
-    <t>weapons/dagger_big.png</t>
-  </si>
-  <si>
-    <t>weapons/axt_big.png</t>
-  </si>
-  <si>
-    <t>weapons/sword_big.png</t>
-  </si>
-  <si>
-    <t>weapons/shield_big.png</t>
-  </si>
-  <si>
-    <t>weapons/sabre_big.png</t>
-  </si>
-  <si>
-    <t>weapons/longsword_big.png</t>
-  </si>
-  <si>
-    <t>weapons/bow_big.png</t>
-  </si>
-  <si>
-    <t>weapons/fists_small.png</t>
-  </si>
-  <si>
-    <t>weapons/dagger_small.png</t>
-  </si>
-  <si>
-    <t>weapons/axt_small.png</t>
-  </si>
-  <si>
-    <t>weapons/sword_small.png</t>
-  </si>
-  <si>
-    <t>weapons/shield_small.png</t>
-  </si>
-  <si>
-    <t>weapons/sabre_small.png</t>
-  </si>
-  <si>
-    <t>weapons/longsword_small.png</t>
-  </si>
-  <si>
-    <t>weapons/bow_small.png</t>
-  </si>
-  <si>
     <t>Stats Low Multiplier</t>
   </si>
   <si>
@@ -970,6 +715,141 @@
   </si>
   <si>
     <t>rooms/tileset.png</t>
+  </si>
+  <si>
+    <t>monsters/rat.png</t>
+  </si>
+  <si>
+    <t>monsters/spider.png</t>
+  </si>
+  <si>
+    <t>monsters/frog.png</t>
+  </si>
+  <si>
+    <t>monsters/bat.png</t>
+  </si>
+  <si>
+    <t>monsters/salamander.png</t>
+  </si>
+  <si>
+    <t>monsters/goblin.png</t>
+  </si>
+  <si>
+    <t>monsters/gremlin.png</t>
+  </si>
+  <si>
+    <t>monsters/ghost.png</t>
+  </si>
+  <si>
+    <t>monsters/zombie.png</t>
+  </si>
+  <si>
+    <t>monsters/ogre.png</t>
+  </si>
+  <si>
+    <t>monsters/giant.png</t>
+  </si>
+  <si>
+    <t>monsters/cyclops.png</t>
+  </si>
+  <si>
+    <t>armaments/leather_helmet.png</t>
+  </si>
+  <si>
+    <t>armaments/leather_harness.png</t>
+  </si>
+  <si>
+    <t>armaments/leather_gauntlets.png</t>
+  </si>
+  <si>
+    <t>armaments/leather_cuisse.png</t>
+  </si>
+  <si>
+    <t>armaments/leather_boots.png</t>
+  </si>
+  <si>
+    <t>armaments/habergeon_helmet.png</t>
+  </si>
+  <si>
+    <t>armaments/habergeon_harness.png</t>
+  </si>
+  <si>
+    <t>armaments/habergeon_gauntlets.png</t>
+  </si>
+  <si>
+    <t>armaments/habergeon_cuisse.png</t>
+  </si>
+  <si>
+    <t>armaments/habergeon_boots.png</t>
+  </si>
+  <si>
+    <t>armaments/plate_helmet.png</t>
+  </si>
+  <si>
+    <t>armaments/plate_harness.png</t>
+  </si>
+  <si>
+    <t>armaments/plate_gauntlets.png</t>
+  </si>
+  <si>
+    <t>armaments/plate_cuisse.png</t>
+  </si>
+  <si>
+    <t>armaments/plate_boots.png</t>
+  </si>
+  <si>
+    <t>potions/instant_cure.png</t>
+  </si>
+  <si>
+    <t>potions/regeneration.png</t>
+  </si>
+  <si>
+    <t>potions/antidote.png</t>
+  </si>
+  <si>
+    <t>potions/strength.png</t>
+  </si>
+  <si>
+    <t>potions/speed.png</t>
+  </si>
+  <si>
+    <t>potions/accuracy.png</t>
+  </si>
+  <si>
+    <t>potions/blindness.png</t>
+  </si>
+  <si>
+    <t>potions/slowness.png</t>
+  </si>
+  <si>
+    <t>potions/poison.png</t>
+  </si>
+  <si>
+    <t>potions/weakness.png</t>
+  </si>
+  <si>
+    <t>weapons/fists.png</t>
+  </si>
+  <si>
+    <t>weapons/dagger.png</t>
+  </si>
+  <si>
+    <t>weapons/axt.png</t>
+  </si>
+  <si>
+    <t>weapons/sword.png</t>
+  </si>
+  <si>
+    <t>weapons/shield.png</t>
+  </si>
+  <si>
+    <t>weapons/sabre.png</t>
+  </si>
+  <si>
+    <t>weapons/longsword.png</t>
+  </si>
+  <si>
+    <t>weapons/bow.png</t>
   </si>
 </sst>
 </file>
@@ -1224,7 +1104,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1442,6 +1322,9 @@
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="1" fontId="2" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1451,9 +1334,6 @@
     <xf numFmtId="1" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="1" fontId="2" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1462,12 +1342,74 @@
     </xf>
     <xf numFmtId="1" fontId="2" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="99">
+  <dxfs count="97">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Verdana"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Verdana"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1485,14 +1427,45 @@
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Verdana"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right/>
         <top/>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -1940,39 +1913,6 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Verdana"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
     </dxf>
     <dxf>
       <font>
@@ -2495,33 +2435,6 @@
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right/>
-        <top/>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Verdana"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
         <top style="thin">
           <color indexed="64"/>
         </top>
@@ -2886,33 +2799,6 @@
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Verdana"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
@@ -3458,64 +3344,6 @@
         </bottom>
         <vertical/>
         <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Verdana"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Verdana"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -3731,7 +3559,60 @@
       </xsd:element>
     </xsd:schema>
   </Schema>
-  <Schema ID="Schema33">
+  <Schema ID="Schema7">
+    <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns="">
+      <xsd:element nillable="true" name="Attacks">
+        <xsd:complexType>
+          <xsd:sequence minOccurs="0">
+            <xsd:element minOccurs="0" maxOccurs="unbounded" nillable="true" name="Attack" form="unqualified">
+              <xsd:complexType>
+                <xsd:sequence minOccurs="0">
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Name" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:double" name="Class_Multiplier" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:double" name="Stats_Low_Multiplier" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:double" name="Stats_High_Multiplier" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:double" name="HP_Damage" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:double" name="Hit_Probability" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Effect" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:double" name="x" form="unqualified"/>
+                </xsd:sequence>
+              </xsd:complexType>
+            </xsd:element>
+          </xsd:sequence>
+        </xsd:complexType>
+      </xsd:element>
+    </xsd:schema>
+  </Schema>
+  <Schema ID="Schema10">
+    <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns="">
+      <xsd:element nillable="true" name="Monsters">
+        <xsd:complexType>
+          <xsd:sequence minOccurs="0">
+            <xsd:element minOccurs="0" maxOccurs="unbounded" nillable="true" name="Monster" form="unqualified">
+              <xsd:complexType>
+                <xsd:sequence minOccurs="0">
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Name" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Level" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:double" name="Class_Multiplier" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:double" name="Stats_Low_Multiplier" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:double" name="Stats_High_Multiplier" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="HP" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="Strength" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="Speed" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="Accuracy" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Kill_Bonus_Type" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="Kill_Bonus_Low" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="Kill_Bonus_High" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Image" form="unqualified"/>
+                </xsd:sequence>
+              </xsd:complexType>
+            </xsd:element>
+          </xsd:sequence>
+        </xsd:complexType>
+      </xsd:element>
+    </xsd:schema>
+  </Schema>
+  <Schema ID="Schema13">
     <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns="">
       <xsd:element nillable="true" name="Armaments">
         <xsd:complexType>
@@ -3748,8 +3629,7 @@
                   <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="Speed" form="unqualified"/>
                   <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Type" form="unqualified"/>
                   <xsd:element minOccurs="0" nillable="true" type="xsd:double" name="Bonus" form="unqualified"/>
-                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Image_Big" form="unqualified"/>
-                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Image_Small" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Image" form="unqualified"/>
                 </xsd:sequence>
               </xsd:complexType>
             </xsd:element>
@@ -3758,59 +3638,7 @@
       </xsd:element>
     </xsd:schema>
   </Schema>
-  <Schema ID="Schema34">
-    <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns="">
-      <xsd:element nillable="true" name="Attacks">
-        <xsd:complexType>
-          <xsd:sequence minOccurs="0">
-            <xsd:element minOccurs="0" maxOccurs="unbounded" nillable="true" name="Attack" form="unqualified">
-              <xsd:complexType>
-                <xsd:sequence minOccurs="0">
-                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Name" form="unqualified"/>
-                  <xsd:element minOccurs="0" nillable="true" type="xsd:double" name="Stats_Low_Multiplier" form="unqualified"/>
-                  <xsd:element minOccurs="0" nillable="true" type="xsd:double" name="Stats_High_Multiplier" form="unqualified"/>
-                  <xsd:element minOccurs="0" nillable="true" type="xsd:double" name="HP_Damage" form="unqualified"/>
-                  <xsd:element minOccurs="0" nillable="true" type="xsd:double" name="Hit_Probability" form="unqualified"/>
-                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Effect" form="unqualified"/>
-                  <xsd:element minOccurs="0" nillable="true" type="xsd:double" name="x" form="unqualified"/>
-                </xsd:sequence>
-              </xsd:complexType>
-            </xsd:element>
-          </xsd:sequence>
-        </xsd:complexType>
-      </xsd:element>
-    </xsd:schema>
-  </Schema>
-  <Schema ID="Schema35">
-    <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns="">
-      <xsd:element nillable="true" name="Monsters">
-        <xsd:complexType>
-          <xsd:sequence minOccurs="0">
-            <xsd:element minOccurs="0" maxOccurs="unbounded" nillable="true" name="Monster" form="unqualified">
-              <xsd:complexType>
-                <xsd:sequence minOccurs="0">
-                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Name" form="unqualified"/>
-                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Level" form="unqualified"/>
-                  <xsd:element minOccurs="0" nillable="true" type="xsd:double" name="Stats_Low_Multiplier" form="unqualified"/>
-                  <xsd:element minOccurs="0" nillable="true" type="xsd:double" name="Stats_High_Multiplier" form="unqualified"/>
-                  <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="HP" form="unqualified"/>
-                  <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="Strength" form="unqualified"/>
-                  <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="Speed" form="unqualified"/>
-                  <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="Accuracy" form="unqualified"/>
-                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Kill_Bonus_Type" form="unqualified"/>
-                  <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="Kill_Bonus_Low" form="unqualified"/>
-                  <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="Kill_Bonus_High" form="unqualified"/>
-                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Image_Big" form="unqualified"/>
-                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Image_Small" form="unqualified"/>
-                </xsd:sequence>
-              </xsd:complexType>
-            </xsd:element>
-          </xsd:sequence>
-        </xsd:complexType>
-      </xsd:element>
-    </xsd:schema>
-  </Schema>
-  <Schema ID="Schema36">
+  <Schema ID="Schema14">
     <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns="">
       <xsd:element nillable="true" name="Potions">
         <xsd:complexType>
@@ -3829,8 +3657,7 @@
                   <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Mode" form="unqualified"/>
                   <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="x" form="unqualified"/>
                   <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="n" form="unqualified"/>
-                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Image_Big" form="unqualified"/>
-                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Image_Small" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Image" form="unqualified"/>
                 </xsd:sequence>
               </xsd:complexType>
             </xsd:element>
@@ -3839,7 +3666,7 @@
       </xsd:element>
     </xsd:schema>
   </Schema>
-  <Schema ID="Schema37">
+  <Schema ID="Schema15">
     <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns="">
       <xsd:element nillable="true" name="Weapons">
         <xsd:complexType>
@@ -3859,8 +3686,7 @@
                   <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="Slots" form="unqualified"/>
                   <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="Max" form="unqualified"/>
                   <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Type" form="unqualified"/>
-                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Image_Big" form="unqualified"/>
-                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Image_Small" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Image" form="unqualified"/>
                 </xsd:sequence>
               </xsd:complexType>
             </xsd:element>
@@ -3869,80 +3695,80 @@
       </xsd:element>
     </xsd:schema>
   </Schema>
-  <Map ID="62" Name="Armaments_Map" RootElement="Armaments" SchemaID="Schema33" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true">
-    <DataBinding FileBinding="true" ConnectionID="10" DataBindingLoadMode="1"/>
+  <Map ID="74" Name="Armaments_Map" RootElement="Armaments" SchemaID="Schema13" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true">
+    <DataBinding FileBinding="true" ConnectionID="3" DataBindingLoadMode="1"/>
   </Map>
-  <Map ID="63" Name="Attacks_Map" RootElement="Attacks" SchemaID="Schema34" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true">
-    <DataBinding FileBinding="true" ConnectionID="16" DataBindingLoadMode="1"/>
+  <Map ID="68" Name="Attacks_Map" RootElement="Attacks" SchemaID="Schema7" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true">
+    <DataBinding FileBinding="true" ConnectionID="18" DataBindingLoadMode="1"/>
   </Map>
-  <Map ID="64" Name="Monsters_Map" RootElement="Monsters" SchemaID="Schema35" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true">
-    <DataBinding FileBinding="true" ConnectionID="25" DataBindingLoadMode="1"/>
+  <Map ID="71" Name="Monsters_Map" RootElement="Monsters" SchemaID="Schema10" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true">
+    <DataBinding FileBinding="true" ConnectionID="21" DataBindingLoadMode="1"/>
   </Map>
-  <Map ID="65" Name="Potions_Map" RootElement="Potions" SchemaID="Schema36" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true">
-    <DataBinding FileBinding="true" ConnectionID="35" DataBindingLoadMode="1"/>
+  <Map ID="75" Name="Potions_Map" RootElement="Potions" SchemaID="Schema14" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true">
+    <DataBinding FileBinding="true" ConnectionID="32" DataBindingLoadMode="1"/>
   </Map>
   <Map ID="60" Name="Rooms_Map" RootElement="Rooms" SchemaID="Schema31" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true">
-    <DataBinding FileBinding="true" ConnectionID="44" DataBindingLoadMode="1"/>
+    <DataBinding FileBinding="true" ConnectionID="49" DataBindingLoadMode="1"/>
   </Map>
-  <Map ID="66" Name="Weapons_Map" RootElement="Weapons" SchemaID="Schema37" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true">
-    <DataBinding FileBinding="true" ConnectionID="50" DataBindingLoadMode="1"/>
+  <Map ID="76" Name="Weapons_Map" RootElement="Weapons" SchemaID="Schema15" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true">
+    <DataBinding FileBinding="true" ConnectionID="56" DataBindingLoadMode="1"/>
   </Map>
 </MapInfo>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table9" displayName="Table9" ref="A2:Q8" tableType="xml" totalsRowShown="0" headerRowDxfId="98" headerRowBorderDxfId="97" connectionId="44">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table9" displayName="Table9" ref="A2:Q8" tableType="xml" totalsRowShown="0" headerRowDxfId="96" headerRowBorderDxfId="95" connectionId="49">
   <autoFilter ref="A2:Q8"/>
   <tableColumns count="17">
-    <tableColumn id="1" uniqueName="Name" name="Name" dataDxfId="96">
+    <tableColumn id="1" uniqueName="Name" name="Name" dataDxfId="94">
       <xmlColumnPr mapId="60" xpath="/Rooms/Room/Name" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="2" uniqueName="Description" name="Description" dataDxfId="95">
+    <tableColumn id="2" uniqueName="Description" name="Description" dataDxfId="93">
       <xmlColumnPr mapId="60" xpath="/Rooms/Room/Description" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="3" uniqueName="N" name="N" dataDxfId="94">
+    <tableColumn id="3" uniqueName="N" name="N" dataDxfId="92">
       <xmlColumnPr mapId="60" xpath="/Rooms/Room/Door_Positions/N" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="4" uniqueName="E" name="E" dataDxfId="93">
+    <tableColumn id="4" uniqueName="E" name="E" dataDxfId="91">
       <xmlColumnPr mapId="60" xpath="/Rooms/Room/Door_Positions/E" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="5" uniqueName="S" name="S" dataDxfId="92">
+    <tableColumn id="5" uniqueName="S" name="S" dataDxfId="90">
       <xmlColumnPr mapId="60" xpath="/Rooms/Room/Door_Positions/S" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="6" uniqueName="W" name="W" dataDxfId="91">
+    <tableColumn id="6" uniqueName="W" name="W" dataDxfId="89">
       <xmlColumnPr mapId="60" xpath="/Rooms/Room/Door_Positions/W" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="7" uniqueName="no" name="no" dataDxfId="90">
+    <tableColumn id="7" uniqueName="no" name="no" dataDxfId="88">
       <xmlColumnPr mapId="60" xpath="/Rooms/Room/Monster/no" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="8" uniqueName="easy" name="easy" dataDxfId="89">
+    <tableColumn id="8" uniqueName="easy" name="easy" dataDxfId="87">
       <xmlColumnPr mapId="60" xpath="/Rooms/Room/Monster/easy" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="9" uniqueName="normal" name="normal" dataDxfId="88">
+    <tableColumn id="9" uniqueName="normal" name="normal" dataDxfId="86">
       <xmlColumnPr mapId="60" xpath="/Rooms/Room/Monster/normal" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="10" uniqueName="hard" name="hard" dataDxfId="87">
+    <tableColumn id="10" uniqueName="hard" name="hard" dataDxfId="85">
       <xmlColumnPr mapId="60" xpath="/Rooms/Room/Monster/hard" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="11" uniqueName="Item_Multiplier" name="Item_Multiplier" dataDxfId="86">
+    <tableColumn id="11" uniqueName="Item_Multiplier" name="Item_Multiplier" dataDxfId="84">
       <xmlColumnPr mapId="60" xpath="/Rooms/Room/Item_Multiplier" xmlDataType="double"/>
     </tableColumn>
-    <tableColumn id="17" uniqueName="none" name="none" dataDxfId="85">
+    <tableColumn id="17" uniqueName="none" name="none" dataDxfId="83">
       <xmlColumnPr mapId="60" xpath="/Rooms/Room/Find_Probabilities/none" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="12" uniqueName="weak" name="weak" dataDxfId="84">
+    <tableColumn id="12" uniqueName="weak" name="weak" dataDxfId="82">
       <xmlColumnPr mapId="60" xpath="/Rooms/Room/Find_Probabilities/weak" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="13" uniqueName="medium" name="medium" dataDxfId="83">
+    <tableColumn id="13" uniqueName="medium" name="medium" dataDxfId="81">
       <xmlColumnPr mapId="60" xpath="/Rooms/Room/Find_Probabilities/medium" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="14" uniqueName="strong" name="strong" dataDxfId="82">
+    <tableColumn id="14" uniqueName="strong" name="strong" dataDxfId="80">
       <xmlColumnPr mapId="60" xpath="/Rooms/Room/Find_Probabilities/strong" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="15" uniqueName="Item_Count" name="Item_Count" dataDxfId="81">
+    <tableColumn id="15" uniqueName="Item_Count" name="Item_Count" dataDxfId="79">
       <xmlColumnPr mapId="60" xpath="/Rooms/Room/Item_Count" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="16" uniqueName="Image" name="Image" dataDxfId="80">
+    <tableColumn id="16" uniqueName="Image" name="Image" dataDxfId="78">
       <xmlColumnPr mapId="60" xpath="/Rooms/Room/Image" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
@@ -3951,29 +3777,32 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table8" displayName="Table8" ref="A1:G5" tableType="xml" totalsRowShown="0" headerRowDxfId="79" dataDxfId="77" headerRowBorderDxfId="78" tableBorderDxfId="76" connectionId="16">
-  <autoFilter ref="A1:G5"/>
-  <tableColumns count="7">
-    <tableColumn id="1" uniqueName="Name" name="Name" dataDxfId="75">
-      <xmlColumnPr mapId="63" xpath="/Attacks/Attack/Name" xmlDataType="string"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table8" displayName="Table8" ref="A1:H5" tableType="xml" totalsRowShown="0" headerRowDxfId="77" dataDxfId="75" headerRowBorderDxfId="76" tableBorderDxfId="74" connectionId="18">
+  <autoFilter ref="A1:H5"/>
+  <tableColumns count="8">
+    <tableColumn id="1" uniqueName="Name" name="Name" dataDxfId="2">
+      <xmlColumnPr mapId="68" xpath="/Attacks/Attack/Name" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="6" uniqueName="Stats_Low_Multiplier" name="Stats Low Multiplier" dataDxfId="74">
-      <xmlColumnPr mapId="63" xpath="/Attacks/Attack/Stats_Low_Multiplier" xmlDataType="double"/>
+    <tableColumn id="8" uniqueName="Class_Multiplier" name="Class Multiplier" dataDxfId="0">
+      <xmlColumnPr mapId="68" xpath="/Attacks/Attack/Class_Multiplier" xmlDataType="double"/>
+    </tableColumn>
+    <tableColumn id="6" uniqueName="Stats_Low_Multiplier" name="Stats Low Multiplier" dataDxfId="1">
+      <xmlColumnPr mapId="68" xpath="/Attacks/Attack/Stats_Low_Multiplier" xmlDataType="double"/>
     </tableColumn>
     <tableColumn id="7" uniqueName="Stats_High_Multiplier" name="Stats High Multiplier" dataDxfId="73">
-      <xmlColumnPr mapId="63" xpath="/Attacks/Attack/Stats_High_Multiplier" xmlDataType="double"/>
+      <xmlColumnPr mapId="68" xpath="/Attacks/Attack/Stats_High_Multiplier" xmlDataType="double"/>
     </tableColumn>
     <tableColumn id="2" uniqueName="HP_Damage" name="HP Damage" dataDxfId="72">
-      <xmlColumnPr mapId="63" xpath="/Attacks/Attack/HP_Damage" xmlDataType="double"/>
+      <xmlColumnPr mapId="68" xpath="/Attacks/Attack/HP_Damage" xmlDataType="double"/>
     </tableColumn>
     <tableColumn id="3" uniqueName="Hit_Probability" name="Hit Probability" dataDxfId="71">
-      <xmlColumnPr mapId="63" xpath="/Attacks/Attack/Hit_Probability" xmlDataType="double"/>
+      <xmlColumnPr mapId="68" xpath="/Attacks/Attack/Hit_Probability" xmlDataType="double"/>
     </tableColumn>
     <tableColumn id="4" uniqueName="Effect" name="Effect" dataDxfId="70">
-      <xmlColumnPr mapId="63" xpath="/Attacks/Attack/Effect" xmlDataType="string"/>
+      <xmlColumnPr mapId="68" xpath="/Attacks/Attack/Effect" xmlDataType="string"/>
     </tableColumn>
     <tableColumn id="5" uniqueName="x" name="x" dataDxfId="69">
-      <xmlColumnPr mapId="63" xpath="/Attacks/Attack/x" xmlDataType="double"/>
+      <xmlColumnPr mapId="68" xpath="/Attacks/Attack/x" xmlDataType="double"/>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -3981,47 +3810,47 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="A1:M13" tableType="xml" totalsRowShown="0" headerRowDxfId="68" dataDxfId="66" headerRowBorderDxfId="67" tableBorderDxfId="65" connectionId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="A1:M13" tableType="xml" totalsRowShown="0" headerRowDxfId="68" dataDxfId="66" headerRowBorderDxfId="67" tableBorderDxfId="65" connectionId="21">
   <autoFilter ref="A1:M13"/>
   <tableColumns count="13">
     <tableColumn id="1" uniqueName="Name" name="Name" dataDxfId="64">
-      <xmlColumnPr mapId="64" xpath="/Monsters/Monster/Name" xmlDataType="string"/>
+      <xmlColumnPr mapId="71" xpath="/Monsters/Monster/Name" xmlDataType="string"/>
     </tableColumn>
     <tableColumn id="2" uniqueName="Level" name="Level" dataDxfId="63">
-      <xmlColumnPr mapId="64" xpath="/Monsters/Monster/Level" xmlDataType="string"/>
+      <xmlColumnPr mapId="71" xpath="/Monsters/Monster/Level" xmlDataType="string"/>
+    </tableColumn>
+    <tableColumn id="14" uniqueName="Class_Multiplier" name="Class Multiplier" dataDxfId="3">
+      <xmlColumnPr mapId="71" xpath="/Monsters/Monster/Class_Multiplier" xmlDataType="double"/>
     </tableColumn>
     <tableColumn id="10" uniqueName="Stats_Low_Multiplier" name="Stats Low Multiplier" dataDxfId="62">
-      <xmlColumnPr mapId="64" xpath="/Monsters/Monster/Stats_Low_Multiplier" xmlDataType="double"/>
+      <xmlColumnPr mapId="71" xpath="/Monsters/Monster/Stats_Low_Multiplier" xmlDataType="double"/>
     </tableColumn>
     <tableColumn id="13" uniqueName="Stats_High_Multiplier" name="Stats High Multiplier" dataDxfId="61">
-      <xmlColumnPr mapId="64" xpath="/Monsters/Monster/Stats_High_Multiplier" xmlDataType="double"/>
+      <xmlColumnPr mapId="71" xpath="/Monsters/Monster/Stats_High_Multiplier" xmlDataType="double"/>
     </tableColumn>
     <tableColumn id="3" uniqueName="HP" name="HP" dataDxfId="60">
-      <xmlColumnPr mapId="64" xpath="/Monsters/Monster/HP" xmlDataType="integer"/>
+      <xmlColumnPr mapId="71" xpath="/Monsters/Monster/HP" xmlDataType="integer"/>
     </tableColumn>
     <tableColumn id="4" uniqueName="Strength" name="Strength" dataDxfId="59">
-      <xmlColumnPr mapId="64" xpath="/Monsters/Monster/Strength" xmlDataType="integer"/>
+      <xmlColumnPr mapId="71" xpath="/Monsters/Monster/Strength" xmlDataType="integer"/>
     </tableColumn>
     <tableColumn id="5" uniqueName="Speed" name="Speed" dataDxfId="58">
-      <xmlColumnPr mapId="64" xpath="/Monsters/Monster/Speed" xmlDataType="integer"/>
+      <xmlColumnPr mapId="71" xpath="/Monsters/Monster/Speed" xmlDataType="integer"/>
     </tableColumn>
     <tableColumn id="6" uniqueName="Accuracy" name="Accuracy" dataDxfId="57">
-      <xmlColumnPr mapId="64" xpath="/Monsters/Monster/Accuracy" xmlDataType="integer"/>
+      <xmlColumnPr mapId="71" xpath="/Monsters/Monster/Accuracy" xmlDataType="integer"/>
     </tableColumn>
     <tableColumn id="7" uniqueName="Kill_Bonus_Type" name="Kill Bonus Type" dataDxfId="56">
-      <xmlColumnPr mapId="64" xpath="/Monsters/Monster/Kill_Bonus_Type" xmlDataType="string"/>
+      <xmlColumnPr mapId="71" xpath="/Monsters/Monster/Kill_Bonus_Type" xmlDataType="string"/>
     </tableColumn>
     <tableColumn id="8" uniqueName="Kill_Bonus_Low" name="Kill Bonus Low" dataDxfId="55">
-      <xmlColumnPr mapId="64" xpath="/Monsters/Monster/Kill_Bonus_Low" xmlDataType="integer"/>
+      <xmlColumnPr mapId="71" xpath="/Monsters/Monster/Kill_Bonus_Low" xmlDataType="integer"/>
     </tableColumn>
     <tableColumn id="9" uniqueName="Kill_Bonus_High" name="Kill Bonus High" dataDxfId="54">
-      <xmlColumnPr mapId="64" xpath="/Monsters/Monster/Kill_Bonus_High" xmlDataType="integer"/>
+      <xmlColumnPr mapId="71" xpath="/Monsters/Monster/Kill_Bonus_High" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="11" uniqueName="Image_Big" name="Image Big" dataDxfId="53">
-      <xmlColumnPr mapId="64" xpath="/Monsters/Monster/Image_Big" xmlDataType="string"/>
-    </tableColumn>
-    <tableColumn id="12" uniqueName="Image_Small" name="Image Small" dataDxfId="52">
-      <xmlColumnPr mapId="64" xpath="/Monsters/Monster/Image_Small" xmlDataType="string"/>
+    <tableColumn id="11" uniqueName="Image" name="Image" dataDxfId="53">
+      <xmlColumnPr mapId="71" xpath="/Monsters/Monster/Image" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -4029,41 +3858,38 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:K16" tableType="xml" totalsRowShown="0" headerRowDxfId="51" dataDxfId="49" headerRowBorderDxfId="50" tableBorderDxfId="48" totalsRowBorderDxfId="47" connectionId="10">
-  <autoFilter ref="A1:K16"/>
-  <tableColumns count="11">
-    <tableColumn id="1" uniqueName="Name" name="Name" dataDxfId="46">
-      <xmlColumnPr mapId="62" xpath="/Armaments/Armament/Name" xmlDataType="string"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:J16" tableType="xml" totalsRowShown="0" headerRowDxfId="52" dataDxfId="50" headerRowBorderDxfId="51" tableBorderDxfId="49" totalsRowBorderDxfId="48" connectionId="3">
+  <autoFilter ref="A1:J16"/>
+  <tableColumns count="10">
+    <tableColumn id="1" uniqueName="Name" name="Name" dataDxfId="47">
+      <xmlColumnPr mapId="74" xpath="/Armaments/Armament/Name" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="9" uniqueName="Item_Class" name="Item Class" dataDxfId="45">
-      <xmlColumnPr mapId="62" xpath="/Armaments/Armament/Item_Class" xmlDataType="string"/>
+    <tableColumn id="9" uniqueName="Item_Class" name="Item Class" dataDxfId="46">
+      <xmlColumnPr mapId="74" xpath="/Armaments/Armament/Item_Class" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="10" uniqueName="Class_Multiplier" name="Class Multiplier" dataDxfId="44">
-      <xmlColumnPr mapId="62" xpath="/Armaments/Armament/Class_Multiplier" xmlDataType="double"/>
+    <tableColumn id="10" uniqueName="Class_Multiplier" name="Class Multiplier" dataDxfId="45">
+      <xmlColumnPr mapId="74" xpath="/Armaments/Armament/Class_Multiplier" xmlDataType="double"/>
     </tableColumn>
-    <tableColumn id="6" uniqueName="Stats_Low_Multiplier" name="Stats Low Multiplier" dataDxfId="43">
-      <xmlColumnPr mapId="62" xpath="/Armaments/Armament/Stats_Low_Multiplier" xmlDataType="double"/>
+    <tableColumn id="6" uniqueName="Stats_Low_Multiplier" name="Stats Low Multiplier" dataDxfId="44">
+      <xmlColumnPr mapId="74" xpath="/Armaments/Armament/Stats_Low_Multiplier" xmlDataType="double"/>
     </tableColumn>
-    <tableColumn id="11" uniqueName="Stats_High_Multiplier" name="Stats High Multiplier" dataDxfId="42">
-      <xmlColumnPr mapId="62" xpath="/Armaments/Armament/Stats_High_Multiplier" xmlDataType="double"/>
+    <tableColumn id="11" uniqueName="Stats_High_Multiplier" name="Stats High Multiplier" dataDxfId="43">
+      <xmlColumnPr mapId="74" xpath="/Armaments/Armament/Stats_High_Multiplier" xmlDataType="double"/>
     </tableColumn>
-    <tableColumn id="2" uniqueName="Armor" name="Armor" dataDxfId="41">
-      <xmlColumnPr mapId="62" xpath="/Armaments/Armament/Armor" xmlDataType="integer"/>
+    <tableColumn id="2" uniqueName="Armor" name="Armor" dataDxfId="42">
+      <xmlColumnPr mapId="74" xpath="/Armaments/Armament/Armor" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="3" uniqueName="Speed" name="Speed" dataDxfId="40">
-      <xmlColumnPr mapId="62" xpath="/Armaments/Armament/Speed" xmlDataType="integer"/>
+    <tableColumn id="3" uniqueName="Speed" name="Speed" dataDxfId="41">
+      <xmlColumnPr mapId="74" xpath="/Armaments/Armament/Speed" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="4" uniqueName="Type" name="Type" dataDxfId="39">
-      <xmlColumnPr mapId="62" xpath="/Armaments/Armament/Type" xmlDataType="string"/>
+    <tableColumn id="4" uniqueName="Type" name="Type" dataDxfId="40">
+      <xmlColumnPr mapId="74" xpath="/Armaments/Armament/Type" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="5" uniqueName="Bonus" name="Bonus" dataDxfId="38">
-      <xmlColumnPr mapId="62" xpath="/Armaments/Armament/Bonus" xmlDataType="double"/>
+    <tableColumn id="5" uniqueName="Bonus" name="Bonus" dataDxfId="39">
+      <xmlColumnPr mapId="74" xpath="/Armaments/Armament/Bonus" xmlDataType="double"/>
     </tableColumn>
-    <tableColumn id="7" uniqueName="Image_Big" name="Image Big" dataDxfId="37">
-      <xmlColumnPr mapId="62" xpath="/Armaments/Armament/Image_Big" xmlDataType="string"/>
-    </tableColumn>
-    <tableColumn id="8" uniqueName="Image_Small" name="Image Small" dataDxfId="36">
-      <xmlColumnPr mapId="62" xpath="/Armaments/Armament/Image_Small" xmlDataType="string"/>
+    <tableColumn id="7" uniqueName="Image" name="Image" dataDxfId="38">
+      <xmlColumnPr mapId="74" xpath="/Armaments/Armament/Image" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -4071,47 +3897,44 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:M11" tableType="xml" totalsRowShown="0" headerRowDxfId="35" dataDxfId="33" headerRowBorderDxfId="34" tableBorderDxfId="32" totalsRowBorderDxfId="31" connectionId="35">
-  <autoFilter ref="A1:M11"/>
-  <tableColumns count="13">
-    <tableColumn id="1" uniqueName="Name" name="Name" dataDxfId="30">
-      <xmlColumnPr mapId="65" xpath="/Potions/Potion/Name" xmlDataType="string"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:L11" tableType="xml" totalsRowShown="0" headerRowDxfId="37" dataDxfId="35" headerRowBorderDxfId="36" tableBorderDxfId="34" totalsRowBorderDxfId="33" connectionId="32">
+  <autoFilter ref="A1:L11"/>
+  <tableColumns count="12">
+    <tableColumn id="1" uniqueName="Name" name="Name" dataDxfId="32">
+      <xmlColumnPr mapId="75" xpath="/Potions/Potion/Name" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="10" uniqueName="Item_Class" name="Item Class" dataDxfId="29">
-      <xmlColumnPr mapId="65" xpath="/Potions/Potion/Item_Class" xmlDataType="string"/>
+    <tableColumn id="10" uniqueName="Item_Class" name="Item Class" dataDxfId="31">
+      <xmlColumnPr mapId="75" xpath="/Potions/Potion/Item_Class" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="11" uniqueName="Class_Multiplier" name="Class Multiplier" dataDxfId="28">
-      <xmlColumnPr mapId="65" xpath="/Potions/Potion/Class_Multiplier" xmlDataType="double"/>
+    <tableColumn id="11" uniqueName="Class_Multiplier" name="Class Multiplier" dataDxfId="30">
+      <xmlColumnPr mapId="75" xpath="/Potions/Potion/Class_Multiplier" xmlDataType="double"/>
     </tableColumn>
-    <tableColumn id="12" uniqueName="Stats_Low_Multiplier" name="Stats Low Multiplier" dataDxfId="27">
-      <xmlColumnPr mapId="65" xpath="/Potions/Potion/Stats_Low_Multiplier" xmlDataType="double"/>
+    <tableColumn id="12" uniqueName="Stats_Low_Multiplier" name="Stats Low Multiplier" dataDxfId="29">
+      <xmlColumnPr mapId="75" xpath="/Potions/Potion/Stats_Low_Multiplier" xmlDataType="double"/>
     </tableColumn>
-    <tableColumn id="13" uniqueName="Stats_High_Multiplier" name="Stats High Multiplier" dataDxfId="26">
-      <xmlColumnPr mapId="65" xpath="/Potions/Potion/Stats_High_Multiplier" xmlDataType="double"/>
+    <tableColumn id="13" uniqueName="Stats_High_Multiplier" name="Stats High Multiplier" dataDxfId="28">
+      <xmlColumnPr mapId="75" xpath="/Potions/Potion/Stats_High_Multiplier" xmlDataType="double"/>
     </tableColumn>
-    <tableColumn id="2" uniqueName="Description" name="Description" dataDxfId="25">
-      <xmlColumnPr mapId="65" xpath="/Potions/Potion/Description" xmlDataType="string"/>
+    <tableColumn id="2" uniqueName="Description" name="Description" dataDxfId="27">
+      <xmlColumnPr mapId="75" xpath="/Potions/Potion/Description" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="3" uniqueName="Target" name="Target" dataDxfId="24">
-      <xmlColumnPr mapId="65" xpath="/Potions/Potion/Target" xmlDataType="string"/>
+    <tableColumn id="3" uniqueName="Target" name="Target" dataDxfId="26">
+      <xmlColumnPr mapId="75" xpath="/Potions/Potion/Target" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="4" uniqueName="Effect" name="Effect" dataDxfId="23">
-      <xmlColumnPr mapId="65" xpath="/Potions/Potion/Effect" xmlDataType="string"/>
+    <tableColumn id="4" uniqueName="Effect" name="Effect" dataDxfId="25">
+      <xmlColumnPr mapId="75" xpath="/Potions/Potion/Effect" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="5" uniqueName="Mode" name="Mode" dataDxfId="22">
-      <xmlColumnPr mapId="65" xpath="/Potions/Potion/Mode" xmlDataType="string"/>
+    <tableColumn id="5" uniqueName="Mode" name="Mode" dataDxfId="24">
+      <xmlColumnPr mapId="75" xpath="/Potions/Potion/Mode" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="6" uniqueName="x" name="x" dataDxfId="21">
-      <xmlColumnPr mapId="65" xpath="/Potions/Potion/x" xmlDataType="integer"/>
+    <tableColumn id="6" uniqueName="x" name="x" dataDxfId="23">
+      <xmlColumnPr mapId="75" xpath="/Potions/Potion/x" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="7" uniqueName="n" name="n" dataDxfId="20">
-      <xmlColumnPr mapId="65" xpath="/Potions/Potion/n" xmlDataType="integer"/>
+    <tableColumn id="7" uniqueName="n" name="n" dataDxfId="22">
+      <xmlColumnPr mapId="75" xpath="/Potions/Potion/n" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="8" uniqueName="Image_Big" name="Image Big" dataDxfId="19">
-      <xmlColumnPr mapId="65" xpath="/Potions/Potion/Image_Big" xmlDataType="string"/>
-    </tableColumn>
-    <tableColumn id="9" uniqueName="Image_Small" name="Image Small" dataDxfId="18">
-      <xmlColumnPr mapId="65" xpath="/Potions/Potion/Image_Small" xmlDataType="string"/>
+    <tableColumn id="8" uniqueName="Image" name="Image" dataDxfId="21">
+      <xmlColumnPr mapId="75" xpath="/Potions/Potion/Image" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -4119,51 +3942,48 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:N9" tableType="xml" totalsRowShown="0" headerRowDxfId="17" dataDxfId="15" headerRowBorderDxfId="16" tableBorderDxfId="14" connectionId="50">
-  <autoFilter ref="A1:N9"/>
-  <tableColumns count="14">
-    <tableColumn id="1" uniqueName="Name" name="Name" dataDxfId="13">
-      <xmlColumnPr mapId="66" xpath="/Weapons/Weapon/Name" xmlDataType="string"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:M9" tableType="xml" totalsRowShown="0" headerRowDxfId="20" dataDxfId="18" headerRowBorderDxfId="19" tableBorderDxfId="17" connectionId="56">
+  <autoFilter ref="A1:M9"/>
+  <tableColumns count="13">
+    <tableColumn id="1" uniqueName="Name" name="Name" dataDxfId="16">
+      <xmlColumnPr mapId="76" xpath="/Weapons/Weapon/Name" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="11" uniqueName="Item_Class" name="Item Class" dataDxfId="12">
-      <xmlColumnPr mapId="66" xpath="/Weapons/Weapon/Item_Class" xmlDataType="string"/>
+    <tableColumn id="11" uniqueName="Item_Class" name="Item Class" dataDxfId="15">
+      <xmlColumnPr mapId="76" xpath="/Weapons/Weapon/Item_Class" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="12" uniqueName="Class_Multiplier" name="Class Multiplier" dataDxfId="11">
-      <xmlColumnPr mapId="66" xpath="/Weapons/Weapon/Class_Multiplier" xmlDataType="double"/>
+    <tableColumn id="12" uniqueName="Class_Multiplier" name="Class Multiplier" dataDxfId="14">
+      <xmlColumnPr mapId="76" xpath="/Weapons/Weapon/Class_Multiplier" xmlDataType="double"/>
     </tableColumn>
-    <tableColumn id="13" uniqueName="Stats_Low_Multiplier" name="Stats Low Multiplier" dataDxfId="10">
-      <xmlColumnPr mapId="66" xpath="/Weapons/Weapon/Stats_Low_Multiplier" xmlDataType="double"/>
+    <tableColumn id="13" uniqueName="Stats_Low_Multiplier" name="Stats Low Multiplier" dataDxfId="13">
+      <xmlColumnPr mapId="76" xpath="/Weapons/Weapon/Stats_Low_Multiplier" xmlDataType="double"/>
     </tableColumn>
-    <tableColumn id="14" uniqueName="Stats_High_Multiplier" name="Stats High Multiplier" dataDxfId="9">
-      <xmlColumnPr mapId="66" xpath="/Weapons/Weapon/Stats_High_Multiplier" xmlDataType="double"/>
+    <tableColumn id="14" uniqueName="Stats_High_Multiplier" name="Stats High Multiplier" dataDxfId="12">
+      <xmlColumnPr mapId="76" xpath="/Weapons/Weapon/Stats_High_Multiplier" xmlDataType="double"/>
     </tableColumn>
-    <tableColumn id="2" uniqueName="Attack" name="Attack" dataDxfId="8">
-      <xmlColumnPr mapId="66" xpath="/Weapons/Weapon/Attack" xmlDataType="integer"/>
+    <tableColumn id="2" uniqueName="Attack" name="Attack" dataDxfId="11">
+      <xmlColumnPr mapId="76" xpath="/Weapons/Weapon/Attack" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="3" uniqueName="Speed" name="Speed" dataDxfId="7">
-      <xmlColumnPr mapId="66" xpath="/Weapons/Weapon/Speed" xmlDataType="integer"/>
+    <tableColumn id="3" uniqueName="Speed" name="Speed" dataDxfId="10">
+      <xmlColumnPr mapId="76" xpath="/Weapons/Weapon/Speed" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="4" uniqueName="Accuracy" name="Accuracy" dataDxfId="6">
-      <xmlColumnPr mapId="66" xpath="/Weapons/Weapon/Accuracy" xmlDataType="integer"/>
+    <tableColumn id="4" uniqueName="Accuracy" name="Accuracy" dataDxfId="9">
+      <xmlColumnPr mapId="76" xpath="/Weapons/Weapon/Accuracy" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="5" uniqueName="Defence" name="Defence" dataDxfId="5">
+    <tableColumn id="5" uniqueName="Defence" name="Defence" dataDxfId="8">
       <calculatedColumnFormula>"-"</calculatedColumnFormula>
-      <xmlColumnPr mapId="66" xpath="/Weapons/Weapon/Defence" xmlDataType="integer"/>
+      <xmlColumnPr mapId="76" xpath="/Weapons/Weapon/Defence" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="6" uniqueName="Slots" name="Slots" dataDxfId="4">
-      <xmlColumnPr mapId="66" xpath="/Weapons/Weapon/Slots" xmlDataType="integer"/>
+    <tableColumn id="6" uniqueName="Slots" name="Slots" dataDxfId="7">
+      <xmlColumnPr mapId="76" xpath="/Weapons/Weapon/Slots" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="7" uniqueName="Max" name="Max" dataDxfId="3">
-      <xmlColumnPr mapId="66" xpath="/Weapons/Weapon/Max" xmlDataType="integer"/>
+    <tableColumn id="7" uniqueName="Max" name="Max" dataDxfId="6">
+      <xmlColumnPr mapId="76" xpath="/Weapons/Weapon/Max" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="8" uniqueName="Type" name="Type" dataDxfId="2">
-      <xmlColumnPr mapId="66" xpath="/Weapons/Weapon/Type" xmlDataType="string"/>
+    <tableColumn id="8" uniqueName="Type" name="Type" dataDxfId="5">
+      <xmlColumnPr mapId="76" xpath="/Weapons/Weapon/Type" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="9" uniqueName="Image_Big" name="Image Big" dataDxfId="1">
-      <xmlColumnPr mapId="66" xpath="/Weapons/Weapon/Image_Big" xmlDataType="string"/>
-    </tableColumn>
-    <tableColumn id="10" uniqueName="Image_Small" name="Image Small" dataDxfId="0">
-      <xmlColumnPr mapId="66" xpath="/Weapons/Weapon/Image_Small" xmlDataType="string"/>
+    <tableColumn id="9" uniqueName="Image" name="Image" dataDxfId="4">
+      <xmlColumnPr mapId="76" xpath="/Weapons/Weapon/Image" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -4477,7 +4297,7 @@
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>254</v>
+        <v>162</v>
       </c>
     </row>
   </sheetData>
@@ -4489,9 +4309,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="Q13" sqref="Q13"/>
+      <selection pane="topRight" activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4518,21 +4338,21 @@
     <row r="1" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="22"/>
       <c r="B1" s="22"/>
-      <c r="C1" s="77" t="s">
-        <v>125</v>
-      </c>
-      <c r="D1" s="78"/>
-      <c r="E1" s="78"/>
-      <c r="F1" s="79"/>
-      <c r="G1" s="77" t="s">
+      <c r="C1" s="78" t="s">
+        <v>123</v>
+      </c>
+      <c r="D1" s="79"/>
+      <c r="E1" s="79"/>
+      <c r="F1" s="80"/>
+      <c r="G1" s="78" t="s">
         <v>120</v>
       </c>
-      <c r="H1" s="78"/>
-      <c r="I1" s="78"/>
-      <c r="J1" s="79"/>
+      <c r="H1" s="79"/>
+      <c r="I1" s="79"/>
+      <c r="J1" s="80"/>
       <c r="K1" s="29"/>
       <c r="L1" s="81" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="M1" s="82"/>
       <c r="N1" s="82"/>
@@ -4548,16 +4368,16 @@
         <v>39</v>
       </c>
       <c r="C2" s="25" t="s">
+        <v>125</v>
+      </c>
+      <c r="D2" s="25" t="s">
+        <v>124</v>
+      </c>
+      <c r="E2" s="25" t="s">
+        <v>126</v>
+      </c>
+      <c r="F2" s="25" t="s">
         <v>127</v>
-      </c>
-      <c r="D2" s="25" t="s">
-        <v>126</v>
-      </c>
-      <c r="E2" s="25" t="s">
-        <v>128</v>
-      </c>
-      <c r="F2" s="25" t="s">
-        <v>129</v>
       </c>
       <c r="G2" s="25" t="s">
         <v>121</v>
@@ -4572,22 +4392,22 @@
         <v>81</v>
       </c>
       <c r="K2" s="30" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="L2" s="32" t="s">
-        <v>253</v>
+        <v>161</v>
       </c>
       <c r="M2" s="32" t="s">
+        <v>147</v>
+      </c>
+      <c r="N2" s="32" t="s">
+        <v>148</v>
+      </c>
+      <c r="O2" s="32" t="s">
         <v>149</v>
       </c>
-      <c r="N2" s="32" t="s">
-        <v>150</v>
-      </c>
-      <c r="O2" s="32" t="s">
-        <v>151</v>
-      </c>
       <c r="P2" s="37" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="Q2" s="39" t="s">
         <v>122</v>
@@ -4643,7 +4463,7 @@
         <v>3</v>
       </c>
       <c r="Q3" s="21" t="s">
-        <v>255</v>
+        <v>163</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
@@ -4696,7 +4516,7 @@
         <v>2</v>
       </c>
       <c r="Q4" s="21" t="s">
-        <v>255</v>
+        <v>163</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
@@ -4749,7 +4569,7 @@
         <v>2</v>
       </c>
       <c r="Q5" s="21" t="s">
-        <v>255</v>
+        <v>163</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
@@ -4802,7 +4622,7 @@
         <v>1</v>
       </c>
       <c r="Q6" s="21" t="s">
-        <v>255</v>
+        <v>163</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
@@ -4855,7 +4675,7 @@
         <v>1</v>
       </c>
       <c r="Q7" s="21" t="s">
-        <v>255</v>
+        <v>163</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
@@ -4908,37 +4728,37 @@
         <v>5</v>
       </c>
       <c r="Q8" s="21" t="s">
-        <v>255</v>
+        <v>163</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="21" t="s">
-        <v>146</v>
-      </c>
-      <c r="C10" s="80" t="s">
-        <v>131</v>
-      </c>
-      <c r="D10" s="80"/>
-      <c r="E10" s="80"/>
-      <c r="F10" s="80"/>
-      <c r="G10" s="80" t="s">
-        <v>130</v>
-      </c>
-      <c r="H10" s="80"/>
-      <c r="I10" s="80"/>
-      <c r="J10" s="80"/>
+        <v>144</v>
+      </c>
+      <c r="C10" s="77" t="s">
+        <v>129</v>
+      </c>
+      <c r="D10" s="77"/>
+      <c r="E10" s="77"/>
+      <c r="F10" s="77"/>
+      <c r="G10" s="77" t="s">
+        <v>128</v>
+      </c>
+      <c r="H10" s="77"/>
+      <c r="I10" s="77"/>
+      <c r="J10" s="77"/>
       <c r="K10" s="31"/>
       <c r="L10" s="33"/>
-      <c r="M10" s="80" t="s">
-        <v>155</v>
-      </c>
-      <c r="N10" s="80"/>
-      <c r="O10" s="80"/>
+      <c r="M10" s="77" t="s">
+        <v>153</v>
+      </c>
+      <c r="N10" s="77"/>
+      <c r="O10" s="77"/>
       <c r="P10" s="33"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="21" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G11" s="34"/>
       <c r="H11" s="34"/>
@@ -4953,10 +4773,10 @@
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="21" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="G12" s="34" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="H12" s="34"/>
       <c r="I12" s="34"/>
@@ -4964,7 +4784,7 @@
       <c r="K12" s="28"/>
       <c r="L12" s="34"/>
       <c r="M12" s="34" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="N12" s="34"/>
       <c r="O12" s="34"/>
@@ -4972,7 +4792,7 @@
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="21" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="G13" s="34"/>
       <c r="H13" s="34"/>
@@ -4981,19 +4801,19 @@
       <c r="K13" s="28"/>
       <c r="L13" s="34"/>
       <c r="M13" s="34" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="N13" s="34"/>
       <c r="O13" s="34"/>
       <c r="P13" s="34"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="G14" s="80" t="s">
-        <v>132</v>
-      </c>
-      <c r="H14" s="80"/>
-      <c r="I14" s="80"/>
-      <c r="J14" s="80"/>
+      <c r="G14" s="77" t="s">
+        <v>130</v>
+      </c>
+      <c r="H14" s="77"/>
+      <c r="I14" s="77"/>
+      <c r="J14" s="77"/>
       <c r="K14" s="31"/>
       <c r="L14" s="33"/>
       <c r="M14" s="33"/>
@@ -5003,14 +4823,14 @@
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="21" t="s">
-        <v>145</v>
-      </c>
-      <c r="G15" s="80" t="s">
-        <v>133</v>
-      </c>
-      <c r="H15" s="80"/>
-      <c r="I15" s="80"/>
-      <c r="J15" s="80"/>
+        <v>143</v>
+      </c>
+      <c r="G15" s="77" t="s">
+        <v>131</v>
+      </c>
+      <c r="H15" s="77"/>
+      <c r="I15" s="77"/>
+      <c r="J15" s="77"/>
       <c r="K15" s="31"/>
       <c r="L15" s="33"/>
       <c r="M15" s="33"/>
@@ -5019,12 +4839,12 @@
       <c r="P15" s="33"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="G16" s="80" t="s">
-        <v>134</v>
-      </c>
-      <c r="H16" s="80"/>
-      <c r="I16" s="80"/>
-      <c r="J16" s="80"/>
+      <c r="G16" s="77" t="s">
+        <v>132</v>
+      </c>
+      <c r="H16" s="77"/>
+      <c r="I16" s="77"/>
+      <c r="J16" s="77"/>
       <c r="K16" s="31"/>
       <c r="L16" s="33"/>
       <c r="M16" s="33"/>
@@ -5033,12 +4853,12 @@
       <c r="P16" s="33"/>
     </row>
     <row r="17" spans="7:16" x14ac:dyDescent="0.25">
-      <c r="G17" s="80" t="s">
-        <v>135</v>
-      </c>
-      <c r="H17" s="80"/>
-      <c r="I17" s="80"/>
-      <c r="J17" s="80"/>
+      <c r="G17" s="77" t="s">
+        <v>133</v>
+      </c>
+      <c r="H17" s="77"/>
+      <c r="I17" s="77"/>
+      <c r="J17" s="77"/>
       <c r="K17" s="31"/>
       <c r="L17" s="33"/>
       <c r="M17" s="33"/>
@@ -5047,12 +4867,12 @@
       <c r="P17" s="33"/>
     </row>
     <row r="18" spans="7:16" x14ac:dyDescent="0.25">
-      <c r="G18" s="80" t="s">
-        <v>136</v>
-      </c>
-      <c r="H18" s="80"/>
-      <c r="I18" s="80"/>
-      <c r="J18" s="80"/>
+      <c r="G18" s="77" t="s">
+        <v>134</v>
+      </c>
+      <c r="H18" s="77"/>
+      <c r="I18" s="77"/>
+      <c r="J18" s="77"/>
       <c r="K18" s="31"/>
       <c r="L18" s="33"/>
       <c r="M18" s="33"/>
@@ -5061,12 +4881,12 @@
       <c r="P18" s="33"/>
     </row>
     <row r="20" spans="7:16" x14ac:dyDescent="0.25">
-      <c r="G20" s="80" t="s">
-        <v>137</v>
-      </c>
-      <c r="H20" s="80"/>
-      <c r="I20" s="80"/>
-      <c r="J20" s="80"/>
+      <c r="G20" s="77" t="s">
+        <v>135</v>
+      </c>
+      <c r="H20" s="77"/>
+      <c r="I20" s="77"/>
+      <c r="J20" s="77"/>
       <c r="K20" s="31"/>
       <c r="L20" s="33"/>
       <c r="M20" s="33"/>
@@ -5075,12 +4895,12 @@
       <c r="P20" s="33"/>
     </row>
     <row r="21" spans="7:16" x14ac:dyDescent="0.25">
-      <c r="G21" s="80" t="s">
-        <v>138</v>
-      </c>
-      <c r="H21" s="80"/>
-      <c r="I21" s="80"/>
-      <c r="J21" s="80"/>
+      <c r="G21" s="77" t="s">
+        <v>136</v>
+      </c>
+      <c r="H21" s="77"/>
+      <c r="I21" s="77"/>
+      <c r="J21" s="77"/>
       <c r="K21" s="31"/>
       <c r="L21" s="33"/>
       <c r="M21" s="33"/>
@@ -5090,16 +4910,16 @@
     </row>
     <row r="23" spans="7:16" x14ac:dyDescent="0.25">
       <c r="G23" s="26" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="24" spans="7:16" x14ac:dyDescent="0.25">
-      <c r="G24" s="80" t="s">
-        <v>139</v>
-      </c>
-      <c r="H24" s="80"/>
-      <c r="I24" s="80"/>
-      <c r="J24" s="80"/>
+      <c r="G24" s="77" t="s">
+        <v>137</v>
+      </c>
+      <c r="H24" s="77"/>
+      <c r="I24" s="77"/>
+      <c r="J24" s="77"/>
       <c r="K24" s="31"/>
       <c r="L24" s="33"/>
       <c r="M24" s="33"/>
@@ -5108,12 +4928,12 @@
       <c r="P24" s="33"/>
     </row>
     <row r="25" spans="7:16" x14ac:dyDescent="0.25">
-      <c r="G25" s="80" t="s">
-        <v>140</v>
-      </c>
-      <c r="H25" s="80"/>
-      <c r="I25" s="80"/>
-      <c r="J25" s="80"/>
+      <c r="G25" s="77" t="s">
+        <v>138</v>
+      </c>
+      <c r="H25" s="77"/>
+      <c r="I25" s="77"/>
+      <c r="J25" s="77"/>
       <c r="K25" s="31"/>
       <c r="L25" s="33"/>
       <c r="M25" s="33"/>
@@ -5122,12 +4942,12 @@
       <c r="P25" s="33"/>
     </row>
     <row r="26" spans="7:16" x14ac:dyDescent="0.25">
-      <c r="G26" s="80" t="s">
-        <v>142</v>
-      </c>
-      <c r="H26" s="80"/>
-      <c r="I26" s="80"/>
-      <c r="J26" s="80"/>
+      <c r="G26" s="77" t="s">
+        <v>140</v>
+      </c>
+      <c r="H26" s="77"/>
+      <c r="I26" s="77"/>
+      <c r="J26" s="77"/>
       <c r="K26" s="31"/>
       <c r="L26" s="33"/>
       <c r="M26" s="33"/>
@@ -5137,6 +4957,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="G1:J1"/>
+    <mergeCell ref="M10:O10"/>
+    <mergeCell ref="G25:J25"/>
+    <mergeCell ref="L1:O1"/>
     <mergeCell ref="G26:J26"/>
     <mergeCell ref="C10:F10"/>
     <mergeCell ref="G10:J10"/>
@@ -5148,11 +4973,6 @@
     <mergeCell ref="G17:J17"/>
     <mergeCell ref="G18:J18"/>
     <mergeCell ref="G21:J21"/>
-    <mergeCell ref="C1:F1"/>
-    <mergeCell ref="G1:J1"/>
-    <mergeCell ref="M10:O10"/>
-    <mergeCell ref="G25:J25"/>
-    <mergeCell ref="L1:O1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5164,140 +4984,156 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="K18" sqref="K18"/>
+      <selection pane="topRight" activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="21" customWidth="1"/>
-    <col min="2" max="2" width="23.7109375" style="27" customWidth="1"/>
-    <col min="3" max="3" width="24.28515625" style="27" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" style="27" customWidth="1"/>
-    <col min="5" max="5" width="18" style="27" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" style="21" customWidth="1"/>
-    <col min="7" max="7" width="5.85546875" style="27" customWidth="1"/>
+    <col min="2" max="2" width="20" style="27" customWidth="1"/>
+    <col min="3" max="3" width="23.7109375" style="27" customWidth="1"/>
+    <col min="4" max="4" width="24.28515625" style="27" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" style="27" customWidth="1"/>
+    <col min="6" max="6" width="18" style="27" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" style="21" customWidth="1"/>
+    <col min="8" max="8" width="5.85546875" style="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="40" t="s">
         <v>40</v>
       </c>
       <c r="B1" s="42" t="s">
-        <v>250</v>
+        <v>150</v>
       </c>
       <c r="C1" s="42" t="s">
-        <v>251</v>
-      </c>
-      <c r="D1" s="43" t="s">
+        <v>158</v>
+      </c>
+      <c r="D1" s="42" t="s">
+        <v>159</v>
+      </c>
+      <c r="E1" s="43" t="s">
         <v>104</v>
       </c>
-      <c r="E1" s="43" t="s">
+      <c r="F1" s="43" t="s">
         <v>105</v>
       </c>
-      <c r="F1" s="48" t="s">
+      <c r="G1" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="47" t="s">
+      <c r="H1" s="47" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>100</v>
       </c>
       <c r="B2" s="44">
+        <v>1</v>
+      </c>
+      <c r="C2" s="44">
         <v>0.8</v>
       </c>
-      <c r="C2" s="44">
+      <c r="D2" s="44">
         <v>1.2</v>
       </c>
-      <c r="D2" s="44">
+      <c r="E2" s="44">
         <v>0.5</v>
       </c>
-      <c r="E2" s="44">
+      <c r="F2" s="44">
         <v>0.8</v>
       </c>
-      <c r="F2" s="16" t="s">
+      <c r="G2" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="44">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2" s="44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>101</v>
       </c>
       <c r="B3" s="44">
+        <v>1</v>
+      </c>
+      <c r="C3" s="44">
         <v>0.8</v>
       </c>
-      <c r="C3" s="45">
+      <c r="D3" s="45">
         <v>1.2</v>
       </c>
-      <c r="D3" s="45">
+      <c r="E3" s="45">
         <v>0.7</v>
       </c>
-      <c r="E3" s="45">
+      <c r="F3" s="45">
         <v>0.3</v>
       </c>
-      <c r="F3" s="14" t="s">
+      <c r="G3" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="45">
+      <c r="H3" s="45">
         <v>0.8</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>102</v>
       </c>
       <c r="B4" s="44">
+        <v>1</v>
+      </c>
+      <c r="C4" s="44">
         <v>0.8</v>
       </c>
-      <c r="C4" s="44">
+      <c r="D4" s="44">
         <v>1.2</v>
       </c>
-      <c r="D4" s="45">
+      <c r="E4" s="45">
         <v>0.3</v>
       </c>
-      <c r="E4" s="45">
+      <c r="F4" s="45">
         <v>0.7</v>
       </c>
-      <c r="F4" s="14" t="s">
+      <c r="G4" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="45">
+      <c r="H4" s="45">
         <v>0.8</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>103</v>
       </c>
-      <c r="B5" s="44">
+      <c r="B5" s="85">
+        <v>1</v>
+      </c>
+      <c r="C5" s="44">
         <v>0.8</v>
       </c>
-      <c r="C5" s="45">
+      <c r="D5" s="45">
         <v>1.2</v>
       </c>
-      <c r="D5" s="46">
+      <c r="E5" s="46">
         <v>0.4</v>
       </c>
-      <c r="E5" s="46">
+      <c r="F5" s="46">
         <v>0.6</v>
       </c>
-      <c r="F5" s="15" t="s">
+      <c r="G5" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="46">
+      <c r="H5" s="46">
         <v>0.8</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="41" t="s">
         <v>106</v>
       </c>
@@ -5305,15 +5141,17 @@
       <c r="C7" s="28"/>
       <c r="D7" s="28"/>
       <c r="E7" s="28"/>
-      <c r="F7" s="49"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F7" s="28"/>
+      <c r="G7" s="49"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="41" t="s">
         <v>107</v>
       </c>
       <c r="B8" s="28"/>
       <c r="C8" s="28"/>
       <c r="D8" s="28"/>
+      <c r="E8" s="28"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5330,24 +5168,24 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="J6" sqref="J6"/>
+      <selection pane="topRight" activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.28515625" style="21" customWidth="1"/>
     <col min="2" max="2" width="19.5703125" style="21" customWidth="1"/>
-    <col min="3" max="3" width="23.85546875" style="27" customWidth="1"/>
-    <col min="4" max="4" width="24.140625" style="27" customWidth="1"/>
-    <col min="5" max="5" width="5.7109375" style="26" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" style="26" customWidth="1"/>
-    <col min="7" max="7" width="7.85546875" style="26" customWidth="1"/>
-    <col min="8" max="8" width="11.42578125" style="26" customWidth="1"/>
-    <col min="9" max="9" width="17.42578125" style="21" customWidth="1"/>
-    <col min="10" max="10" width="16" style="26" customWidth="1"/>
-    <col min="11" max="11" width="16.42578125" style="26" customWidth="1"/>
-    <col min="12" max="12" width="64" style="21" customWidth="1"/>
-    <col min="13" max="13" width="46.85546875" style="21" customWidth="1"/>
+    <col min="3" max="3" width="17.140625" style="27" customWidth="1"/>
+    <col min="4" max="4" width="23.85546875" style="27" customWidth="1"/>
+    <col min="5" max="5" width="24.140625" style="27" customWidth="1"/>
+    <col min="6" max="6" width="5.7109375" style="26" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" style="26" customWidth="1"/>
+    <col min="8" max="8" width="7.85546875" style="26" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="26" customWidth="1"/>
+    <col min="10" max="10" width="17.42578125" style="21" customWidth="1"/>
+    <col min="11" max="11" width="16" style="26" customWidth="1"/>
+    <col min="12" max="12" width="16.42578125" style="26" customWidth="1"/>
+    <col min="13" max="13" width="34" style="21" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5358,37 +5196,37 @@
         <v>96</v>
       </c>
       <c r="C1" s="54" t="s">
-        <v>250</v>
+        <v>150</v>
       </c>
       <c r="D1" s="54" t="s">
-        <v>251</v>
-      </c>
-      <c r="E1" s="57" t="s">
+        <v>158</v>
+      </c>
+      <c r="E1" s="54" t="s">
+        <v>159</v>
+      </c>
+      <c r="F1" s="57" t="s">
         <v>78</v>
       </c>
-      <c r="F1" s="57" t="s">
+      <c r="G1" s="57" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="57" t="s">
+      <c r="H1" s="57" t="s">
         <v>23</v>
       </c>
-      <c r="H1" s="57" t="s">
+      <c r="I1" s="57" t="s">
         <v>24</v>
       </c>
-      <c r="I1" s="53" t="s">
+      <c r="J1" s="53" t="s">
         <v>99</v>
       </c>
-      <c r="J1" s="61" t="s">
+      <c r="K1" s="61" t="s">
         <v>97</v>
       </c>
-      <c r="K1" s="61" t="s">
+      <c r="L1" s="61" t="s">
         <v>98</v>
       </c>
-      <c r="L1" s="50" t="s">
-        <v>123</v>
-      </c>
       <c r="M1" s="50" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5399,37 +5237,37 @@
         <v>79</v>
       </c>
       <c r="C2" s="55">
+        <v>1</v>
+      </c>
+      <c r="D2" s="55">
         <v>0.8</v>
       </c>
-      <c r="D2" s="55">
+      <c r="E2" s="55">
         <v>1.2</v>
       </c>
-      <c r="E2" s="58">
+      <c r="F2" s="58">
         <v>20</v>
       </c>
-      <c r="F2" s="58">
+      <c r="G2" s="58">
         <v>25</v>
       </c>
-      <c r="G2" s="58">
+      <c r="H2" s="58">
         <v>70</v>
       </c>
-      <c r="H2" s="58">
+      <c r="I2" s="58">
         <v>45</v>
       </c>
-      <c r="I2" s="10" t="s">
+      <c r="J2" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="58">
+      <c r="K2" s="58">
         <v>2</v>
       </c>
-      <c r="K2" s="62">
+      <c r="L2" s="62">
         <v>4</v>
       </c>
-      <c r="L2" s="3" t="s">
-        <v>160</v>
-      </c>
       <c r="M2" s="3" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5440,37 +5278,37 @@
         <v>79</v>
       </c>
       <c r="C3" s="55">
+        <v>1</v>
+      </c>
+      <c r="D3" s="55">
         <v>0.8</v>
       </c>
-      <c r="D3" s="55">
+      <c r="E3" s="55">
         <v>1.2</v>
       </c>
-      <c r="E3" s="59">
+      <c r="F3" s="59">
         <v>25</v>
       </c>
-      <c r="F3" s="59">
+      <c r="G3" s="59">
         <v>20</v>
-      </c>
-      <c r="G3" s="59">
-        <v>60</v>
       </c>
       <c r="H3" s="59">
         <v>60</v>
       </c>
-      <c r="I3" s="11" t="s">
+      <c r="I3" s="59">
+        <v>60</v>
+      </c>
+      <c r="J3" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="J3" s="59">
-        <v>1</v>
-      </c>
       <c r="K3" s="59">
+        <v>1</v>
+      </c>
+      <c r="L3" s="59">
         <v>2</v>
       </c>
-      <c r="L3" s="3" t="s">
-        <v>161</v>
-      </c>
       <c r="M3" s="3" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5481,37 +5319,37 @@
         <v>79</v>
       </c>
       <c r="C4" s="55">
+        <v>1</v>
+      </c>
+      <c r="D4" s="55">
         <v>0.8</v>
       </c>
-      <c r="D4" s="55">
+      <c r="E4" s="55">
         <v>1.2</v>
       </c>
-      <c r="E4" s="59">
+      <c r="F4" s="59">
         <v>15</v>
       </c>
-      <c r="F4" s="59">
+      <c r="G4" s="59">
         <v>10</v>
       </c>
-      <c r="G4" s="59">
+      <c r="H4" s="59">
         <v>65</v>
       </c>
-      <c r="H4" s="59">
+      <c r="I4" s="59">
         <v>55</v>
       </c>
-      <c r="I4" s="11" t="s">
+      <c r="J4" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="J4" s="59">
-        <v>1</v>
-      </c>
       <c r="K4" s="59">
+        <v>1</v>
+      </c>
+      <c r="L4" s="59">
         <v>2</v>
       </c>
-      <c r="L4" s="3" t="s">
-        <v>162</v>
-      </c>
       <c r="M4" s="3" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5522,37 +5360,37 @@
         <v>79</v>
       </c>
       <c r="C5" s="55">
+        <v>1</v>
+      </c>
+      <c r="D5" s="55">
         <v>0.8</v>
       </c>
-      <c r="D5" s="55">
+      <c r="E5" s="55">
         <v>1.2</v>
       </c>
-      <c r="E5" s="59">
+      <c r="F5" s="59">
         <v>25</v>
       </c>
-      <c r="F5" s="59">
+      <c r="G5" s="59">
         <v>15</v>
       </c>
-      <c r="G5" s="59">
+      <c r="H5" s="59">
         <v>80</v>
       </c>
-      <c r="H5" s="59">
+      <c r="I5" s="59">
         <v>50</v>
       </c>
-      <c r="I5" s="11" t="s">
+      <c r="J5" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="J5" s="59">
-        <v>1</v>
-      </c>
       <c r="K5" s="59">
+        <v>1</v>
+      </c>
+      <c r="L5" s="59">
         <v>2</v>
       </c>
-      <c r="L5" s="3" t="s">
-        <v>163</v>
-      </c>
       <c r="M5" s="3" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5563,37 +5401,37 @@
         <v>79</v>
       </c>
       <c r="C6" s="55">
+        <v>1</v>
+      </c>
+      <c r="D6" s="55">
         <v>0.8</v>
       </c>
-      <c r="D6" s="55">
+      <c r="E6" s="55">
         <v>1.2</v>
       </c>
-      <c r="E6" s="59">
+      <c r="F6" s="59">
         <v>15</v>
       </c>
-      <c r="F6" s="59">
+      <c r="G6" s="59">
         <v>20</v>
       </c>
-      <c r="G6" s="59">
+      <c r="H6" s="59">
         <v>75</v>
       </c>
-      <c r="H6" s="59">
+      <c r="I6" s="59">
         <v>55</v>
       </c>
-      <c r="I6" s="11" t="s">
+      <c r="J6" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="J6" s="59">
-        <v>1</v>
-      </c>
       <c r="K6" s="59">
+        <v>1</v>
+      </c>
+      <c r="L6" s="59">
         <v>2</v>
       </c>
-      <c r="L6" s="3" t="s">
-        <v>164</v>
-      </c>
       <c r="M6" s="3" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5604,37 +5442,37 @@
         <v>80</v>
       </c>
       <c r="C7" s="55">
+        <v>1</v>
+      </c>
+      <c r="D7" s="55">
         <v>0.8</v>
       </c>
-      <c r="D7" s="55">
+      <c r="E7" s="55">
         <v>1.2</v>
-      </c>
-      <c r="E7" s="59">
-        <v>35</v>
       </c>
       <c r="F7" s="59">
         <v>35</v>
       </c>
       <c r="G7" s="59">
+        <v>35</v>
+      </c>
+      <c r="H7" s="59">
         <v>55</v>
       </c>
-      <c r="H7" s="59">
+      <c r="I7" s="59">
         <v>60</v>
       </c>
-      <c r="I7" s="11" t="s">
+      <c r="J7" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="J7" s="59">
+      <c r="K7" s="59">
         <v>3</v>
       </c>
-      <c r="K7" s="59">
+      <c r="L7" s="59">
         <v>5</v>
       </c>
-      <c r="L7" s="3" t="s">
-        <v>165</v>
-      </c>
       <c r="M7" s="3" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5645,37 +5483,37 @@
         <v>80</v>
       </c>
       <c r="C8" s="55">
+        <v>1</v>
+      </c>
+      <c r="D8" s="55">
         <v>0.8</v>
       </c>
-      <c r="D8" s="55">
+      <c r="E8" s="55">
         <v>1.2</v>
       </c>
-      <c r="E8" s="59">
+      <c r="F8" s="59">
         <v>40</v>
       </c>
-      <c r="F8" s="59">
+      <c r="G8" s="59">
         <v>45</v>
       </c>
-      <c r="G8" s="59">
+      <c r="H8" s="59">
         <v>40</v>
       </c>
-      <c r="H8" s="59">
+      <c r="I8" s="59">
         <v>50</v>
       </c>
-      <c r="I8" s="11" t="s">
+      <c r="J8" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="J8" s="59">
+      <c r="K8" s="59">
         <v>4</v>
       </c>
-      <c r="K8" s="59">
+      <c r="L8" s="59">
         <v>7</v>
       </c>
-      <c r="L8" s="3" t="s">
-        <v>166</v>
-      </c>
       <c r="M8" s="3" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5686,37 +5524,37 @@
         <v>80</v>
       </c>
       <c r="C9" s="55">
+        <v>1</v>
+      </c>
+      <c r="D9" s="55">
         <v>0.8</v>
       </c>
-      <c r="D9" s="55">
+      <c r="E9" s="55">
         <v>1.2</v>
       </c>
-      <c r="E9" s="59">
+      <c r="F9" s="59">
         <v>45</v>
       </c>
-      <c r="F9" s="59">
+      <c r="G9" s="59">
         <v>50</v>
       </c>
-      <c r="G9" s="59">
+      <c r="H9" s="59">
         <v>45</v>
       </c>
-      <c r="H9" s="59">
+      <c r="I9" s="59">
         <v>20</v>
       </c>
-      <c r="I9" s="11" t="s">
+      <c r="J9" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="J9" s="59">
+      <c r="K9" s="59">
         <v>3</v>
       </c>
-      <c r="K9" s="59">
+      <c r="L9" s="59">
         <v>5</v>
       </c>
-      <c r="L9" s="3" t="s">
-        <v>167</v>
-      </c>
       <c r="M9" s="3" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5727,37 +5565,37 @@
         <v>80</v>
       </c>
       <c r="C10" s="55">
+        <v>1</v>
+      </c>
+      <c r="D10" s="55">
         <v>0.8</v>
       </c>
-      <c r="D10" s="55">
+      <c r="E10" s="55">
         <v>1.2</v>
       </c>
-      <c r="E10" s="59">
+      <c r="F10" s="59">
         <v>55</v>
       </c>
-      <c r="F10" s="59">
+      <c r="G10" s="59">
         <v>45</v>
-      </c>
-      <c r="G10" s="59">
-        <v>30</v>
       </c>
       <c r="H10" s="59">
         <v>30</v>
       </c>
-      <c r="I10" s="11" t="s">
+      <c r="I10" s="59">
+        <v>30</v>
+      </c>
+      <c r="J10" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="J10" s="59">
+      <c r="K10" s="59">
         <v>5</v>
       </c>
-      <c r="K10" s="59">
+      <c r="L10" s="59">
         <v>10</v>
       </c>
-      <c r="L10" s="3" t="s">
-        <v>168</v>
-      </c>
       <c r="M10" s="3" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5768,37 +5606,37 @@
         <v>81</v>
       </c>
       <c r="C11" s="55">
+        <v>1</v>
+      </c>
+      <c r="D11" s="55">
         <v>0.8</v>
       </c>
-      <c r="D11" s="55">
+      <c r="E11" s="55">
         <v>1.2</v>
       </c>
-      <c r="E11" s="59">
+      <c r="F11" s="59">
         <v>60</v>
       </c>
-      <c r="F11" s="59">
+      <c r="G11" s="59">
         <v>80</v>
       </c>
-      <c r="G11" s="59">
+      <c r="H11" s="59">
         <v>15</v>
       </c>
-      <c r="H11" s="59">
+      <c r="I11" s="59">
         <v>30</v>
       </c>
-      <c r="I11" s="11" t="s">
+      <c r="J11" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="J11" s="59">
+      <c r="K11" s="59">
         <v>20</v>
       </c>
-      <c r="K11" s="59">
+      <c r="L11" s="59">
         <v>30</v>
       </c>
-      <c r="L11" s="3" t="s">
-        <v>169</v>
-      </c>
       <c r="M11" s="3" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5809,37 +5647,37 @@
         <v>81</v>
       </c>
       <c r="C12" s="55">
+        <v>1</v>
+      </c>
+      <c r="D12" s="55">
         <v>0.8</v>
       </c>
-      <c r="D12" s="55">
+      <c r="E12" s="55">
         <v>1.2</v>
       </c>
-      <c r="E12" s="59">
+      <c r="F12" s="59">
         <v>80</v>
       </c>
-      <c r="F12" s="59">
+      <c r="G12" s="59">
         <v>65</v>
       </c>
-      <c r="G12" s="59">
+      <c r="H12" s="59">
         <v>20</v>
       </c>
-      <c r="H12" s="59">
+      <c r="I12" s="59">
         <v>35</v>
       </c>
-      <c r="I12" s="11" t="s">
+      <c r="J12" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="J12" s="59">
+      <c r="K12" s="59">
         <v>20</v>
       </c>
-      <c r="K12" s="59">
+      <c r="L12" s="59">
         <v>30</v>
       </c>
-      <c r="L12" s="3" t="s">
-        <v>170</v>
-      </c>
       <c r="M12" s="3" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5849,38 +5687,38 @@
       <c r="B13" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="C13" s="55">
+      <c r="C13" s="84">
+        <v>1</v>
+      </c>
+      <c r="D13" s="55">
         <v>0.8</v>
       </c>
-      <c r="D13" s="55">
+      <c r="E13" s="55">
         <v>1.2</v>
-      </c>
-      <c r="E13" s="60">
-        <v>70</v>
       </c>
       <c r="F13" s="60">
         <v>70</v>
       </c>
       <c r="G13" s="60">
+        <v>70</v>
+      </c>
+      <c r="H13" s="60">
         <v>25</v>
       </c>
-      <c r="H13" s="60">
+      <c r="I13" s="60">
         <v>40</v>
       </c>
-      <c r="I13" s="12" t="s">
+      <c r="J13" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="J13" s="60">
+      <c r="K13" s="60">
         <v>20</v>
       </c>
-      <c r="K13" s="60">
+      <c r="L13" s="60">
         <v>30</v>
       </c>
-      <c r="L13" s="3" t="s">
-        <v>171</v>
-      </c>
       <c r="M13" s="3" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
@@ -5892,6 +5730,7 @@
       </c>
       <c r="C15" s="56"/>
       <c r="D15" s="56"/>
+      <c r="E15" s="56"/>
     </row>
     <row r="16" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="52" t="s">
@@ -5902,8 +5741,9 @@
       </c>
       <c r="C16" s="56"/>
       <c r="D16" s="56"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16" s="56"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="52" t="s">
         <v>86</v>
       </c>
@@ -5912,22 +5752,24 @@
       </c>
       <c r="C17" s="56"/>
       <c r="D17" s="56"/>
+      <c r="E17" s="56"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K18"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="L18" sqref="L18"/>
+      <selection pane="topRight" activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5942,24 +5784,23 @@
     <col min="8" max="8" width="12.5703125" style="21" customWidth="1"/>
     <col min="9" max="9" width="8.5703125" style="27" customWidth="1"/>
     <col min="10" max="10" width="55" style="21" customWidth="1"/>
-    <col min="11" max="11" width="55.140625" style="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="50" t="s">
         <v>40</v>
       </c>
       <c r="B1" s="50" t="s">
-        <v>252</v>
+        <v>160</v>
       </c>
       <c r="C1" s="63" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D1" s="63" t="s">
-        <v>250</v>
+        <v>158</v>
       </c>
       <c r="E1" s="63" t="s">
-        <v>251</v>
+        <v>159</v>
       </c>
       <c r="F1" s="57" t="s">
         <v>76</v>
@@ -5974,18 +5815,15 @@
         <v>75</v>
       </c>
       <c r="J1" s="50" t="s">
-        <v>123</v>
-      </c>
-      <c r="K1" s="50" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>59</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C2" s="64">
         <v>1</v>
@@ -6011,18 +5849,15 @@
         <v>0.1</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>60</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C3" s="65">
         <v>1</v>
@@ -6046,18 +5881,15 @@
         <v>0.1</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>61</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C4" s="64">
         <v>1</v>
@@ -6083,18 +5915,15 @@
         <v>0.1</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>62</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C5" s="65">
         <v>1</v>
@@ -6120,18 +5949,15 @@
         <v>0.1</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="K5" s="3" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>63</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C6" s="64">
         <v>1</v>
@@ -6157,18 +5983,15 @@
         <v>0.1</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="K6" s="3" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>64</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C7" s="65">
         <v>1</v>
@@ -6194,18 +6017,15 @@
         <v>0.15</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="K7" s="3" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>65</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C8" s="64">
         <v>1</v>
@@ -6229,18 +6049,15 @@
         <v>0.15</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="K8" s="3" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>66</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C9" s="65">
         <v>1</v>
@@ -6266,18 +6083,15 @@
         <v>0.15</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="K9" s="3" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>67</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C10" s="64">
         <v>1</v>
@@ -6303,18 +6117,15 @@
         <v>0.15</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="K10" s="3" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>68</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C11" s="65">
         <v>1</v>
@@ -6340,18 +6151,15 @@
         <v>0.15</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="K11" s="3" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>70</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C12" s="64">
         <v>1</v>
@@ -6377,18 +6185,15 @@
         <v>0.2</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="K12" s="3" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>71</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C13" s="65">
         <v>1</v>
@@ -6412,18 +6217,15 @@
         <v>0.2</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="K13" s="3" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C14" s="64">
         <v>1</v>
@@ -6449,18 +6251,15 @@
         <v>0.2</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>196</v>
-      </c>
-      <c r="K14" s="3" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>73</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C15" s="65">
         <v>1</v>
@@ -6486,18 +6285,15 @@
         <v>0.2</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="K15" s="3" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>74</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C16" s="64">
         <v>1</v>
@@ -6523,15 +6319,12 @@
         <v>0.2</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>198</v>
-      </c>
-      <c r="K16" s="3" t="s">
-        <v>213</v>
+        <v>190</v>
       </c>
     </row>
     <row r="18" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C18" s="27" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G18" s="26" t="s">
         <v>77</v>
@@ -6548,11 +6341,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M13"/>
+  <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="L5" sqref="L5"/>
+      <selection pane="topRight" activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6569,24 +6362,23 @@
     <col min="10" max="10" width="3.28515625" style="26" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="2.5703125" style="26" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="54.85546875" style="21" customWidth="1"/>
-    <col min="13" max="13" width="56.7109375" style="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="50" t="s">
         <v>40</v>
       </c>
       <c r="B1" s="50" t="s">
-        <v>252</v>
+        <v>160</v>
       </c>
       <c r="C1" s="63" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D1" s="63" t="s">
-        <v>250</v>
+        <v>158</v>
       </c>
       <c r="E1" s="63" t="s">
-        <v>251</v>
+        <v>159</v>
       </c>
       <c r="F1" s="70" t="s">
         <v>39</v>
@@ -6607,18 +6399,15 @@
         <v>6</v>
       </c>
       <c r="L1" s="50" t="s">
-        <v>123</v>
-      </c>
-      <c r="M1" s="50" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C2" s="64">
         <v>1</v>
@@ -6649,18 +6438,15 @@
         <v>1</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>214</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C3" s="65">
         <v>1</v>
@@ -6691,18 +6477,15 @@
         <v>5</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>215</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C4" s="64">
         <v>1</v>
@@ -6732,18 +6515,15 @@
         <v>1</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>216</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C5" s="65">
         <v>1</v>
@@ -6773,18 +6553,15 @@
         <v>5</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="M5" s="3" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C6" s="64">
         <v>1</v>
@@ -6814,18 +6591,15 @@
         <v>5</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>218</v>
-      </c>
-      <c r="M6" s="3" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C7" s="65">
         <v>1</v>
@@ -6855,18 +6629,15 @@
         <v>5</v>
       </c>
       <c r="L7" s="3" t="s">
-        <v>219</v>
-      </c>
-      <c r="M7" s="3" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>25</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C8" s="64">
         <v>1</v>
@@ -6896,18 +6667,15 @@
         <v>5</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>220</v>
-      </c>
-      <c r="M8" s="3" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>28</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C9" s="65">
         <v>1</v>
@@ -6937,18 +6705,15 @@
         <v>5</v>
       </c>
       <c r="L9" s="3" t="s">
-        <v>221</v>
-      </c>
-      <c r="M9" s="3" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>27</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C10" s="64">
         <v>1</v>
@@ -6979,18 +6744,15 @@
         <v>5</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>222</v>
-      </c>
-      <c r="M10" s="3" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>26</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C11" s="65">
         <v>1</v>
@@ -7020,15 +6782,12 @@
         <v>5</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="M11" s="3" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C13" s="27" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -7041,11 +6800,11 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N11"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="M11" sqref="M11"/>
+      <selection pane="topRight" activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7061,24 +6820,23 @@
     <col min="11" max="11" width="6.7109375" style="26" customWidth="1"/>
     <col min="12" max="12" width="20.5703125" style="21" customWidth="1"/>
     <col min="13" max="13" width="55.42578125" style="21" customWidth="1"/>
-    <col min="14" max="14" width="55" style="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="23" t="s">
         <v>40</v>
       </c>
       <c r="B1" s="23" t="s">
-        <v>252</v>
+        <v>160</v>
       </c>
       <c r="C1" s="30" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D1" s="30" t="s">
-        <v>250</v>
+        <v>158</v>
       </c>
       <c r="E1" s="30" t="s">
-        <v>251</v>
+        <v>159</v>
       </c>
       <c r="F1" s="35" t="s">
         <v>50</v>
@@ -7102,13 +6860,10 @@
         <v>52</v>
       </c>
       <c r="M1" s="23" t="s">
-        <v>123</v>
-      </c>
-      <c r="N1" s="23" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>43</v>
       </c>
@@ -7146,18 +6901,15 @@
         <v>55</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>234</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C3" s="64">
         <v>1</v>
@@ -7190,18 +6942,15 @@
         <v>55</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>235</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C4" s="64">
         <v>1</v>
@@ -7234,18 +6983,15 @@
         <v>55</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>236</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C5" s="64">
         <v>1</v>
@@ -7278,18 +7024,15 @@
         <v>55</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>237</v>
-      </c>
-      <c r="N5" s="3" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C6" s="64">
         <v>1</v>
@@ -7322,18 +7065,15 @@
         <v>55</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>238</v>
-      </c>
-      <c r="N6" s="3" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>47</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C7" s="64">
         <v>1</v>
@@ -7366,18 +7106,15 @@
         <v>55</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="N7" s="3" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>48</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C8" s="64">
         <v>1</v>
@@ -7410,18 +7147,15 @@
         <v>56</v>
       </c>
       <c r="M8" s="3" t="s">
-        <v>240</v>
-      </c>
-      <c r="N8" s="3" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>49</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C9" s="64">
         <v>1</v>
@@ -7454,15 +7188,12 @@
         <v>56</v>
       </c>
       <c r="M9" s="3" t="s">
-        <v>241</v>
-      </c>
-      <c r="N9" s="3" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C11" s="27" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed Factory Class methods to static, Combined Armament-, Potion- and WeaponFactory into ItemFactory, added Template loading and list creation stuff to Resourceloader, Finished random Monster placement according to room Type in random field in room, added monsterCount to Room config
</commit_message>
<xml_diff>
--- a/RDG/config/RDG.xlsx
+++ b/RDG/config/RDG.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="10725" windowHeight="8580" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="10725" windowHeight="8580" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="6" r:id="rId1"/>
@@ -168,62 +168,65 @@
   <connection id="49" name="D_Rooms7" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="C:\Users\Flo\git\RDG\RDG\config\Drafts\D_Rooms.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="50" name="D_text" type="4" refreshedVersion="0" background="1">
+  <connection id="50" name="D_Rooms8" type="4" refreshedVersion="0" background="1">
+    <webPr xml="1" sourceData="1" url="C:\Users\Flo\git\RDG\RDG\config\Drafts\D_Rooms.xml" htmlTables="1" htmlFormat="all"/>
+  </connection>
+  <connection id="51" name="D_text" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="D:\Dokumente\fh\bif\3\ITP3\Config\Drafts\D_text.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="51" name="D_text1" type="4" refreshedVersion="0" background="1">
+  <connection id="52" name="D_text1" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="D:\Dokumente\fh\bif\3\ITP3\Config\Drafts\D_text.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="52" name="D_text2" type="4" refreshedVersion="0" background="1">
+  <connection id="53" name="D_text2" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="D:\Dokumente\fh\bif\3\ITP3\Config\Drafts\D_text.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="53" name="D_Weapons" type="4" refreshedVersion="0" background="1">
+  <connection id="54" name="D_Weapons" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="D:\Dokumente\fh\bif\3\ITP3\Config\Drafts\D_Weapons.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="54" name="D_Weapons1" type="4" refreshedVersion="0" background="1">
+  <connection id="55" name="D_Weapons1" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="D:\Dokumente\fh\bif\3\ITP3\Config\Drafts\D_Weapons.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="55" name="D_Weapons10" type="4" refreshedVersion="0" background="1">
+  <connection id="56" name="D_Weapons10" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="C:\Users\Flo\git\RDG\RDG\config\Drafts\D_Weapons.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="56" name="D_Weapons11" type="4" refreshedVersion="0" background="1">
+  <connection id="57" name="D_Weapons11" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="C:\Users\Flo\git\RDG\RDG\config\Drafts\D_Weapons.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="57" name="D_Weapons2" type="4" refreshedVersion="0" background="1">
+  <connection id="58" name="D_Weapons2" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="D:\Dokumente\fh\bif\3\ITP3\Config\Drafts\D_Weapons.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="58" name="D_Weapons3" type="4" refreshedVersion="0" background="1">
+  <connection id="59" name="D_Weapons3" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="D:\Dokumente\fh\bif\3\ITP3\Config\Drafts\D_Weapons.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="59" name="D_Weapons4" type="4" refreshedVersion="0" background="1">
+  <connection id="60" name="D_Weapons4" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="D:\Dokumente\fh\bif\3\ITP3\Config\Drafts\D_Weapons.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="60" name="D_Weapons5" type="4" refreshedVersion="0" background="1">
+  <connection id="61" name="D_Weapons5" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="C:\Users\Flo\git\RDG\RDG\config\Drafts\D_Weapons.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="61" name="D_Weapons6" type="4" refreshedVersion="0" background="1">
+  <connection id="62" name="D_Weapons6" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="C:\Users\Flo\git\RDG\RDG\config\Drafts\D_Weapons.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="62" name="D_Weapons7" type="4" refreshedVersion="0" background="1">
+  <connection id="63" name="D_Weapons7" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="C:\Users\Flo\git\RDG\RDG\config\Drafts\D_Weapons.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="63" name="D_Weapons8" type="4" refreshedVersion="0" background="1">
+  <connection id="64" name="D_Weapons8" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="C:\Users\Flo\git\RDG\RDG\config\Drafts\D_Weapons.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="64" name="D_Weapons9" type="4" refreshedVersion="0" background="1">
+  <connection id="65" name="D_Weapons9" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="C:\Users\Flo\git\RDG\RDG\config\Drafts\D_Weapons.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="65" name="Monsters" type="4" refreshedVersion="0" background="1">
+  <connection id="66" name="Monsters" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="C:\Users\Flo\git\RDG\RDG\config\Results\Monsters.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="66" name="Schema_Potions" type="4" refreshedVersion="0" background="1">
+  <connection id="67" name="Schema_Potions" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="D:\Dokumente\fh\bif\3\ITP3\Config\Schema_Potions.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="210">
   <si>
     <t>Axt</t>
   </si>
@@ -850,6 +853,9 @@
   </si>
   <si>
     <t>weapons/bow.png</t>
+  </si>
+  <si>
+    <t>Monster_Count</t>
   </si>
 </sst>
 </file>
@@ -1104,7 +1110,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1325,6 +1331,18 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="1" fontId="2" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="1" fontId="2" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1334,6 +1352,9 @@
     <xf numFmtId="1" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="1" fontId="2" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1342,131 +1363,14 @@
     </xf>
     <xf numFmtId="1" fontId="2" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="97">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Verdana"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Verdana"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Verdana"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Verdana"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
+  <dxfs count="98">
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
       <font>
@@ -3088,6 +2992,35 @@
         <name val="Verdana"/>
         <scheme val="none"/>
       </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Verdana"/>
+        <scheme val="none"/>
+      </font>
       <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
@@ -3347,6 +3280,91 @@
       </border>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Verdana"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Verdana"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Verdana"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <border outline="0">
         <left style="medium">
           <color indexed="64"/>
@@ -3508,57 +3526,6 @@
 
 <file path=xl/xmlMaps.xml><?xml version="1.0" encoding="utf-8"?>
 <MapInfo xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" SelectionNamespaces="">
-  <Schema ID="Schema31">
-    <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns="">
-      <xsd:element nillable="true" name="Rooms">
-        <xsd:complexType>
-          <xsd:sequence minOccurs="0">
-            <xsd:element minOccurs="0" maxOccurs="unbounded" nillable="true" name="Room" form="unqualified">
-              <xsd:complexType>
-                <xsd:sequence minOccurs="0">
-                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Name" form="unqualified"/>
-                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Description" form="unqualified"/>
-                  <xsd:element minOccurs="0" nillable="true" name="Door_Positions" form="unqualified">
-                    <xsd:complexType>
-                      <xsd:sequence minOccurs="0">
-                        <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="N" form="unqualified"/>
-                        <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="E" form="unqualified"/>
-                        <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="S" form="unqualified"/>
-                        <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="W" form="unqualified"/>
-                      </xsd:sequence>
-                    </xsd:complexType>
-                  </xsd:element>
-                  <xsd:element minOccurs="0" nillable="true" name="Monster" form="unqualified">
-                    <xsd:complexType>
-                      <xsd:sequence minOccurs="0">
-                        <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="no" form="unqualified"/>
-                        <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="easy" form="unqualified"/>
-                        <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="normal" form="unqualified"/>
-                        <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="hard" form="unqualified"/>
-                      </xsd:sequence>
-                    </xsd:complexType>
-                  </xsd:element>
-                  <xsd:element minOccurs="0" nillable="true" type="xsd:double" name="Item_Multiplier" form="unqualified"/>
-                  <xsd:element minOccurs="0" nillable="true" name="Find_Probabilities" form="unqualified">
-                    <xsd:complexType>
-                      <xsd:sequence minOccurs="0">
-                        <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="none" form="unqualified"/>
-                        <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="weak" form="unqualified"/>
-                        <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="medium" form="unqualified"/>
-                        <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="strong" form="unqualified"/>
-                      </xsd:sequence>
-                    </xsd:complexType>
-                  </xsd:element>
-                  <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="Item_Count" form="unqualified"/>
-                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Image" form="unqualified"/>
-                </xsd:sequence>
-              </xsd:complexType>
-            </xsd:element>
-          </xsd:sequence>
-        </xsd:complexType>
-      </xsd:element>
-    </xsd:schema>
-  </Schema>
   <Schema ID="Schema7">
     <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns="">
       <xsd:element nillable="true" name="Attacks">
@@ -3695,6 +3662,58 @@
       </xsd:element>
     </xsd:schema>
   </Schema>
+  <Schema ID="Schema8">
+    <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns="">
+      <xsd:element nillable="true" name="Rooms">
+        <xsd:complexType>
+          <xsd:sequence minOccurs="0">
+            <xsd:element minOccurs="0" maxOccurs="unbounded" nillable="true" name="Room" form="unqualified">
+              <xsd:complexType>
+                <xsd:sequence minOccurs="0">
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Name" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Description" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" name="Door_Positions" form="unqualified">
+                    <xsd:complexType>
+                      <xsd:sequence minOccurs="0">
+                        <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="N" form="unqualified"/>
+                        <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="E" form="unqualified"/>
+                        <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="S" form="unqualified"/>
+                        <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="W" form="unqualified"/>
+                      </xsd:sequence>
+                    </xsd:complexType>
+                  </xsd:element>
+                  <xsd:element minOccurs="0" nillable="true" name="Monster" form="unqualified">
+                    <xsd:complexType>
+                      <xsd:sequence minOccurs="0">
+                        <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="no" form="unqualified"/>
+                        <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="easy" form="unqualified"/>
+                        <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="normal" form="unqualified"/>
+                        <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="hard" form="unqualified"/>
+                      </xsd:sequence>
+                    </xsd:complexType>
+                  </xsd:element>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="Monster_Count" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:double" name="Item_Multiplier" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" name="Find_Probabilities" form="unqualified">
+                    <xsd:complexType>
+                      <xsd:sequence minOccurs="0">
+                        <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="none" form="unqualified"/>
+                        <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="weak" form="unqualified"/>
+                        <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="medium" form="unqualified"/>
+                        <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="strong" form="unqualified"/>
+                      </xsd:sequence>
+                    </xsd:complexType>
+                  </xsd:element>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="Item_Count" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Image" form="unqualified"/>
+                </xsd:sequence>
+              </xsd:complexType>
+            </xsd:element>
+          </xsd:sequence>
+        </xsd:complexType>
+      </xsd:element>
+    </xsd:schema>
+  </Schema>
   <Map ID="74" Name="Armaments_Map" RootElement="Armaments" SchemaID="Schema13" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true">
     <DataBinding FileBinding="true" ConnectionID="3" DataBindingLoadMode="1"/>
   </Map>
@@ -3707,69 +3726,72 @@
   <Map ID="75" Name="Potions_Map" RootElement="Potions" SchemaID="Schema14" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true">
     <DataBinding FileBinding="true" ConnectionID="32" DataBindingLoadMode="1"/>
   </Map>
-  <Map ID="60" Name="Rooms_Map" RootElement="Rooms" SchemaID="Schema31" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true">
-    <DataBinding FileBinding="true" ConnectionID="49" DataBindingLoadMode="1"/>
+  <Map ID="80" Name="Rooms_Map" RootElement="Rooms" SchemaID="Schema8" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true">
+    <DataBinding FileBinding="true" ConnectionID="50" DataBindingLoadMode="1"/>
   </Map>
   <Map ID="76" Name="Weapons_Map" RootElement="Weapons" SchemaID="Schema15" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true">
-    <DataBinding FileBinding="true" ConnectionID="56" DataBindingLoadMode="1"/>
+    <DataBinding FileBinding="true" ConnectionID="57" DataBindingLoadMode="1"/>
   </Map>
 </MapInfo>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table9" displayName="Table9" ref="A2:Q8" tableType="xml" totalsRowShown="0" headerRowDxfId="96" headerRowBorderDxfId="95" connectionId="49">
-  <autoFilter ref="A2:Q8"/>
-  <tableColumns count="17">
-    <tableColumn id="1" uniqueName="Name" name="Name" dataDxfId="94">
-      <xmlColumnPr mapId="60" xpath="/Rooms/Room/Name" xmlDataType="string"/>
-    </tableColumn>
-    <tableColumn id="2" uniqueName="Description" name="Description" dataDxfId="93">
-      <xmlColumnPr mapId="60" xpath="/Rooms/Room/Description" xmlDataType="string"/>
-    </tableColumn>
-    <tableColumn id="3" uniqueName="N" name="N" dataDxfId="92">
-      <xmlColumnPr mapId="60" xpath="/Rooms/Room/Door_Positions/N" xmlDataType="integer"/>
-    </tableColumn>
-    <tableColumn id="4" uniqueName="E" name="E" dataDxfId="91">
-      <xmlColumnPr mapId="60" xpath="/Rooms/Room/Door_Positions/E" xmlDataType="integer"/>
-    </tableColumn>
-    <tableColumn id="5" uniqueName="S" name="S" dataDxfId="90">
-      <xmlColumnPr mapId="60" xpath="/Rooms/Room/Door_Positions/S" xmlDataType="integer"/>
-    </tableColumn>
-    <tableColumn id="6" uniqueName="W" name="W" dataDxfId="89">
-      <xmlColumnPr mapId="60" xpath="/Rooms/Room/Door_Positions/W" xmlDataType="integer"/>
-    </tableColumn>
-    <tableColumn id="7" uniqueName="no" name="no" dataDxfId="88">
-      <xmlColumnPr mapId="60" xpath="/Rooms/Room/Monster/no" xmlDataType="integer"/>
-    </tableColumn>
-    <tableColumn id="8" uniqueName="easy" name="easy" dataDxfId="87">
-      <xmlColumnPr mapId="60" xpath="/Rooms/Room/Monster/easy" xmlDataType="integer"/>
-    </tableColumn>
-    <tableColumn id="9" uniqueName="normal" name="normal" dataDxfId="86">
-      <xmlColumnPr mapId="60" xpath="/Rooms/Room/Monster/normal" xmlDataType="integer"/>
-    </tableColumn>
-    <tableColumn id="10" uniqueName="hard" name="hard" dataDxfId="85">
-      <xmlColumnPr mapId="60" xpath="/Rooms/Room/Monster/hard" xmlDataType="integer"/>
-    </tableColumn>
-    <tableColumn id="11" uniqueName="Item_Multiplier" name="Item_Multiplier" dataDxfId="84">
-      <xmlColumnPr mapId="60" xpath="/Rooms/Room/Item_Multiplier" xmlDataType="double"/>
-    </tableColumn>
-    <tableColumn id="17" uniqueName="none" name="none" dataDxfId="83">
-      <xmlColumnPr mapId="60" xpath="/Rooms/Room/Find_Probabilities/none" xmlDataType="integer"/>
-    </tableColumn>
-    <tableColumn id="12" uniqueName="weak" name="weak" dataDxfId="82">
-      <xmlColumnPr mapId="60" xpath="/Rooms/Room/Find_Probabilities/weak" xmlDataType="integer"/>
-    </tableColumn>
-    <tableColumn id="13" uniqueName="medium" name="medium" dataDxfId="81">
-      <xmlColumnPr mapId="60" xpath="/Rooms/Room/Find_Probabilities/medium" xmlDataType="integer"/>
-    </tableColumn>
-    <tableColumn id="14" uniqueName="strong" name="strong" dataDxfId="80">
-      <xmlColumnPr mapId="60" xpath="/Rooms/Room/Find_Probabilities/strong" xmlDataType="integer"/>
-    </tableColumn>
-    <tableColumn id="15" uniqueName="Item_Count" name="Item_Count" dataDxfId="79">
-      <xmlColumnPr mapId="60" xpath="/Rooms/Room/Item_Count" xmlDataType="integer"/>
-    </tableColumn>
-    <tableColumn id="16" uniqueName="Image" name="Image" dataDxfId="78">
-      <xmlColumnPr mapId="60" xpath="/Rooms/Room/Image" xmlDataType="string"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table9" displayName="Table9" ref="A2:R8" tableType="xml" totalsRowShown="0" headerRowDxfId="97" headerRowBorderDxfId="96" connectionId="50">
+  <autoFilter ref="A2:R8"/>
+  <tableColumns count="18">
+    <tableColumn id="1" uniqueName="Name" name="Name" dataDxfId="95">
+      <xmlColumnPr mapId="80" xpath="/Rooms/Room/Name" xmlDataType="string"/>
+    </tableColumn>
+    <tableColumn id="2" uniqueName="Description" name="Description" dataDxfId="94">
+      <xmlColumnPr mapId="80" xpath="/Rooms/Room/Description" xmlDataType="string"/>
+    </tableColumn>
+    <tableColumn id="3" uniqueName="N" name="N" dataDxfId="93">
+      <xmlColumnPr mapId="80" xpath="/Rooms/Room/Door_Positions/N" xmlDataType="integer"/>
+    </tableColumn>
+    <tableColumn id="4" uniqueName="E" name="E" dataDxfId="92">
+      <xmlColumnPr mapId="80" xpath="/Rooms/Room/Door_Positions/E" xmlDataType="integer"/>
+    </tableColumn>
+    <tableColumn id="5" uniqueName="S" name="S" dataDxfId="91">
+      <xmlColumnPr mapId="80" xpath="/Rooms/Room/Door_Positions/S" xmlDataType="integer"/>
+    </tableColumn>
+    <tableColumn id="6" uniqueName="W" name="W" dataDxfId="90">
+      <xmlColumnPr mapId="80" xpath="/Rooms/Room/Door_Positions/W" xmlDataType="integer"/>
+    </tableColumn>
+    <tableColumn id="7" uniqueName="no" name="no" dataDxfId="89">
+      <xmlColumnPr mapId="80" xpath="/Rooms/Room/Monster/no" xmlDataType="integer"/>
+    </tableColumn>
+    <tableColumn id="8" uniqueName="easy" name="easy" dataDxfId="88">
+      <xmlColumnPr mapId="80" xpath="/Rooms/Room/Monster/easy" xmlDataType="integer"/>
+    </tableColumn>
+    <tableColumn id="9" uniqueName="normal" name="normal" dataDxfId="87">
+      <xmlColumnPr mapId="80" xpath="/Rooms/Room/Monster/normal" xmlDataType="integer"/>
+    </tableColumn>
+    <tableColumn id="10" uniqueName="hard" name="hard" dataDxfId="86">
+      <xmlColumnPr mapId="80" xpath="/Rooms/Room/Monster/hard" xmlDataType="integer"/>
+    </tableColumn>
+    <tableColumn id="18" uniqueName="Monster_Count" name="Monster_Count" dataDxfId="0">
+      <xmlColumnPr mapId="80" xpath="/Rooms/Room/Monster_Count" xmlDataType="integer"/>
+    </tableColumn>
+    <tableColumn id="11" uniqueName="Item_Multiplier" name="Item_Multiplier" dataDxfId="85">
+      <xmlColumnPr mapId="80" xpath="/Rooms/Room/Item_Multiplier" xmlDataType="double"/>
+    </tableColumn>
+    <tableColumn id="17" uniqueName="none" name="none" dataDxfId="84">
+      <xmlColumnPr mapId="80" xpath="/Rooms/Room/Find_Probabilities/none" xmlDataType="integer"/>
+    </tableColumn>
+    <tableColumn id="12" uniqueName="weak" name="weak" dataDxfId="83">
+      <xmlColumnPr mapId="80" xpath="/Rooms/Room/Find_Probabilities/weak" xmlDataType="integer"/>
+    </tableColumn>
+    <tableColumn id="13" uniqueName="medium" name="medium" dataDxfId="82">
+      <xmlColumnPr mapId="80" xpath="/Rooms/Room/Find_Probabilities/medium" xmlDataType="integer"/>
+    </tableColumn>
+    <tableColumn id="14" uniqueName="strong" name="strong" dataDxfId="81">
+      <xmlColumnPr mapId="80" xpath="/Rooms/Room/Find_Probabilities/strong" xmlDataType="integer"/>
+    </tableColumn>
+    <tableColumn id="15" uniqueName="Item_Count" name="Item_Count" dataDxfId="80">
+      <xmlColumnPr mapId="80" xpath="/Rooms/Room/Item_Count" xmlDataType="integer"/>
+    </tableColumn>
+    <tableColumn id="16" uniqueName="Image" name="Image" dataDxfId="79">
+      <xmlColumnPr mapId="80" xpath="/Rooms/Room/Image" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -3777,31 +3799,31 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table8" displayName="Table8" ref="A1:H5" tableType="xml" totalsRowShown="0" headerRowDxfId="77" dataDxfId="75" headerRowBorderDxfId="76" tableBorderDxfId="74" connectionId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table8" displayName="Table8" ref="A1:H5" tableType="xml" totalsRowShown="0" headerRowDxfId="78" dataDxfId="76" headerRowBorderDxfId="77" tableBorderDxfId="75" connectionId="18">
   <autoFilter ref="A1:H5"/>
   <tableColumns count="8">
-    <tableColumn id="1" uniqueName="Name" name="Name" dataDxfId="2">
+    <tableColumn id="1" uniqueName="Name" name="Name" dataDxfId="74">
       <xmlColumnPr mapId="68" xpath="/Attacks/Attack/Name" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="8" uniqueName="Class_Multiplier" name="Class Multiplier" dataDxfId="0">
+    <tableColumn id="8" uniqueName="Class_Multiplier" name="Class Multiplier" dataDxfId="73">
       <xmlColumnPr mapId="68" xpath="/Attacks/Attack/Class_Multiplier" xmlDataType="double"/>
     </tableColumn>
-    <tableColumn id="6" uniqueName="Stats_Low_Multiplier" name="Stats Low Multiplier" dataDxfId="1">
+    <tableColumn id="6" uniqueName="Stats_Low_Multiplier" name="Stats Low Multiplier" dataDxfId="72">
       <xmlColumnPr mapId="68" xpath="/Attacks/Attack/Stats_Low_Multiplier" xmlDataType="double"/>
     </tableColumn>
-    <tableColumn id="7" uniqueName="Stats_High_Multiplier" name="Stats High Multiplier" dataDxfId="73">
+    <tableColumn id="7" uniqueName="Stats_High_Multiplier" name="Stats High Multiplier" dataDxfId="71">
       <xmlColumnPr mapId="68" xpath="/Attacks/Attack/Stats_High_Multiplier" xmlDataType="double"/>
     </tableColumn>
-    <tableColumn id="2" uniqueName="HP_Damage" name="HP Damage" dataDxfId="72">
+    <tableColumn id="2" uniqueName="HP_Damage" name="HP Damage" dataDxfId="70">
       <xmlColumnPr mapId="68" xpath="/Attacks/Attack/HP_Damage" xmlDataType="double"/>
     </tableColumn>
-    <tableColumn id="3" uniqueName="Hit_Probability" name="Hit Probability" dataDxfId="71">
+    <tableColumn id="3" uniqueName="Hit_Probability" name="Hit Probability" dataDxfId="69">
       <xmlColumnPr mapId="68" xpath="/Attacks/Attack/Hit_Probability" xmlDataType="double"/>
     </tableColumn>
-    <tableColumn id="4" uniqueName="Effect" name="Effect" dataDxfId="70">
+    <tableColumn id="4" uniqueName="Effect" name="Effect" dataDxfId="68">
       <xmlColumnPr mapId="68" xpath="/Attacks/Attack/Effect" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="5" uniqueName="x" name="x" dataDxfId="69">
+    <tableColumn id="5" uniqueName="x" name="x" dataDxfId="67">
       <xmlColumnPr mapId="68" xpath="/Attacks/Attack/x" xmlDataType="double"/>
     </tableColumn>
   </tableColumns>
@@ -3810,46 +3832,46 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="A1:M13" tableType="xml" totalsRowShown="0" headerRowDxfId="68" dataDxfId="66" headerRowBorderDxfId="67" tableBorderDxfId="65" connectionId="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="A1:M13" tableType="xml" totalsRowShown="0" headerRowDxfId="66" dataDxfId="64" headerRowBorderDxfId="65" tableBorderDxfId="63" connectionId="21">
   <autoFilter ref="A1:M13"/>
   <tableColumns count="13">
-    <tableColumn id="1" uniqueName="Name" name="Name" dataDxfId="64">
+    <tableColumn id="1" uniqueName="Name" name="Name" dataDxfId="62">
       <xmlColumnPr mapId="71" xpath="/Monsters/Monster/Name" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="2" uniqueName="Level" name="Level" dataDxfId="63">
+    <tableColumn id="2" uniqueName="Level" name="Level" dataDxfId="61">
       <xmlColumnPr mapId="71" xpath="/Monsters/Monster/Level" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="14" uniqueName="Class_Multiplier" name="Class Multiplier" dataDxfId="3">
+    <tableColumn id="14" uniqueName="Class_Multiplier" name="Class Multiplier" dataDxfId="60">
       <xmlColumnPr mapId="71" xpath="/Monsters/Monster/Class_Multiplier" xmlDataType="double"/>
     </tableColumn>
-    <tableColumn id="10" uniqueName="Stats_Low_Multiplier" name="Stats Low Multiplier" dataDxfId="62">
+    <tableColumn id="10" uniqueName="Stats_Low_Multiplier" name="Stats Low Multiplier" dataDxfId="59">
       <xmlColumnPr mapId="71" xpath="/Monsters/Monster/Stats_Low_Multiplier" xmlDataType="double"/>
     </tableColumn>
-    <tableColumn id="13" uniqueName="Stats_High_Multiplier" name="Stats High Multiplier" dataDxfId="61">
+    <tableColumn id="13" uniqueName="Stats_High_Multiplier" name="Stats High Multiplier" dataDxfId="58">
       <xmlColumnPr mapId="71" xpath="/Monsters/Monster/Stats_High_Multiplier" xmlDataType="double"/>
     </tableColumn>
-    <tableColumn id="3" uniqueName="HP" name="HP" dataDxfId="60">
+    <tableColumn id="3" uniqueName="HP" name="HP" dataDxfId="57">
       <xmlColumnPr mapId="71" xpath="/Monsters/Monster/HP" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="4" uniqueName="Strength" name="Strength" dataDxfId="59">
+    <tableColumn id="4" uniqueName="Strength" name="Strength" dataDxfId="56">
       <xmlColumnPr mapId="71" xpath="/Monsters/Monster/Strength" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="5" uniqueName="Speed" name="Speed" dataDxfId="58">
+    <tableColumn id="5" uniqueName="Speed" name="Speed" dataDxfId="55">
       <xmlColumnPr mapId="71" xpath="/Monsters/Monster/Speed" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="6" uniqueName="Accuracy" name="Accuracy" dataDxfId="57">
+    <tableColumn id="6" uniqueName="Accuracy" name="Accuracy" dataDxfId="54">
       <xmlColumnPr mapId="71" xpath="/Monsters/Monster/Accuracy" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="7" uniqueName="Kill_Bonus_Type" name="Kill Bonus Type" dataDxfId="56">
+    <tableColumn id="7" uniqueName="Kill_Bonus_Type" name="Kill Bonus Type" dataDxfId="53">
       <xmlColumnPr mapId="71" xpath="/Monsters/Monster/Kill_Bonus_Type" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="8" uniqueName="Kill_Bonus_Low" name="Kill Bonus Low" dataDxfId="55">
+    <tableColumn id="8" uniqueName="Kill_Bonus_Low" name="Kill Bonus Low" dataDxfId="52">
       <xmlColumnPr mapId="71" xpath="/Monsters/Monster/Kill_Bonus_Low" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="9" uniqueName="Kill_Bonus_High" name="Kill Bonus High" dataDxfId="54">
+    <tableColumn id="9" uniqueName="Kill_Bonus_High" name="Kill Bonus High" dataDxfId="51">
       <xmlColumnPr mapId="71" xpath="/Monsters/Monster/Kill_Bonus_High" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="11" uniqueName="Image" name="Image" dataDxfId="53">
+    <tableColumn id="11" uniqueName="Image" name="Image" dataDxfId="50">
       <xmlColumnPr mapId="71" xpath="/Monsters/Monster/Image" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
@@ -3858,37 +3880,37 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:J16" tableType="xml" totalsRowShown="0" headerRowDxfId="52" dataDxfId="50" headerRowBorderDxfId="51" tableBorderDxfId="49" totalsRowBorderDxfId="48" connectionId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:J16" tableType="xml" totalsRowShown="0" headerRowDxfId="49" dataDxfId="47" headerRowBorderDxfId="48" tableBorderDxfId="46" totalsRowBorderDxfId="45" connectionId="3">
   <autoFilter ref="A1:J16"/>
   <tableColumns count="10">
-    <tableColumn id="1" uniqueName="Name" name="Name" dataDxfId="47">
+    <tableColumn id="1" uniqueName="Name" name="Name" dataDxfId="44">
       <xmlColumnPr mapId="74" xpath="/Armaments/Armament/Name" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="9" uniqueName="Item_Class" name="Item Class" dataDxfId="46">
+    <tableColumn id="9" uniqueName="Item_Class" name="Item Class" dataDxfId="43">
       <xmlColumnPr mapId="74" xpath="/Armaments/Armament/Item_Class" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="10" uniqueName="Class_Multiplier" name="Class Multiplier" dataDxfId="45">
+    <tableColumn id="10" uniqueName="Class_Multiplier" name="Class Multiplier" dataDxfId="42">
       <xmlColumnPr mapId="74" xpath="/Armaments/Armament/Class_Multiplier" xmlDataType="double"/>
     </tableColumn>
-    <tableColumn id="6" uniqueName="Stats_Low_Multiplier" name="Stats Low Multiplier" dataDxfId="44">
+    <tableColumn id="6" uniqueName="Stats_Low_Multiplier" name="Stats Low Multiplier" dataDxfId="41">
       <xmlColumnPr mapId="74" xpath="/Armaments/Armament/Stats_Low_Multiplier" xmlDataType="double"/>
     </tableColumn>
-    <tableColumn id="11" uniqueName="Stats_High_Multiplier" name="Stats High Multiplier" dataDxfId="43">
+    <tableColumn id="11" uniqueName="Stats_High_Multiplier" name="Stats High Multiplier" dataDxfId="40">
       <xmlColumnPr mapId="74" xpath="/Armaments/Armament/Stats_High_Multiplier" xmlDataType="double"/>
     </tableColumn>
-    <tableColumn id="2" uniqueName="Armor" name="Armor" dataDxfId="42">
+    <tableColumn id="2" uniqueName="Armor" name="Armor" dataDxfId="39">
       <xmlColumnPr mapId="74" xpath="/Armaments/Armament/Armor" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="3" uniqueName="Speed" name="Speed" dataDxfId="41">
+    <tableColumn id="3" uniqueName="Speed" name="Speed" dataDxfId="38">
       <xmlColumnPr mapId="74" xpath="/Armaments/Armament/Speed" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="4" uniqueName="Type" name="Type" dataDxfId="40">
+    <tableColumn id="4" uniqueName="Type" name="Type" dataDxfId="37">
       <xmlColumnPr mapId="74" xpath="/Armaments/Armament/Type" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="5" uniqueName="Bonus" name="Bonus" dataDxfId="39">
+    <tableColumn id="5" uniqueName="Bonus" name="Bonus" dataDxfId="36">
       <xmlColumnPr mapId="74" xpath="/Armaments/Armament/Bonus" xmlDataType="double"/>
     </tableColumn>
-    <tableColumn id="7" uniqueName="Image" name="Image" dataDxfId="38">
+    <tableColumn id="7" uniqueName="Image" name="Image" dataDxfId="35">
       <xmlColumnPr mapId="74" xpath="/Armaments/Armament/Image" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
@@ -3897,43 +3919,43 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:L11" tableType="xml" totalsRowShown="0" headerRowDxfId="37" dataDxfId="35" headerRowBorderDxfId="36" tableBorderDxfId="34" totalsRowBorderDxfId="33" connectionId="32">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:L11" tableType="xml" totalsRowShown="0" headerRowDxfId="34" dataDxfId="32" headerRowBorderDxfId="33" tableBorderDxfId="31" totalsRowBorderDxfId="30" connectionId="32">
   <autoFilter ref="A1:L11"/>
   <tableColumns count="12">
-    <tableColumn id="1" uniqueName="Name" name="Name" dataDxfId="32">
+    <tableColumn id="1" uniqueName="Name" name="Name" dataDxfId="29">
       <xmlColumnPr mapId="75" xpath="/Potions/Potion/Name" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="10" uniqueName="Item_Class" name="Item Class" dataDxfId="31">
+    <tableColumn id="10" uniqueName="Item_Class" name="Item Class" dataDxfId="28">
       <xmlColumnPr mapId="75" xpath="/Potions/Potion/Item_Class" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="11" uniqueName="Class_Multiplier" name="Class Multiplier" dataDxfId="30">
+    <tableColumn id="11" uniqueName="Class_Multiplier" name="Class Multiplier" dataDxfId="27">
       <xmlColumnPr mapId="75" xpath="/Potions/Potion/Class_Multiplier" xmlDataType="double"/>
     </tableColumn>
-    <tableColumn id="12" uniqueName="Stats_Low_Multiplier" name="Stats Low Multiplier" dataDxfId="29">
+    <tableColumn id="12" uniqueName="Stats_Low_Multiplier" name="Stats Low Multiplier" dataDxfId="26">
       <xmlColumnPr mapId="75" xpath="/Potions/Potion/Stats_Low_Multiplier" xmlDataType="double"/>
     </tableColumn>
-    <tableColumn id="13" uniqueName="Stats_High_Multiplier" name="Stats High Multiplier" dataDxfId="28">
+    <tableColumn id="13" uniqueName="Stats_High_Multiplier" name="Stats High Multiplier" dataDxfId="25">
       <xmlColumnPr mapId="75" xpath="/Potions/Potion/Stats_High_Multiplier" xmlDataType="double"/>
     </tableColumn>
-    <tableColumn id="2" uniqueName="Description" name="Description" dataDxfId="27">
+    <tableColumn id="2" uniqueName="Description" name="Description" dataDxfId="24">
       <xmlColumnPr mapId="75" xpath="/Potions/Potion/Description" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="3" uniqueName="Target" name="Target" dataDxfId="26">
+    <tableColumn id="3" uniqueName="Target" name="Target" dataDxfId="23">
       <xmlColumnPr mapId="75" xpath="/Potions/Potion/Target" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="4" uniqueName="Effect" name="Effect" dataDxfId="25">
+    <tableColumn id="4" uniqueName="Effect" name="Effect" dataDxfId="22">
       <xmlColumnPr mapId="75" xpath="/Potions/Potion/Effect" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="5" uniqueName="Mode" name="Mode" dataDxfId="24">
+    <tableColumn id="5" uniqueName="Mode" name="Mode" dataDxfId="21">
       <xmlColumnPr mapId="75" xpath="/Potions/Potion/Mode" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="6" uniqueName="x" name="x" dataDxfId="23">
+    <tableColumn id="6" uniqueName="x" name="x" dataDxfId="20">
       <xmlColumnPr mapId="75" xpath="/Potions/Potion/x" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="7" uniqueName="n" name="n" dataDxfId="22">
+    <tableColumn id="7" uniqueName="n" name="n" dataDxfId="19">
       <xmlColumnPr mapId="75" xpath="/Potions/Potion/n" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="8" uniqueName="Image" name="Image" dataDxfId="21">
+    <tableColumn id="8" uniqueName="Image" name="Image" dataDxfId="18">
       <xmlColumnPr mapId="75" xpath="/Potions/Potion/Image" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
@@ -3942,47 +3964,47 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:M9" tableType="xml" totalsRowShown="0" headerRowDxfId="20" dataDxfId="18" headerRowBorderDxfId="19" tableBorderDxfId="17" connectionId="56">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:M9" tableType="xml" totalsRowShown="0" headerRowDxfId="17" dataDxfId="15" headerRowBorderDxfId="16" tableBorderDxfId="14" connectionId="57">
   <autoFilter ref="A1:M9"/>
   <tableColumns count="13">
-    <tableColumn id="1" uniqueName="Name" name="Name" dataDxfId="16">
+    <tableColumn id="1" uniqueName="Name" name="Name" dataDxfId="13">
       <xmlColumnPr mapId="76" xpath="/Weapons/Weapon/Name" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="11" uniqueName="Item_Class" name="Item Class" dataDxfId="15">
+    <tableColumn id="11" uniqueName="Item_Class" name="Item Class" dataDxfId="12">
       <xmlColumnPr mapId="76" xpath="/Weapons/Weapon/Item_Class" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="12" uniqueName="Class_Multiplier" name="Class Multiplier" dataDxfId="14">
+    <tableColumn id="12" uniqueName="Class_Multiplier" name="Class Multiplier" dataDxfId="11">
       <xmlColumnPr mapId="76" xpath="/Weapons/Weapon/Class_Multiplier" xmlDataType="double"/>
     </tableColumn>
-    <tableColumn id="13" uniqueName="Stats_Low_Multiplier" name="Stats Low Multiplier" dataDxfId="13">
+    <tableColumn id="13" uniqueName="Stats_Low_Multiplier" name="Stats Low Multiplier" dataDxfId="10">
       <xmlColumnPr mapId="76" xpath="/Weapons/Weapon/Stats_Low_Multiplier" xmlDataType="double"/>
     </tableColumn>
-    <tableColumn id="14" uniqueName="Stats_High_Multiplier" name="Stats High Multiplier" dataDxfId="12">
+    <tableColumn id="14" uniqueName="Stats_High_Multiplier" name="Stats High Multiplier" dataDxfId="9">
       <xmlColumnPr mapId="76" xpath="/Weapons/Weapon/Stats_High_Multiplier" xmlDataType="double"/>
     </tableColumn>
-    <tableColumn id="2" uniqueName="Attack" name="Attack" dataDxfId="11">
+    <tableColumn id="2" uniqueName="Attack" name="Attack" dataDxfId="8">
       <xmlColumnPr mapId="76" xpath="/Weapons/Weapon/Attack" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="3" uniqueName="Speed" name="Speed" dataDxfId="10">
+    <tableColumn id="3" uniqueName="Speed" name="Speed" dataDxfId="7">
       <xmlColumnPr mapId="76" xpath="/Weapons/Weapon/Speed" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="4" uniqueName="Accuracy" name="Accuracy" dataDxfId="9">
+    <tableColumn id="4" uniqueName="Accuracy" name="Accuracy" dataDxfId="6">
       <xmlColumnPr mapId="76" xpath="/Weapons/Weapon/Accuracy" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="5" uniqueName="Defence" name="Defence" dataDxfId="8">
+    <tableColumn id="5" uniqueName="Defence" name="Defence" dataDxfId="5">
       <calculatedColumnFormula>"-"</calculatedColumnFormula>
       <xmlColumnPr mapId="76" xpath="/Weapons/Weapon/Defence" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="6" uniqueName="Slots" name="Slots" dataDxfId="7">
+    <tableColumn id="6" uniqueName="Slots" name="Slots" dataDxfId="4">
       <xmlColumnPr mapId="76" xpath="/Weapons/Weapon/Slots" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="7" uniqueName="Max" name="Max" dataDxfId="6">
+    <tableColumn id="7" uniqueName="Max" name="Max" dataDxfId="3">
       <xmlColumnPr mapId="76" xpath="/Weapons/Weapon/Max" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="8" uniqueName="Type" name="Type" dataDxfId="5">
+    <tableColumn id="8" uniqueName="Type" name="Type" dataDxfId="2">
       <xmlColumnPr mapId="76" xpath="/Weapons/Weapon/Type" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="9" uniqueName="Image" name="Image" dataDxfId="4">
+    <tableColumn id="9" uniqueName="Image" name="Image" dataDxfId="1">
       <xmlColumnPr mapId="76" xpath="/Weapons/Weapon/Image" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
@@ -4307,11 +4329,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q26"/>
+  <dimension ref="A1:R26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="L23" sqref="L23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="Q31" sqref="Q31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4326,41 +4348,43 @@
     <col min="8" max="8" width="11.140625" style="26" customWidth="1"/>
     <col min="9" max="9" width="11.28515625" style="26" customWidth="1"/>
     <col min="10" max="10" width="13" style="26" customWidth="1"/>
-    <col min="11" max="11" width="21.85546875" style="27" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.5703125" style="26" customWidth="1"/>
-    <col min="13" max="13" width="8" style="26" customWidth="1"/>
-    <col min="14" max="14" width="14.28515625" style="26" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.85546875" style="26" customWidth="1"/>
-    <col min="16" max="16" width="18.42578125" style="26" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="28.5703125" style="21" customWidth="1"/>
+    <col min="11" max="11" width="18.85546875" style="26" customWidth="1"/>
+    <col min="12" max="12" width="21.85546875" style="27" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.5703125" style="26" customWidth="1"/>
+    <col min="14" max="14" width="8" style="26" customWidth="1"/>
+    <col min="15" max="15" width="14.28515625" style="26" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.85546875" style="26" customWidth="1"/>
+    <col min="17" max="17" width="18.42578125" style="26" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="28.5703125" style="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="22"/>
       <c r="B1" s="22"/>
-      <c r="C1" s="78" t="s">
+      <c r="C1" s="82" t="s">
         <v>123</v>
       </c>
-      <c r="D1" s="79"/>
-      <c r="E1" s="79"/>
-      <c r="F1" s="80"/>
-      <c r="G1" s="78" t="s">
+      <c r="D1" s="83"/>
+      <c r="E1" s="83"/>
+      <c r="F1" s="84"/>
+      <c r="G1" s="82" t="s">
         <v>120</v>
       </c>
-      <c r="H1" s="79"/>
-      <c r="I1" s="79"/>
-      <c r="J1" s="80"/>
-      <c r="K1" s="29"/>
-      <c r="L1" s="81" t="s">
+      <c r="H1" s="83"/>
+      <c r="I1" s="83"/>
+      <c r="J1" s="84"/>
+      <c r="K1" s="79"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="86" t="s">
         <v>152</v>
       </c>
-      <c r="M1" s="82"/>
-      <c r="N1" s="82"/>
-      <c r="O1" s="83"/>
-      <c r="P1" s="36"/>
-      <c r="Q1" s="38"/>
-    </row>
-    <row r="2" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N1" s="87"/>
+      <c r="O1" s="87"/>
+      <c r="P1" s="88"/>
+      <c r="Q1" s="36"/>
+      <c r="R1" s="38"/>
+    </row>
+    <row r="2" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="23" t="s">
         <v>40</v>
       </c>
@@ -4391,29 +4415,32 @@
       <c r="J2" s="35" t="s">
         <v>81</v>
       </c>
-      <c r="K2" s="30" t="s">
+      <c r="K2" s="78" t="s">
+        <v>209</v>
+      </c>
+      <c r="L2" s="30" t="s">
         <v>156</v>
       </c>
-      <c r="L2" s="32" t="s">
+      <c r="M2" s="32" t="s">
         <v>161</v>
       </c>
-      <c r="M2" s="32" t="s">
+      <c r="N2" s="32" t="s">
         <v>147</v>
       </c>
-      <c r="N2" s="32" t="s">
+      <c r="O2" s="32" t="s">
         <v>148</v>
       </c>
-      <c r="O2" s="32" t="s">
+      <c r="P2" s="32" t="s">
         <v>149</v>
       </c>
-      <c r="P2" s="37" t="s">
+      <c r="Q2" s="37" t="s">
         <v>157</v>
       </c>
-      <c r="Q2" s="39" t="s">
+      <c r="R2" s="39" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
         <v>108</v>
       </c>
@@ -4444,29 +4471,32 @@
       <c r="J3" s="26">
         <v>0</v>
       </c>
-      <c r="K3" s="27">
+      <c r="K3" s="26">
+        <v>1</v>
+      </c>
+      <c r="L3" s="27">
         <v>1.5</v>
       </c>
-      <c r="L3" s="26">
+      <c r="M3" s="26">
         <v>0</v>
       </c>
-      <c r="M3" s="26">
+      <c r="N3" s="26">
         <v>30</v>
       </c>
-      <c r="N3" s="26">
+      <c r="O3" s="26">
         <v>50</v>
       </c>
-      <c r="O3" s="26">
+      <c r="P3" s="26">
         <v>20</v>
       </c>
-      <c r="P3" s="26">
+      <c r="Q3" s="26">
         <v>3</v>
       </c>
-      <c r="Q3" s="21" t="s">
+      <c r="R3" s="21" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
         <v>109</v>
       </c>
@@ -4497,29 +4527,32 @@
       <c r="J4" s="26">
         <v>0</v>
       </c>
-      <c r="K4" s="27">
+      <c r="K4" s="26">
+        <v>1</v>
+      </c>
+      <c r="L4" s="27">
         <v>1.25</v>
-      </c>
-      <c r="L4" s="26">
-        <v>30</v>
       </c>
       <c r="M4" s="26">
         <v>30</v>
       </c>
       <c r="N4" s="26">
+        <v>30</v>
+      </c>
+      <c r="O4" s="26">
         <v>40</v>
       </c>
-      <c r="O4" s="26">
+      <c r="P4" s="26">
         <v>0</v>
       </c>
-      <c r="P4" s="26">
+      <c r="Q4" s="26">
         <v>2</v>
       </c>
-      <c r="Q4" s="21" t="s">
+      <c r="R4" s="21" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
         <v>110</v>
       </c>
@@ -4550,29 +4583,32 @@
       <c r="J5" s="26">
         <v>0</v>
       </c>
-      <c r="K5" s="27">
+      <c r="K5" s="26">
+        <v>1</v>
+      </c>
+      <c r="L5" s="27">
         <v>1.25</v>
-      </c>
-      <c r="L5" s="26">
-        <v>30</v>
       </c>
       <c r="M5" s="26">
         <v>30</v>
       </c>
       <c r="N5" s="26">
+        <v>30</v>
+      </c>
+      <c r="O5" s="26">
         <v>40</v>
       </c>
-      <c r="O5" s="26">
+      <c r="P5" s="26">
         <v>0</v>
       </c>
-      <c r="P5" s="26">
+      <c r="Q5" s="26">
         <v>2</v>
       </c>
-      <c r="Q5" s="21" t="s">
+      <c r="R5" s="21" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="21" t="s">
         <v>111</v>
       </c>
@@ -4603,29 +4639,32 @@
       <c r="J6" s="26">
         <v>0</v>
       </c>
-      <c r="K6" s="27">
+      <c r="K6" s="26">
+        <v>1</v>
+      </c>
+      <c r="L6" s="27">
         <v>1.1000000000000001</v>
       </c>
-      <c r="L6" s="26">
+      <c r="M6" s="26">
         <v>25</v>
       </c>
-      <c r="M6" s="26">
+      <c r="N6" s="26">
         <v>50</v>
       </c>
-      <c r="N6" s="26">
+      <c r="O6" s="26">
         <v>25</v>
       </c>
-      <c r="O6" s="26">
+      <c r="P6" s="26">
         <v>0</v>
       </c>
-      <c r="P6" s="26">
-        <v>1</v>
-      </c>
-      <c r="Q6" s="21" t="s">
+      <c r="Q6" s="26">
+        <v>1</v>
+      </c>
+      <c r="R6" s="21" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="21" t="s">
         <v>112</v>
       </c>
@@ -4656,29 +4695,32 @@
       <c r="J7" s="26">
         <v>0</v>
       </c>
-      <c r="K7" s="27">
-        <v>1</v>
-      </c>
-      <c r="L7" s="26">
-        <v>50</v>
+      <c r="K7" s="26">
+        <v>1</v>
+      </c>
+      <c r="L7" s="27">
+        <v>1</v>
       </c>
       <c r="M7" s="26">
         <v>50</v>
       </c>
       <c r="N7" s="26">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="O7" s="26">
         <v>0</v>
       </c>
       <c r="P7" s="26">
-        <v>1</v>
-      </c>
-      <c r="Q7" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="26">
+        <v>1</v>
+      </c>
+      <c r="R7" s="21" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="21" t="s">
         <v>113</v>
       </c>
@@ -4709,54 +4751,58 @@
       <c r="J8" s="26">
         <v>1</v>
       </c>
-      <c r="K8" s="27">
+      <c r="K8" s="26">
+        <v>1</v>
+      </c>
+      <c r="L8" s="27">
         <v>2</v>
       </c>
-      <c r="L8" s="26">
+      <c r="M8" s="26">
         <v>0</v>
       </c>
-      <c r="M8" s="26">
+      <c r="N8" s="26">
         <v>10</v>
       </c>
-      <c r="N8" s="26">
+      <c r="O8" s="26">
         <v>20</v>
       </c>
-      <c r="O8" s="26">
+      <c r="P8" s="26">
         <v>70</v>
       </c>
-      <c r="P8" s="26">
+      <c r="Q8" s="26">
         <v>5</v>
       </c>
-      <c r="Q8" s="21" t="s">
+      <c r="R8" s="21" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="21" t="s">
         <v>144</v>
       </c>
-      <c r="C10" s="77" t="s">
+      <c r="C10" s="85" t="s">
         <v>129</v>
       </c>
-      <c r="D10" s="77"/>
-      <c r="E10" s="77"/>
-      <c r="F10" s="77"/>
-      <c r="G10" s="77" t="s">
+      <c r="D10" s="85"/>
+      <c r="E10" s="85"/>
+      <c r="F10" s="85"/>
+      <c r="G10" s="85" t="s">
         <v>128</v>
       </c>
-      <c r="H10" s="77"/>
-      <c r="I10" s="77"/>
-      <c r="J10" s="77"/>
-      <c r="K10" s="31"/>
-      <c r="L10" s="33"/>
-      <c r="M10" s="77" t="s">
+      <c r="H10" s="85"/>
+      <c r="I10" s="85"/>
+      <c r="J10" s="85"/>
+      <c r="K10" s="77"/>
+      <c r="L10" s="31"/>
+      <c r="M10" s="33"/>
+      <c r="N10" s="85" t="s">
         <v>153</v>
       </c>
-      <c r="N10" s="77"/>
-      <c r="O10" s="77"/>
-      <c r="P10" s="33"/>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="O10" s="85"/>
+      <c r="P10" s="85"/>
+      <c r="Q10" s="33"/>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="21" t="s">
         <v>142</v>
       </c>
@@ -4764,14 +4810,15 @@
       <c r="H11" s="34"/>
       <c r="I11" s="34"/>
       <c r="J11" s="34"/>
-      <c r="K11" s="28"/>
-      <c r="L11" s="34"/>
+      <c r="K11" s="34"/>
+      <c r="L11" s="28"/>
       <c r="M11" s="34"/>
       <c r="N11" s="34"/>
       <c r="O11" s="34"/>
       <c r="P11" s="34"/>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q11" s="34"/>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="21" t="s">
         <v>145</v>
       </c>
@@ -4781,16 +4828,17 @@
       <c r="H12" s="34"/>
       <c r="I12" s="34"/>
       <c r="J12" s="34"/>
-      <c r="K12" s="28"/>
-      <c r="L12" s="34"/>
-      <c r="M12" s="34" t="s">
+      <c r="K12" s="34"/>
+      <c r="L12" s="28"/>
+      <c r="M12" s="34"/>
+      <c r="N12" s="34" t="s">
         <v>154</v>
       </c>
-      <c r="N12" s="34"/>
       <c r="O12" s="34"/>
       <c r="P12" s="34"/>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q12" s="34"/>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="21" t="s">
         <v>146</v>
       </c>
@@ -4798,170 +4846,176 @@
       <c r="H13" s="34"/>
       <c r="I13" s="34"/>
       <c r="J13" s="34"/>
-      <c r="K13" s="28"/>
-      <c r="L13" s="34"/>
-      <c r="M13" s="34" t="s">
+      <c r="K13" s="34"/>
+      <c r="L13" s="28"/>
+      <c r="M13" s="34"/>
+      <c r="N13" s="34" t="s">
         <v>155</v>
       </c>
-      <c r="N13" s="34"/>
       <c r="O13" s="34"/>
       <c r="P13" s="34"/>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="G14" s="77" t="s">
+      <c r="Q13" s="34"/>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="G14" s="85" t="s">
         <v>130</v>
       </c>
-      <c r="H14" s="77"/>
-      <c r="I14" s="77"/>
-      <c r="J14" s="77"/>
-      <c r="K14" s="31"/>
-      <c r="L14" s="33"/>
+      <c r="H14" s="85"/>
+      <c r="I14" s="85"/>
+      <c r="J14" s="85"/>
+      <c r="K14" s="77"/>
+      <c r="L14" s="31"/>
       <c r="M14" s="33"/>
       <c r="N14" s="33"/>
       <c r="O14" s="33"/>
       <c r="P14" s="33"/>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q14" s="33"/>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="21" t="s">
         <v>143</v>
       </c>
-      <c r="G15" s="77" t="s">
+      <c r="G15" s="85" t="s">
         <v>131</v>
       </c>
-      <c r="H15" s="77"/>
-      <c r="I15" s="77"/>
-      <c r="J15" s="77"/>
-      <c r="K15" s="31"/>
-      <c r="L15" s="33"/>
+      <c r="H15" s="85"/>
+      <c r="I15" s="85"/>
+      <c r="J15" s="85"/>
+      <c r="K15" s="77"/>
+      <c r="L15" s="31"/>
       <c r="M15" s="33"/>
       <c r="N15" s="33"/>
       <c r="O15" s="33"/>
       <c r="P15" s="33"/>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="G16" s="77" t="s">
+      <c r="Q15" s="33"/>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="G16" s="85" t="s">
         <v>132</v>
       </c>
-      <c r="H16" s="77"/>
-      <c r="I16" s="77"/>
-      <c r="J16" s="77"/>
-      <c r="K16" s="31"/>
-      <c r="L16" s="33"/>
+      <c r="H16" s="85"/>
+      <c r="I16" s="85"/>
+      <c r="J16" s="85"/>
+      <c r="K16" s="77"/>
+      <c r="L16" s="31"/>
       <c r="M16" s="33"/>
       <c r="N16" s="33"/>
       <c r="O16" s="33"/>
       <c r="P16" s="33"/>
-    </row>
-    <row r="17" spans="7:16" x14ac:dyDescent="0.25">
-      <c r="G17" s="77" t="s">
+      <c r="Q16" s="33"/>
+    </row>
+    <row r="17" spans="7:17" x14ac:dyDescent="0.25">
+      <c r="G17" s="85" t="s">
         <v>133</v>
       </c>
-      <c r="H17" s="77"/>
-      <c r="I17" s="77"/>
-      <c r="J17" s="77"/>
-      <c r="K17" s="31"/>
-      <c r="L17" s="33"/>
+      <c r="H17" s="85"/>
+      <c r="I17" s="85"/>
+      <c r="J17" s="85"/>
+      <c r="K17" s="77"/>
+      <c r="L17" s="31"/>
       <c r="M17" s="33"/>
       <c r="N17" s="33"/>
       <c r="O17" s="33"/>
       <c r="P17" s="33"/>
-    </row>
-    <row r="18" spans="7:16" x14ac:dyDescent="0.25">
-      <c r="G18" s="77" t="s">
+      <c r="Q17" s="33"/>
+    </row>
+    <row r="18" spans="7:17" x14ac:dyDescent="0.25">
+      <c r="G18" s="85" t="s">
         <v>134</v>
       </c>
-      <c r="H18" s="77"/>
-      <c r="I18" s="77"/>
-      <c r="J18" s="77"/>
-      <c r="K18" s="31"/>
-      <c r="L18" s="33"/>
+      <c r="H18" s="85"/>
+      <c r="I18" s="85"/>
+      <c r="J18" s="85"/>
+      <c r="K18" s="77"/>
+      <c r="L18" s="31"/>
       <c r="M18" s="33"/>
       <c r="N18" s="33"/>
       <c r="O18" s="33"/>
       <c r="P18" s="33"/>
-    </row>
-    <row r="20" spans="7:16" x14ac:dyDescent="0.25">
-      <c r="G20" s="77" t="s">
+      <c r="Q18" s="33"/>
+    </row>
+    <row r="20" spans="7:17" x14ac:dyDescent="0.25">
+      <c r="G20" s="85" t="s">
         <v>135</v>
       </c>
-      <c r="H20" s="77"/>
-      <c r="I20" s="77"/>
-      <c r="J20" s="77"/>
-      <c r="K20" s="31"/>
-      <c r="L20" s="33"/>
+      <c r="H20" s="85"/>
+      <c r="I20" s="85"/>
+      <c r="J20" s="85"/>
+      <c r="K20" s="77"/>
+      <c r="L20" s="31"/>
       <c r="M20" s="33"/>
       <c r="N20" s="33"/>
       <c r="O20" s="33"/>
       <c r="P20" s="33"/>
-    </row>
-    <row r="21" spans="7:16" x14ac:dyDescent="0.25">
-      <c r="G21" s="77" t="s">
+      <c r="Q20" s="33"/>
+    </row>
+    <row r="21" spans="7:17" x14ac:dyDescent="0.25">
+      <c r="G21" s="85" t="s">
         <v>136</v>
       </c>
-      <c r="H21" s="77"/>
-      <c r="I21" s="77"/>
-      <c r="J21" s="77"/>
-      <c r="K21" s="31"/>
-      <c r="L21" s="33"/>
+      <c r="H21" s="85"/>
+      <c r="I21" s="85"/>
+      <c r="J21" s="85"/>
+      <c r="K21" s="77"/>
+      <c r="L21" s="31"/>
       <c r="M21" s="33"/>
       <c r="N21" s="33"/>
       <c r="O21" s="33"/>
       <c r="P21" s="33"/>
-    </row>
-    <row r="23" spans="7:16" x14ac:dyDescent="0.25">
+      <c r="Q21" s="33"/>
+    </row>
+    <row r="23" spans="7:17" x14ac:dyDescent="0.25">
       <c r="G23" s="26" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="24" spans="7:16" x14ac:dyDescent="0.25">
-      <c r="G24" s="77" t="s">
+    <row r="24" spans="7:17" x14ac:dyDescent="0.25">
+      <c r="G24" s="85" t="s">
         <v>137</v>
       </c>
-      <c r="H24" s="77"/>
-      <c r="I24" s="77"/>
-      <c r="J24" s="77"/>
-      <c r="K24" s="31"/>
-      <c r="L24" s="33"/>
+      <c r="H24" s="85"/>
+      <c r="I24" s="85"/>
+      <c r="J24" s="85"/>
+      <c r="K24" s="77"/>
+      <c r="L24" s="31"/>
       <c r="M24" s="33"/>
       <c r="N24" s="33"/>
       <c r="O24" s="33"/>
       <c r="P24" s="33"/>
-    </row>
-    <row r="25" spans="7:16" x14ac:dyDescent="0.25">
-      <c r="G25" s="77" t="s">
+      <c r="Q24" s="33"/>
+    </row>
+    <row r="25" spans="7:17" x14ac:dyDescent="0.25">
+      <c r="G25" s="85" t="s">
         <v>138</v>
       </c>
-      <c r="H25" s="77"/>
-      <c r="I25" s="77"/>
-      <c r="J25" s="77"/>
-      <c r="K25" s="31"/>
-      <c r="L25" s="33"/>
+      <c r="H25" s="85"/>
+      <c r="I25" s="85"/>
+      <c r="J25" s="85"/>
+      <c r="K25" s="77"/>
+      <c r="L25" s="31"/>
       <c r="M25" s="33"/>
       <c r="N25" s="33"/>
       <c r="O25" s="33"/>
       <c r="P25" s="33"/>
-    </row>
-    <row r="26" spans="7:16" x14ac:dyDescent="0.25">
-      <c r="G26" s="77" t="s">
+      <c r="Q25" s="33"/>
+    </row>
+    <row r="26" spans="7:17" x14ac:dyDescent="0.25">
+      <c r="G26" s="85" t="s">
         <v>140</v>
       </c>
-      <c r="H26" s="77"/>
-      <c r="I26" s="77"/>
-      <c r="J26" s="77"/>
-      <c r="K26" s="31"/>
-      <c r="L26" s="33"/>
+      <c r="H26" s="85"/>
+      <c r="I26" s="85"/>
+      <c r="J26" s="85"/>
+      <c r="K26" s="77"/>
+      <c r="L26" s="31"/>
       <c r="M26" s="33"/>
       <c r="N26" s="33"/>
       <c r="O26" s="33"/>
       <c r="P26" s="33"/>
+      <c r="Q26" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="C1:F1"/>
-    <mergeCell ref="G1:J1"/>
-    <mergeCell ref="M10:O10"/>
-    <mergeCell ref="G25:J25"/>
-    <mergeCell ref="L1:O1"/>
     <mergeCell ref="G26:J26"/>
     <mergeCell ref="C10:F10"/>
     <mergeCell ref="G10:J10"/>
@@ -4973,6 +5027,11 @@
     <mergeCell ref="G17:J17"/>
     <mergeCell ref="G18:J18"/>
     <mergeCell ref="G21:J21"/>
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="G1:J1"/>
+    <mergeCell ref="N10:P10"/>
+    <mergeCell ref="G25:J25"/>
+    <mergeCell ref="M1:P1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5111,7 +5170,7 @@
       <c r="A5" s="15" t="s">
         <v>103</v>
       </c>
-      <c r="B5" s="85">
+      <c r="B5" s="81">
         <v>1</v>
       </c>
       <c r="C5" s="44">
@@ -5687,7 +5746,7 @@
       <c r="B13" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="C13" s="84">
+      <c r="C13" s="80">
         <v>1</v>
       </c>
       <c r="D13" s="55">
@@ -6802,7 +6861,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="J17" sqref="J17"/>
     </sheetView>

</xml_diff>

<commit_message>
changed speed calculation -> needs further tweaking -> replace default fist values (hardcoded) with config ones -> slots must always be at least outfitted with fists!
</commit_message>
<xml_diff>
--- a/RDG/config/RDG.xlsx
+++ b/RDG/config/RDG.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="10725" windowHeight="8580" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="10725" windowHeight="8580" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="6" r:id="rId1"/>
@@ -1343,6 +1343,9 @@
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="1" fontId="2" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1351,9 +1354,6 @@
     </xf>
     <xf numFmtId="1" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="2" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1369,9 +1369,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="98">
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -3449,6 +3446,9 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
@@ -3769,28 +3769,28 @@
     <tableColumn id="10" uniqueName="hard" name="hard" dataDxfId="86">
       <xmlColumnPr mapId="80" xpath="/Rooms/Room/Monster/hard" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="18" uniqueName="Monster_Count" name="Monster_Count" dataDxfId="0">
+    <tableColumn id="18" uniqueName="Monster_Count" name="Monster_Count" dataDxfId="85">
       <xmlColumnPr mapId="80" xpath="/Rooms/Room/Monster_Count" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="11" uniqueName="Item_Multiplier" name="Item_Multiplier" dataDxfId="85">
+    <tableColumn id="11" uniqueName="Item_Multiplier" name="Item_Multiplier" dataDxfId="84">
       <xmlColumnPr mapId="80" xpath="/Rooms/Room/Item_Multiplier" xmlDataType="double"/>
     </tableColumn>
-    <tableColumn id="17" uniqueName="none" name="none" dataDxfId="84">
+    <tableColumn id="17" uniqueName="none" name="none" dataDxfId="83">
       <xmlColumnPr mapId="80" xpath="/Rooms/Room/Find_Probabilities/none" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="12" uniqueName="weak" name="weak" dataDxfId="83">
+    <tableColumn id="12" uniqueName="weak" name="weak" dataDxfId="82">
       <xmlColumnPr mapId="80" xpath="/Rooms/Room/Find_Probabilities/weak" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="13" uniqueName="medium" name="medium" dataDxfId="82">
+    <tableColumn id="13" uniqueName="medium" name="medium" dataDxfId="81">
       <xmlColumnPr mapId="80" xpath="/Rooms/Room/Find_Probabilities/medium" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="14" uniqueName="strong" name="strong" dataDxfId="81">
+    <tableColumn id="14" uniqueName="strong" name="strong" dataDxfId="80">
       <xmlColumnPr mapId="80" xpath="/Rooms/Room/Find_Probabilities/strong" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="15" uniqueName="Item_Count" name="Item_Count" dataDxfId="80">
+    <tableColumn id="15" uniqueName="Item_Count" name="Item_Count" dataDxfId="79">
       <xmlColumnPr mapId="80" xpath="/Rooms/Room/Item_Count" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="16" uniqueName="Image" name="Image" dataDxfId="79">
+    <tableColumn id="16" uniqueName="Image" name="Image" dataDxfId="78">
       <xmlColumnPr mapId="80" xpath="/Rooms/Room/Image" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
@@ -3799,31 +3799,31 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table8" displayName="Table8" ref="A1:H5" tableType="xml" totalsRowShown="0" headerRowDxfId="78" dataDxfId="76" headerRowBorderDxfId="77" tableBorderDxfId="75" connectionId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table8" displayName="Table8" ref="A1:H5" tableType="xml" totalsRowShown="0" headerRowDxfId="77" dataDxfId="75" headerRowBorderDxfId="76" tableBorderDxfId="74" connectionId="18">
   <autoFilter ref="A1:H5"/>
   <tableColumns count="8">
-    <tableColumn id="1" uniqueName="Name" name="Name" dataDxfId="74">
+    <tableColumn id="1" uniqueName="Name" name="Name" dataDxfId="73">
       <xmlColumnPr mapId="68" xpath="/Attacks/Attack/Name" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="8" uniqueName="Class_Multiplier" name="Class Multiplier" dataDxfId="73">
+    <tableColumn id="8" uniqueName="Class_Multiplier" name="Class Multiplier" dataDxfId="72">
       <xmlColumnPr mapId="68" xpath="/Attacks/Attack/Class_Multiplier" xmlDataType="double"/>
     </tableColumn>
-    <tableColumn id="6" uniqueName="Stats_Low_Multiplier" name="Stats Low Multiplier" dataDxfId="72">
+    <tableColumn id="6" uniqueName="Stats_Low_Multiplier" name="Stats Low Multiplier" dataDxfId="71">
       <xmlColumnPr mapId="68" xpath="/Attacks/Attack/Stats_Low_Multiplier" xmlDataType="double"/>
     </tableColumn>
-    <tableColumn id="7" uniqueName="Stats_High_Multiplier" name="Stats High Multiplier" dataDxfId="71">
+    <tableColumn id="7" uniqueName="Stats_High_Multiplier" name="Stats High Multiplier" dataDxfId="70">
       <xmlColumnPr mapId="68" xpath="/Attacks/Attack/Stats_High_Multiplier" xmlDataType="double"/>
     </tableColumn>
-    <tableColumn id="2" uniqueName="HP_Damage" name="HP Damage" dataDxfId="70">
+    <tableColumn id="2" uniqueName="HP_Damage" name="HP Damage" dataDxfId="69">
       <xmlColumnPr mapId="68" xpath="/Attacks/Attack/HP_Damage" xmlDataType="double"/>
     </tableColumn>
-    <tableColumn id="3" uniqueName="Hit_Probability" name="Hit Probability" dataDxfId="69">
+    <tableColumn id="3" uniqueName="Hit_Probability" name="Hit Probability" dataDxfId="68">
       <xmlColumnPr mapId="68" xpath="/Attacks/Attack/Hit_Probability" xmlDataType="double"/>
     </tableColumn>
-    <tableColumn id="4" uniqueName="Effect" name="Effect" dataDxfId="68">
+    <tableColumn id="4" uniqueName="Effect" name="Effect" dataDxfId="67">
       <xmlColumnPr mapId="68" xpath="/Attacks/Attack/Effect" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="5" uniqueName="x" name="x" dataDxfId="67">
+    <tableColumn id="5" uniqueName="x" name="x" dataDxfId="66">
       <xmlColumnPr mapId="68" xpath="/Attacks/Attack/x" xmlDataType="double"/>
     </tableColumn>
   </tableColumns>
@@ -3832,46 +3832,46 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="A1:M13" tableType="xml" totalsRowShown="0" headerRowDxfId="66" dataDxfId="64" headerRowBorderDxfId="65" tableBorderDxfId="63" connectionId="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="A1:M13" tableType="xml" totalsRowShown="0" headerRowDxfId="65" dataDxfId="63" headerRowBorderDxfId="64" tableBorderDxfId="62" connectionId="21">
   <autoFilter ref="A1:M13"/>
   <tableColumns count="13">
-    <tableColumn id="1" uniqueName="Name" name="Name" dataDxfId="62">
+    <tableColumn id="1" uniqueName="Name" name="Name" dataDxfId="61">
       <xmlColumnPr mapId="71" xpath="/Monsters/Monster/Name" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="2" uniqueName="Level" name="Level" dataDxfId="61">
+    <tableColumn id="2" uniqueName="Level" name="Level" dataDxfId="60">
       <xmlColumnPr mapId="71" xpath="/Monsters/Monster/Level" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="14" uniqueName="Class_Multiplier" name="Class Multiplier" dataDxfId="60">
+    <tableColumn id="14" uniqueName="Class_Multiplier" name="Class Multiplier" dataDxfId="59">
       <xmlColumnPr mapId="71" xpath="/Monsters/Monster/Class_Multiplier" xmlDataType="double"/>
     </tableColumn>
-    <tableColumn id="10" uniqueName="Stats_Low_Multiplier" name="Stats Low Multiplier" dataDxfId="59">
+    <tableColumn id="10" uniqueName="Stats_Low_Multiplier" name="Stats Low Multiplier" dataDxfId="58">
       <xmlColumnPr mapId="71" xpath="/Monsters/Monster/Stats_Low_Multiplier" xmlDataType="double"/>
     </tableColumn>
-    <tableColumn id="13" uniqueName="Stats_High_Multiplier" name="Stats High Multiplier" dataDxfId="58">
+    <tableColumn id="13" uniqueName="Stats_High_Multiplier" name="Stats High Multiplier" dataDxfId="57">
       <xmlColumnPr mapId="71" xpath="/Monsters/Monster/Stats_High_Multiplier" xmlDataType="double"/>
     </tableColumn>
-    <tableColumn id="3" uniqueName="HP" name="HP" dataDxfId="57">
+    <tableColumn id="3" uniqueName="HP" name="HP" dataDxfId="56">
       <xmlColumnPr mapId="71" xpath="/Monsters/Monster/HP" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="4" uniqueName="Strength" name="Strength" dataDxfId="56">
+    <tableColumn id="4" uniqueName="Strength" name="Strength" dataDxfId="55">
       <xmlColumnPr mapId="71" xpath="/Monsters/Monster/Strength" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="5" uniqueName="Speed" name="Speed" dataDxfId="55">
+    <tableColumn id="5" uniqueName="Speed" name="Speed" dataDxfId="54">
       <xmlColumnPr mapId="71" xpath="/Monsters/Monster/Speed" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="6" uniqueName="Accuracy" name="Accuracy" dataDxfId="54">
+    <tableColumn id="6" uniqueName="Accuracy" name="Accuracy" dataDxfId="53">
       <xmlColumnPr mapId="71" xpath="/Monsters/Monster/Accuracy" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="7" uniqueName="Kill_Bonus_Type" name="Kill Bonus Type" dataDxfId="53">
+    <tableColumn id="7" uniqueName="Kill_Bonus_Type" name="Kill Bonus Type" dataDxfId="52">
       <xmlColumnPr mapId="71" xpath="/Monsters/Monster/Kill_Bonus_Type" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="8" uniqueName="Kill_Bonus_Low" name="Kill Bonus Low" dataDxfId="52">
+    <tableColumn id="8" uniqueName="Kill_Bonus_Low" name="Kill Bonus Low" dataDxfId="51">
       <xmlColumnPr mapId="71" xpath="/Monsters/Monster/Kill_Bonus_Low" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="9" uniqueName="Kill_Bonus_High" name="Kill Bonus High" dataDxfId="51">
+    <tableColumn id="9" uniqueName="Kill_Bonus_High" name="Kill Bonus High" dataDxfId="50">
       <xmlColumnPr mapId="71" xpath="/Monsters/Monster/Kill_Bonus_High" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="11" uniqueName="Image" name="Image" dataDxfId="50">
+    <tableColumn id="11" uniqueName="Image" name="Image" dataDxfId="49">
       <xmlColumnPr mapId="71" xpath="/Monsters/Monster/Image" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
@@ -3880,37 +3880,37 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:J16" tableType="xml" totalsRowShown="0" headerRowDxfId="49" dataDxfId="47" headerRowBorderDxfId="48" tableBorderDxfId="46" totalsRowBorderDxfId="45" connectionId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:J16" tableType="xml" totalsRowShown="0" headerRowDxfId="48" dataDxfId="46" headerRowBorderDxfId="47" tableBorderDxfId="45" totalsRowBorderDxfId="44" connectionId="3">
   <autoFilter ref="A1:J16"/>
   <tableColumns count="10">
-    <tableColumn id="1" uniqueName="Name" name="Name" dataDxfId="44">
+    <tableColumn id="1" uniqueName="Name" name="Name" dataDxfId="43">
       <xmlColumnPr mapId="74" xpath="/Armaments/Armament/Name" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="9" uniqueName="Item_Class" name="Item Class" dataDxfId="43">
+    <tableColumn id="9" uniqueName="Item_Class" name="Item Class" dataDxfId="42">
       <xmlColumnPr mapId="74" xpath="/Armaments/Armament/Item_Class" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="10" uniqueName="Class_Multiplier" name="Class Multiplier" dataDxfId="42">
+    <tableColumn id="10" uniqueName="Class_Multiplier" name="Class Multiplier" dataDxfId="41">
       <xmlColumnPr mapId="74" xpath="/Armaments/Armament/Class_Multiplier" xmlDataType="double"/>
     </tableColumn>
-    <tableColumn id="6" uniqueName="Stats_Low_Multiplier" name="Stats Low Multiplier" dataDxfId="41">
+    <tableColumn id="6" uniqueName="Stats_Low_Multiplier" name="Stats Low Multiplier" dataDxfId="40">
       <xmlColumnPr mapId="74" xpath="/Armaments/Armament/Stats_Low_Multiplier" xmlDataType="double"/>
     </tableColumn>
-    <tableColumn id="11" uniqueName="Stats_High_Multiplier" name="Stats High Multiplier" dataDxfId="40">
+    <tableColumn id="11" uniqueName="Stats_High_Multiplier" name="Stats High Multiplier" dataDxfId="39">
       <xmlColumnPr mapId="74" xpath="/Armaments/Armament/Stats_High_Multiplier" xmlDataType="double"/>
     </tableColumn>
-    <tableColumn id="2" uniqueName="Armor" name="Armor" dataDxfId="39">
+    <tableColumn id="2" uniqueName="Armor" name="Armor" dataDxfId="38">
       <xmlColumnPr mapId="74" xpath="/Armaments/Armament/Armor" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="3" uniqueName="Speed" name="Speed" dataDxfId="38">
+    <tableColumn id="3" uniqueName="Speed" name="Speed" dataDxfId="37">
       <xmlColumnPr mapId="74" xpath="/Armaments/Armament/Speed" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="4" uniqueName="Type" name="Type" dataDxfId="37">
+    <tableColumn id="4" uniqueName="Type" name="Type" dataDxfId="36">
       <xmlColumnPr mapId="74" xpath="/Armaments/Armament/Type" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="5" uniqueName="Bonus" name="Bonus" dataDxfId="36">
+    <tableColumn id="5" uniqueName="Bonus" name="Bonus" dataDxfId="35">
       <xmlColumnPr mapId="74" xpath="/Armaments/Armament/Bonus" xmlDataType="double"/>
     </tableColumn>
-    <tableColumn id="7" uniqueName="Image" name="Image" dataDxfId="35">
+    <tableColumn id="7" uniqueName="Image" name="Image" dataDxfId="34">
       <xmlColumnPr mapId="74" xpath="/Armaments/Armament/Image" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
@@ -3919,43 +3919,43 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:L11" tableType="xml" totalsRowShown="0" headerRowDxfId="34" dataDxfId="32" headerRowBorderDxfId="33" tableBorderDxfId="31" totalsRowBorderDxfId="30" connectionId="32">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:L11" tableType="xml" totalsRowShown="0" headerRowDxfId="33" dataDxfId="31" headerRowBorderDxfId="32" tableBorderDxfId="30" totalsRowBorderDxfId="29" connectionId="32">
   <autoFilter ref="A1:L11"/>
   <tableColumns count="12">
-    <tableColumn id="1" uniqueName="Name" name="Name" dataDxfId="29">
+    <tableColumn id="1" uniqueName="Name" name="Name" dataDxfId="28">
       <xmlColumnPr mapId="75" xpath="/Potions/Potion/Name" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="10" uniqueName="Item_Class" name="Item Class" dataDxfId="28">
+    <tableColumn id="10" uniqueName="Item_Class" name="Item Class" dataDxfId="27">
       <xmlColumnPr mapId="75" xpath="/Potions/Potion/Item_Class" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="11" uniqueName="Class_Multiplier" name="Class Multiplier" dataDxfId="27">
+    <tableColumn id="11" uniqueName="Class_Multiplier" name="Class Multiplier" dataDxfId="26">
       <xmlColumnPr mapId="75" xpath="/Potions/Potion/Class_Multiplier" xmlDataType="double"/>
     </tableColumn>
-    <tableColumn id="12" uniqueName="Stats_Low_Multiplier" name="Stats Low Multiplier" dataDxfId="26">
+    <tableColumn id="12" uniqueName="Stats_Low_Multiplier" name="Stats Low Multiplier" dataDxfId="25">
       <xmlColumnPr mapId="75" xpath="/Potions/Potion/Stats_Low_Multiplier" xmlDataType="double"/>
     </tableColumn>
-    <tableColumn id="13" uniqueName="Stats_High_Multiplier" name="Stats High Multiplier" dataDxfId="25">
+    <tableColumn id="13" uniqueName="Stats_High_Multiplier" name="Stats High Multiplier" dataDxfId="24">
       <xmlColumnPr mapId="75" xpath="/Potions/Potion/Stats_High_Multiplier" xmlDataType="double"/>
     </tableColumn>
-    <tableColumn id="2" uniqueName="Description" name="Description" dataDxfId="24">
+    <tableColumn id="2" uniqueName="Description" name="Description" dataDxfId="23">
       <xmlColumnPr mapId="75" xpath="/Potions/Potion/Description" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="3" uniqueName="Target" name="Target" dataDxfId="23">
+    <tableColumn id="3" uniqueName="Target" name="Target" dataDxfId="22">
       <xmlColumnPr mapId="75" xpath="/Potions/Potion/Target" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="4" uniqueName="Effect" name="Effect" dataDxfId="22">
+    <tableColumn id="4" uniqueName="Effect" name="Effect" dataDxfId="21">
       <xmlColumnPr mapId="75" xpath="/Potions/Potion/Effect" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="5" uniqueName="Mode" name="Mode" dataDxfId="21">
+    <tableColumn id="5" uniqueName="Mode" name="Mode" dataDxfId="20">
       <xmlColumnPr mapId="75" xpath="/Potions/Potion/Mode" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="6" uniqueName="x" name="x" dataDxfId="20">
+    <tableColumn id="6" uniqueName="x" name="x" dataDxfId="19">
       <xmlColumnPr mapId="75" xpath="/Potions/Potion/x" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="7" uniqueName="n" name="n" dataDxfId="19">
+    <tableColumn id="7" uniqueName="n" name="n" dataDxfId="18">
       <xmlColumnPr mapId="75" xpath="/Potions/Potion/n" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="8" uniqueName="Image" name="Image" dataDxfId="18">
+    <tableColumn id="8" uniqueName="Image" name="Image" dataDxfId="17">
       <xmlColumnPr mapId="75" xpath="/Potions/Potion/Image" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
@@ -3964,47 +3964,47 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:M9" tableType="xml" totalsRowShown="0" headerRowDxfId="17" dataDxfId="15" headerRowBorderDxfId="16" tableBorderDxfId="14" connectionId="57">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:M9" tableType="xml" totalsRowShown="0" headerRowDxfId="16" dataDxfId="14" headerRowBorderDxfId="15" tableBorderDxfId="13" connectionId="57">
   <autoFilter ref="A1:M9"/>
   <tableColumns count="13">
-    <tableColumn id="1" uniqueName="Name" name="Name" dataDxfId="13">
+    <tableColumn id="1" uniqueName="Name" name="Name" dataDxfId="12">
       <xmlColumnPr mapId="76" xpath="/Weapons/Weapon/Name" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="11" uniqueName="Item_Class" name="Item Class" dataDxfId="12">
+    <tableColumn id="11" uniqueName="Item_Class" name="Item Class" dataDxfId="11">
       <xmlColumnPr mapId="76" xpath="/Weapons/Weapon/Item_Class" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="12" uniqueName="Class_Multiplier" name="Class Multiplier" dataDxfId="11">
+    <tableColumn id="12" uniqueName="Class_Multiplier" name="Class Multiplier" dataDxfId="10">
       <xmlColumnPr mapId="76" xpath="/Weapons/Weapon/Class_Multiplier" xmlDataType="double"/>
     </tableColumn>
-    <tableColumn id="13" uniqueName="Stats_Low_Multiplier" name="Stats Low Multiplier" dataDxfId="10">
+    <tableColumn id="13" uniqueName="Stats_Low_Multiplier" name="Stats Low Multiplier" dataDxfId="9">
       <xmlColumnPr mapId="76" xpath="/Weapons/Weapon/Stats_Low_Multiplier" xmlDataType="double"/>
     </tableColumn>
-    <tableColumn id="14" uniqueName="Stats_High_Multiplier" name="Stats High Multiplier" dataDxfId="9">
+    <tableColumn id="14" uniqueName="Stats_High_Multiplier" name="Stats High Multiplier" dataDxfId="8">
       <xmlColumnPr mapId="76" xpath="/Weapons/Weapon/Stats_High_Multiplier" xmlDataType="double"/>
     </tableColumn>
-    <tableColumn id="2" uniqueName="Attack" name="Attack" dataDxfId="8">
+    <tableColumn id="2" uniqueName="Attack" name="Attack" dataDxfId="7">
       <xmlColumnPr mapId="76" xpath="/Weapons/Weapon/Attack" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="3" uniqueName="Speed" name="Speed" dataDxfId="7">
+    <tableColumn id="3" uniqueName="Speed" name="Speed" dataDxfId="6">
       <xmlColumnPr mapId="76" xpath="/Weapons/Weapon/Speed" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="4" uniqueName="Accuracy" name="Accuracy" dataDxfId="6">
+    <tableColumn id="4" uniqueName="Accuracy" name="Accuracy" dataDxfId="5">
       <xmlColumnPr mapId="76" xpath="/Weapons/Weapon/Accuracy" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="5" uniqueName="Defence" name="Defence" dataDxfId="5">
+    <tableColumn id="5" uniqueName="Defence" name="Defence" dataDxfId="4">
       <calculatedColumnFormula>"-"</calculatedColumnFormula>
       <xmlColumnPr mapId="76" xpath="/Weapons/Weapon/Defence" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="6" uniqueName="Slots" name="Slots" dataDxfId="4">
+    <tableColumn id="6" uniqueName="Slots" name="Slots" dataDxfId="3">
       <xmlColumnPr mapId="76" xpath="/Weapons/Weapon/Slots" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="7" uniqueName="Max" name="Max" dataDxfId="3">
+    <tableColumn id="7" uniqueName="Max" name="Max" dataDxfId="2">
       <xmlColumnPr mapId="76" xpath="/Weapons/Weapon/Max" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="8" uniqueName="Type" name="Type" dataDxfId="2">
+    <tableColumn id="8" uniqueName="Type" name="Type" dataDxfId="1">
       <xmlColumnPr mapId="76" xpath="/Weapons/Weapon/Type" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="9" uniqueName="Image" name="Image" dataDxfId="1">
+    <tableColumn id="9" uniqueName="Image" name="Image" dataDxfId="0">
       <xmlColumnPr mapId="76" xpath="/Weapons/Weapon/Image" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
@@ -4331,7 +4331,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="Q31" sqref="Q31"/>
     </sheetView>
@@ -4361,18 +4361,18 @@
     <row r="1" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="22"/>
       <c r="B1" s="22"/>
-      <c r="C1" s="82" t="s">
+      <c r="C1" s="83" t="s">
         <v>123</v>
       </c>
-      <c r="D1" s="83"/>
-      <c r="E1" s="83"/>
-      <c r="F1" s="84"/>
-      <c r="G1" s="82" t="s">
+      <c r="D1" s="84"/>
+      <c r="E1" s="84"/>
+      <c r="F1" s="85"/>
+      <c r="G1" s="83" t="s">
         <v>120</v>
       </c>
-      <c r="H1" s="83"/>
-      <c r="I1" s="83"/>
-      <c r="J1" s="84"/>
+      <c r="H1" s="84"/>
+      <c r="I1" s="84"/>
+      <c r="J1" s="85"/>
       <c r="K1" s="79"/>
       <c r="L1" s="29"/>
       <c r="M1" s="86" t="s">
@@ -4780,26 +4780,26 @@
       <c r="A10" s="21" t="s">
         <v>144</v>
       </c>
-      <c r="C10" s="85" t="s">
+      <c r="C10" s="82" t="s">
         <v>129</v>
       </c>
-      <c r="D10" s="85"/>
-      <c r="E10" s="85"/>
-      <c r="F10" s="85"/>
-      <c r="G10" s="85" t="s">
+      <c r="D10" s="82"/>
+      <c r="E10" s="82"/>
+      <c r="F10" s="82"/>
+      <c r="G10" s="82" t="s">
         <v>128</v>
       </c>
-      <c r="H10" s="85"/>
-      <c r="I10" s="85"/>
-      <c r="J10" s="85"/>
+      <c r="H10" s="82"/>
+      <c r="I10" s="82"/>
+      <c r="J10" s="82"/>
       <c r="K10" s="77"/>
       <c r="L10" s="31"/>
       <c r="M10" s="33"/>
-      <c r="N10" s="85" t="s">
+      <c r="N10" s="82" t="s">
         <v>153</v>
       </c>
-      <c r="O10" s="85"/>
-      <c r="P10" s="85"/>
+      <c r="O10" s="82"/>
+      <c r="P10" s="82"/>
       <c r="Q10" s="33"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
@@ -4857,12 +4857,12 @@
       <c r="Q13" s="34"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="G14" s="85" t="s">
+      <c r="G14" s="82" t="s">
         <v>130</v>
       </c>
-      <c r="H14" s="85"/>
-      <c r="I14" s="85"/>
-      <c r="J14" s="85"/>
+      <c r="H14" s="82"/>
+      <c r="I14" s="82"/>
+      <c r="J14" s="82"/>
       <c r="K14" s="77"/>
       <c r="L14" s="31"/>
       <c r="M14" s="33"/>
@@ -4875,12 +4875,12 @@
       <c r="A15" s="21" t="s">
         <v>143</v>
       </c>
-      <c r="G15" s="85" t="s">
+      <c r="G15" s="82" t="s">
         <v>131</v>
       </c>
-      <c r="H15" s="85"/>
-      <c r="I15" s="85"/>
-      <c r="J15" s="85"/>
+      <c r="H15" s="82"/>
+      <c r="I15" s="82"/>
+      <c r="J15" s="82"/>
       <c r="K15" s="77"/>
       <c r="L15" s="31"/>
       <c r="M15" s="33"/>
@@ -4890,12 +4890,12 @@
       <c r="Q15" s="33"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="G16" s="85" t="s">
+      <c r="G16" s="82" t="s">
         <v>132</v>
       </c>
-      <c r="H16" s="85"/>
-      <c r="I16" s="85"/>
-      <c r="J16" s="85"/>
+      <c r="H16" s="82"/>
+      <c r="I16" s="82"/>
+      <c r="J16" s="82"/>
       <c r="K16" s="77"/>
       <c r="L16" s="31"/>
       <c r="M16" s="33"/>
@@ -4905,12 +4905,12 @@
       <c r="Q16" s="33"/>
     </row>
     <row r="17" spans="7:17" x14ac:dyDescent="0.25">
-      <c r="G17" s="85" t="s">
+      <c r="G17" s="82" t="s">
         <v>133</v>
       </c>
-      <c r="H17" s="85"/>
-      <c r="I17" s="85"/>
-      <c r="J17" s="85"/>
+      <c r="H17" s="82"/>
+      <c r="I17" s="82"/>
+      <c r="J17" s="82"/>
       <c r="K17" s="77"/>
       <c r="L17" s="31"/>
       <c r="M17" s="33"/>
@@ -4920,12 +4920,12 @@
       <c r="Q17" s="33"/>
     </row>
     <row r="18" spans="7:17" x14ac:dyDescent="0.25">
-      <c r="G18" s="85" t="s">
+      <c r="G18" s="82" t="s">
         <v>134</v>
       </c>
-      <c r="H18" s="85"/>
-      <c r="I18" s="85"/>
-      <c r="J18" s="85"/>
+      <c r="H18" s="82"/>
+      <c r="I18" s="82"/>
+      <c r="J18" s="82"/>
       <c r="K18" s="77"/>
       <c r="L18" s="31"/>
       <c r="M18" s="33"/>
@@ -4935,12 +4935,12 @@
       <c r="Q18" s="33"/>
     </row>
     <row r="20" spans="7:17" x14ac:dyDescent="0.25">
-      <c r="G20" s="85" t="s">
+      <c r="G20" s="82" t="s">
         <v>135</v>
       </c>
-      <c r="H20" s="85"/>
-      <c r="I20" s="85"/>
-      <c r="J20" s="85"/>
+      <c r="H20" s="82"/>
+      <c r="I20" s="82"/>
+      <c r="J20" s="82"/>
       <c r="K20" s="77"/>
       <c r="L20" s="31"/>
       <c r="M20" s="33"/>
@@ -4950,12 +4950,12 @@
       <c r="Q20" s="33"/>
     </row>
     <row r="21" spans="7:17" x14ac:dyDescent="0.25">
-      <c r="G21" s="85" t="s">
+      <c r="G21" s="82" t="s">
         <v>136</v>
       </c>
-      <c r="H21" s="85"/>
-      <c r="I21" s="85"/>
-      <c r="J21" s="85"/>
+      <c r="H21" s="82"/>
+      <c r="I21" s="82"/>
+      <c r="J21" s="82"/>
       <c r="K21" s="77"/>
       <c r="L21" s="31"/>
       <c r="M21" s="33"/>
@@ -4970,12 +4970,12 @@
       </c>
     </row>
     <row r="24" spans="7:17" x14ac:dyDescent="0.25">
-      <c r="G24" s="85" t="s">
+      <c r="G24" s="82" t="s">
         <v>137</v>
       </c>
-      <c r="H24" s="85"/>
-      <c r="I24" s="85"/>
-      <c r="J24" s="85"/>
+      <c r="H24" s="82"/>
+      <c r="I24" s="82"/>
+      <c r="J24" s="82"/>
       <c r="K24" s="77"/>
       <c r="L24" s="31"/>
       <c r="M24" s="33"/>
@@ -4985,12 +4985,12 @@
       <c r="Q24" s="33"/>
     </row>
     <row r="25" spans="7:17" x14ac:dyDescent="0.25">
-      <c r="G25" s="85" t="s">
+      <c r="G25" s="82" t="s">
         <v>138</v>
       </c>
-      <c r="H25" s="85"/>
-      <c r="I25" s="85"/>
-      <c r="J25" s="85"/>
+      <c r="H25" s="82"/>
+      <c r="I25" s="82"/>
+      <c r="J25" s="82"/>
       <c r="K25" s="77"/>
       <c r="L25" s="31"/>
       <c r="M25" s="33"/>
@@ -5000,12 +5000,12 @@
       <c r="Q25" s="33"/>
     </row>
     <row r="26" spans="7:17" x14ac:dyDescent="0.25">
-      <c r="G26" s="85" t="s">
+      <c r="G26" s="82" t="s">
         <v>140</v>
       </c>
-      <c r="H26" s="85"/>
-      <c r="I26" s="85"/>
-      <c r="J26" s="85"/>
+      <c r="H26" s="82"/>
+      <c r="I26" s="82"/>
+      <c r="J26" s="82"/>
       <c r="K26" s="77"/>
       <c r="L26" s="31"/>
       <c r="M26" s="33"/>
@@ -5016,6 +5016,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="G1:J1"/>
+    <mergeCell ref="N10:P10"/>
+    <mergeCell ref="G25:J25"/>
+    <mergeCell ref="M1:P1"/>
     <mergeCell ref="G26:J26"/>
     <mergeCell ref="C10:F10"/>
     <mergeCell ref="G10:J10"/>
@@ -5027,11 +5032,6 @@
     <mergeCell ref="G17:J17"/>
     <mergeCell ref="G18:J18"/>
     <mergeCell ref="G21:J21"/>
-    <mergeCell ref="C1:F1"/>
-    <mergeCell ref="G1:J1"/>
-    <mergeCell ref="N10:P10"/>
-    <mergeCell ref="G25:J25"/>
-    <mergeCell ref="M1:P1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -6861,9 +6861,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="J17" sqref="J17"/>
+      <selection pane="topRight" activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7106,10 +7106,10 @@
         <v>0</v>
       </c>
       <c r="G6" s="68">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="H6" s="68">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="I6" s="68">
         <v>50</v>

</xml_diff>

<commit_message>
implemented fight class but not yet working
</commit_message>
<xml_diff>
--- a/RDG/config/RDG.xlsx
+++ b/RDG/config/RDG.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="10725" windowHeight="8580" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="10725" windowHeight="8580" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="6" r:id="rId1"/>
@@ -1343,17 +1343,17 @@
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="2" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="2" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -4361,18 +4361,18 @@
     <row r="1" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="22"/>
       <c r="B1" s="22"/>
-      <c r="C1" s="83" t="s">
+      <c r="C1" s="82" t="s">
         <v>123</v>
       </c>
-      <c r="D1" s="84"/>
-      <c r="E1" s="84"/>
-      <c r="F1" s="85"/>
-      <c r="G1" s="83" t="s">
+      <c r="D1" s="83"/>
+      <c r="E1" s="83"/>
+      <c r="F1" s="84"/>
+      <c r="G1" s="82" t="s">
         <v>120</v>
       </c>
-      <c r="H1" s="84"/>
-      <c r="I1" s="84"/>
-      <c r="J1" s="85"/>
+      <c r="H1" s="83"/>
+      <c r="I1" s="83"/>
+      <c r="J1" s="84"/>
       <c r="K1" s="79"/>
       <c r="L1" s="29"/>
       <c r="M1" s="86" t="s">
@@ -4780,26 +4780,26 @@
       <c r="A10" s="21" t="s">
         <v>144</v>
       </c>
-      <c r="C10" s="82" t="s">
+      <c r="C10" s="85" t="s">
         <v>129</v>
       </c>
-      <c r="D10" s="82"/>
-      <c r="E10" s="82"/>
-      <c r="F10" s="82"/>
-      <c r="G10" s="82" t="s">
+      <c r="D10" s="85"/>
+      <c r="E10" s="85"/>
+      <c r="F10" s="85"/>
+      <c r="G10" s="85" t="s">
         <v>128</v>
       </c>
-      <c r="H10" s="82"/>
-      <c r="I10" s="82"/>
-      <c r="J10" s="82"/>
+      <c r="H10" s="85"/>
+      <c r="I10" s="85"/>
+      <c r="J10" s="85"/>
       <c r="K10" s="77"/>
       <c r="L10" s="31"/>
       <c r="M10" s="33"/>
-      <c r="N10" s="82" t="s">
+      <c r="N10" s="85" t="s">
         <v>153</v>
       </c>
-      <c r="O10" s="82"/>
-      <c r="P10" s="82"/>
+      <c r="O10" s="85"/>
+      <c r="P10" s="85"/>
       <c r="Q10" s="33"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
@@ -4857,12 +4857,12 @@
       <c r="Q13" s="34"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="G14" s="82" t="s">
+      <c r="G14" s="85" t="s">
         <v>130</v>
       </c>
-      <c r="H14" s="82"/>
-      <c r="I14" s="82"/>
-      <c r="J14" s="82"/>
+      <c r="H14" s="85"/>
+      <c r="I14" s="85"/>
+      <c r="J14" s="85"/>
       <c r="K14" s="77"/>
       <c r="L14" s="31"/>
       <c r="M14" s="33"/>
@@ -4875,12 +4875,12 @@
       <c r="A15" s="21" t="s">
         <v>143</v>
       </c>
-      <c r="G15" s="82" t="s">
+      <c r="G15" s="85" t="s">
         <v>131</v>
       </c>
-      <c r="H15" s="82"/>
-      <c r="I15" s="82"/>
-      <c r="J15" s="82"/>
+      <c r="H15" s="85"/>
+      <c r="I15" s="85"/>
+      <c r="J15" s="85"/>
       <c r="K15" s="77"/>
       <c r="L15" s="31"/>
       <c r="M15" s="33"/>
@@ -4890,12 +4890,12 @@
       <c r="Q15" s="33"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="G16" s="82" t="s">
+      <c r="G16" s="85" t="s">
         <v>132</v>
       </c>
-      <c r="H16" s="82"/>
-      <c r="I16" s="82"/>
-      <c r="J16" s="82"/>
+      <c r="H16" s="85"/>
+      <c r="I16" s="85"/>
+      <c r="J16" s="85"/>
       <c r="K16" s="77"/>
       <c r="L16" s="31"/>
       <c r="M16" s="33"/>
@@ -4905,12 +4905,12 @@
       <c r="Q16" s="33"/>
     </row>
     <row r="17" spans="7:17" x14ac:dyDescent="0.25">
-      <c r="G17" s="82" t="s">
+      <c r="G17" s="85" t="s">
         <v>133</v>
       </c>
-      <c r="H17" s="82"/>
-      <c r="I17" s="82"/>
-      <c r="J17" s="82"/>
+      <c r="H17" s="85"/>
+      <c r="I17" s="85"/>
+      <c r="J17" s="85"/>
       <c r="K17" s="77"/>
       <c r="L17" s="31"/>
       <c r="M17" s="33"/>
@@ -4920,12 +4920,12 @@
       <c r="Q17" s="33"/>
     </row>
     <row r="18" spans="7:17" x14ac:dyDescent="0.25">
-      <c r="G18" s="82" t="s">
+      <c r="G18" s="85" t="s">
         <v>134</v>
       </c>
-      <c r="H18" s="82"/>
-      <c r="I18" s="82"/>
-      <c r="J18" s="82"/>
+      <c r="H18" s="85"/>
+      <c r="I18" s="85"/>
+      <c r="J18" s="85"/>
       <c r="K18" s="77"/>
       <c r="L18" s="31"/>
       <c r="M18" s="33"/>
@@ -4935,12 +4935,12 @@
       <c r="Q18" s="33"/>
     </row>
     <row r="20" spans="7:17" x14ac:dyDescent="0.25">
-      <c r="G20" s="82" t="s">
+      <c r="G20" s="85" t="s">
         <v>135</v>
       </c>
-      <c r="H20" s="82"/>
-      <c r="I20" s="82"/>
-      <c r="J20" s="82"/>
+      <c r="H20" s="85"/>
+      <c r="I20" s="85"/>
+      <c r="J20" s="85"/>
       <c r="K20" s="77"/>
       <c r="L20" s="31"/>
       <c r="M20" s="33"/>
@@ -4950,12 +4950,12 @@
       <c r="Q20" s="33"/>
     </row>
     <row r="21" spans="7:17" x14ac:dyDescent="0.25">
-      <c r="G21" s="82" t="s">
+      <c r="G21" s="85" t="s">
         <v>136</v>
       </c>
-      <c r="H21" s="82"/>
-      <c r="I21" s="82"/>
-      <c r="J21" s="82"/>
+      <c r="H21" s="85"/>
+      <c r="I21" s="85"/>
+      <c r="J21" s="85"/>
       <c r="K21" s="77"/>
       <c r="L21" s="31"/>
       <c r="M21" s="33"/>
@@ -4970,12 +4970,12 @@
       </c>
     </row>
     <row r="24" spans="7:17" x14ac:dyDescent="0.25">
-      <c r="G24" s="82" t="s">
+      <c r="G24" s="85" t="s">
         <v>137</v>
       </c>
-      <c r="H24" s="82"/>
-      <c r="I24" s="82"/>
-      <c r="J24" s="82"/>
+      <c r="H24" s="85"/>
+      <c r="I24" s="85"/>
+      <c r="J24" s="85"/>
       <c r="K24" s="77"/>
       <c r="L24" s="31"/>
       <c r="M24" s="33"/>
@@ -4985,12 +4985,12 @@
       <c r="Q24" s="33"/>
     </row>
     <row r="25" spans="7:17" x14ac:dyDescent="0.25">
-      <c r="G25" s="82" t="s">
+      <c r="G25" s="85" t="s">
         <v>138</v>
       </c>
-      <c r="H25" s="82"/>
-      <c r="I25" s="82"/>
-      <c r="J25" s="82"/>
+      <c r="H25" s="85"/>
+      <c r="I25" s="85"/>
+      <c r="J25" s="85"/>
       <c r="K25" s="77"/>
       <c r="L25" s="31"/>
       <c r="M25" s="33"/>
@@ -5000,12 +5000,12 @@
       <c r="Q25" s="33"/>
     </row>
     <row r="26" spans="7:17" x14ac:dyDescent="0.25">
-      <c r="G26" s="82" t="s">
+      <c r="G26" s="85" t="s">
         <v>140</v>
       </c>
-      <c r="H26" s="82"/>
-      <c r="I26" s="82"/>
-      <c r="J26" s="82"/>
+      <c r="H26" s="85"/>
+      <c r="I26" s="85"/>
+      <c r="J26" s="85"/>
       <c r="K26" s="77"/>
       <c r="L26" s="31"/>
       <c r="M26" s="33"/>
@@ -5016,11 +5016,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="C1:F1"/>
-    <mergeCell ref="G1:J1"/>
-    <mergeCell ref="N10:P10"/>
-    <mergeCell ref="G25:J25"/>
-    <mergeCell ref="M1:P1"/>
     <mergeCell ref="G26:J26"/>
     <mergeCell ref="C10:F10"/>
     <mergeCell ref="G10:J10"/>
@@ -5032,6 +5027,11 @@
     <mergeCell ref="G17:J17"/>
     <mergeCell ref="G18:J18"/>
     <mergeCell ref="G21:J21"/>
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="G1:J1"/>
+    <mergeCell ref="N10:P10"/>
+    <mergeCell ref="G25:J25"/>
+    <mergeCell ref="M1:P1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5045,9 +5045,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G12" sqref="G12"/>
+      <selection pane="topRight" activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5096,10 +5096,10 @@
         <v>1</v>
       </c>
       <c r="C2" s="44">
-        <v>0.8</v>
+        <v>0.75</v>
       </c>
       <c r="D2" s="44">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="E2" s="44">
         <v>0.5</v>
@@ -5122,10 +5122,10 @@
         <v>1</v>
       </c>
       <c r="C3" s="44">
-        <v>0.8</v>
+        <v>0.75</v>
       </c>
       <c r="D3" s="45">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="E3" s="45">
         <v>0.7</v>
@@ -5148,10 +5148,10 @@
         <v>1</v>
       </c>
       <c r="C4" s="44">
-        <v>0.8</v>
+        <v>0.75</v>
       </c>
       <c r="D4" s="44">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="E4" s="45">
         <v>0.3</v>
@@ -5174,10 +5174,10 @@
         <v>1</v>
       </c>
       <c r="C5" s="44">
-        <v>0.8</v>
+        <v>0.75</v>
       </c>
       <c r="D5" s="45">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="E5" s="46">
         <v>0.4</v>
@@ -6861,7 +6861,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="I18" sqref="I18"/>
     </sheetView>

</xml_diff>

<commit_message>
changed players movement, implemented minimap with drag n drop function, started implementation of mouseover infotext
</commit_message>
<xml_diff>
--- a/RDG/config/RDG.xlsx
+++ b/RDG/config/RDG.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="10725" windowHeight="8580" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="12420" windowHeight="4245" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="6" r:id="rId1"/>
@@ -15,7 +15,7 @@
     <sheet name="Potions" sheetId="5" r:id="rId6"/>
     <sheet name="Weapons" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -315,36 +315,9 @@
     <t>Slowness</t>
   </si>
   <si>
-    <t>fills x HP immediatly</t>
-  </si>
-  <si>
-    <t>regenerates x HP over n rounds</t>
-  </si>
-  <si>
     <t>reverses poison effect</t>
   </si>
   <si>
-    <t>increases strength by x for n rounds</t>
-  </si>
-  <si>
-    <t>increases speed by x for n rounds</t>
-  </si>
-  <si>
-    <t>increases accuracy by x for n rounds</t>
-  </si>
-  <si>
-    <t>decreases accuracy by x for n rounds</t>
-  </si>
-  <si>
-    <t>descreases speed by x for n rounds</t>
-  </si>
-  <si>
-    <t>deals x damage for n rounds</t>
-  </si>
-  <si>
-    <t>decreases strength by x for n rounds</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
@@ -856,13 +829,40 @@
   </si>
   <si>
     <t>Monster_Count</t>
+  </si>
+  <si>
+    <t>fills xxx HP immediatly</t>
+  </si>
+  <si>
+    <t>regenerates xxx HP over nnn rounds</t>
+  </si>
+  <si>
+    <t>increases strength by xxx for nnn rounds</t>
+  </si>
+  <si>
+    <t>increases speed by xxx for nnn rounds</t>
+  </si>
+  <si>
+    <t>increases accuracy by xxx for nnn rounds</t>
+  </si>
+  <si>
+    <t>decreases accuracy by xxx for nnn rounds</t>
+  </si>
+  <si>
+    <t>descreases speed by xxx for nnn rounds</t>
+  </si>
+  <si>
+    <t>deals xxx damage for nnn rounds</t>
+  </si>
+  <si>
+    <t>decreases strength by xxx for nnn rounds</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1366,12 +1366,9 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="98">
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1389,7 +1386,7 @@
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right/>
@@ -1418,7 +1415,7 @@
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right/>
@@ -1447,7 +1444,7 @@
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="1" formatCode="0"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right/>
@@ -1476,7 +1473,7 @@
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="1" formatCode="0"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right/>
@@ -1505,7 +1502,7 @@
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="1" formatCode="0"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right/>
@@ -1534,7 +1531,7 @@
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="1" formatCode="0"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right/>
@@ -1563,7 +1560,7 @@
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="1" formatCode="0"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right/>
@@ -1592,7 +1589,7 @@
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="1" formatCode="0"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right/>
@@ -1621,7 +1618,7 @@
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right/>
@@ -1652,7 +1649,7 @@
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right/>
@@ -1683,7 +1680,7 @@
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right/>
@@ -1712,7 +1709,7 @@
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right/>
@@ -1741,7 +1738,7 @@
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right/>
@@ -1785,7 +1782,7 @@
         <name val="Verdana"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <border outline="0">
@@ -1816,7 +1813,7 @@
           <bgColor rgb="FFFF6600"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1841,7 +1838,7 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right/>
@@ -1876,7 +1873,7 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right/>
@@ -1911,7 +1908,7 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right/>
@@ -1946,7 +1943,7 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right/>
@@ -1981,7 +1978,7 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right/>
@@ -2016,7 +2013,7 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right/>
@@ -2051,7 +2048,7 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right/>
@@ -2086,7 +2083,7 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right/>
@@ -2121,7 +2118,7 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right/>
@@ -2158,7 +2155,7 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right/>
@@ -2193,7 +2190,7 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right/>
@@ -2228,7 +2225,7 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right/>
@@ -2285,7 +2282,7 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <border outline="0">
@@ -2316,7 +2313,7 @@
           <bgColor rgb="FFFF6600"/>
         </patternFill>
       </fill>
-      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -2335,7 +2332,7 @@
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right/>
@@ -2364,7 +2361,7 @@
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right/>
@@ -2393,7 +2390,7 @@
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right/>
@@ -2422,7 +2419,7 @@
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="1" formatCode="0"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right/>
@@ -2451,7 +2448,7 @@
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="1" formatCode="0"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right/>
@@ -2482,7 +2479,7 @@
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right/>
@@ -2513,7 +2510,7 @@
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right/>
@@ -2544,7 +2541,7 @@
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right/>
@@ -2573,7 +2570,7 @@
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right/>
@@ -2602,7 +2599,7 @@
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right/>
@@ -2653,7 +2650,7 @@
         <name val="Verdana"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <border outline="0">
@@ -2684,7 +2681,7 @@
           <bgColor rgb="FFFF6600"/>
         </patternFill>
       </fill>
-      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -2703,7 +2700,7 @@
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right/>
@@ -2732,7 +2729,7 @@
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="1" formatCode="0"/>
-      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right/>
@@ -2761,7 +2758,7 @@
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="1" formatCode="0"/>
-      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right/>
@@ -2790,7 +2787,7 @@
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right/>
@@ -2817,7 +2814,7 @@
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="1" formatCode="0"/>
-      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right/>
@@ -2844,7 +2841,7 @@
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="1" formatCode="0"/>
-      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right/>
@@ -2873,7 +2870,7 @@
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="1" formatCode="0"/>
-      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right/>
@@ -2902,7 +2899,7 @@
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="1" formatCode="0"/>
-      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right/>
@@ -2931,7 +2928,7 @@
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right/>
@@ -2962,7 +2959,7 @@
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right/>
@@ -2993,7 +2990,7 @@
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right/>
@@ -3022,7 +3019,7 @@
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right/>
@@ -3051,7 +3048,7 @@
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right/>
@@ -3095,7 +3092,7 @@
         <name val="Verdana"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <border outline="0">
@@ -3126,7 +3123,7 @@
           <bgColor rgb="FFFF6600"/>
         </patternFill>
       </fill>
-      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -3145,7 +3142,7 @@
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right/>
@@ -3176,7 +3173,7 @@
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right/>
@@ -3205,7 +3202,7 @@
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right/>
@@ -3234,7 +3231,7 @@
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right/>
@@ -3265,7 +3262,7 @@
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right/>
@@ -3296,7 +3293,7 @@
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right/>
@@ -3325,7 +3322,7 @@
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right/>
@@ -3352,7 +3349,7 @@
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right/>
@@ -3396,7 +3393,7 @@
         <name val="Verdana"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <border outline="0">
@@ -3427,7 +3424,7 @@
           <bgColor rgb="FFFF6600"/>
         </patternFill>
       </fill>
-      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -3449,6 +3446,9 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
@@ -3509,7 +3509,7 @@
           <bgColor rgb="FFFF6600"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -3769,28 +3769,28 @@
     <tableColumn id="10" uniqueName="hard" name="hard" dataDxfId="86">
       <xmlColumnPr mapId="80" xpath="/Rooms/Room/Monster/hard" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="18" uniqueName="Monster_Count" name="Monster_Count" dataDxfId="0">
+    <tableColumn id="18" uniqueName="Monster_Count" name="Monster_Count" dataDxfId="85">
       <xmlColumnPr mapId="80" xpath="/Rooms/Room/Monster_Count" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="11" uniqueName="Item_Multiplier" name="Item_Multiplier" dataDxfId="85">
+    <tableColumn id="11" uniqueName="Item_Multiplier" name="Item_Multiplier" dataDxfId="84">
       <xmlColumnPr mapId="80" xpath="/Rooms/Room/Item_Multiplier" xmlDataType="double"/>
     </tableColumn>
-    <tableColumn id="17" uniqueName="none" name="none" dataDxfId="84">
+    <tableColumn id="17" uniqueName="none" name="none" dataDxfId="83">
       <xmlColumnPr mapId="80" xpath="/Rooms/Room/Find_Probabilities/none" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="12" uniqueName="weak" name="weak" dataDxfId="83">
+    <tableColumn id="12" uniqueName="weak" name="weak" dataDxfId="82">
       <xmlColumnPr mapId="80" xpath="/Rooms/Room/Find_Probabilities/weak" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="13" uniqueName="medium" name="medium" dataDxfId="82">
+    <tableColumn id="13" uniqueName="medium" name="medium" dataDxfId="81">
       <xmlColumnPr mapId="80" xpath="/Rooms/Room/Find_Probabilities/medium" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="14" uniqueName="strong" name="strong" dataDxfId="81">
+    <tableColumn id="14" uniqueName="strong" name="strong" dataDxfId="80">
       <xmlColumnPr mapId="80" xpath="/Rooms/Room/Find_Probabilities/strong" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="15" uniqueName="Item_Count" name="Item_Count" dataDxfId="80">
+    <tableColumn id="15" uniqueName="Item_Count" name="Item_Count" dataDxfId="79">
       <xmlColumnPr mapId="80" xpath="/Rooms/Room/Item_Count" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="16" uniqueName="Image" name="Image" dataDxfId="79">
+    <tableColumn id="16" uniqueName="Image" name="Image" dataDxfId="78">
       <xmlColumnPr mapId="80" xpath="/Rooms/Room/Image" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
@@ -3799,31 +3799,31 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table8" displayName="Table8" ref="A1:H5" tableType="xml" totalsRowShown="0" headerRowDxfId="78" dataDxfId="76" headerRowBorderDxfId="77" tableBorderDxfId="75" connectionId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table8" displayName="Table8" ref="A1:H5" tableType="xml" totalsRowShown="0" headerRowDxfId="77" dataDxfId="75" headerRowBorderDxfId="76" tableBorderDxfId="74" connectionId="18">
   <autoFilter ref="A1:H5"/>
   <tableColumns count="8">
-    <tableColumn id="1" uniqueName="Name" name="Name" dataDxfId="74">
+    <tableColumn id="1" uniqueName="Name" name="Name" dataDxfId="73">
       <xmlColumnPr mapId="68" xpath="/Attacks/Attack/Name" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="8" uniqueName="Class_Multiplier" name="Class Multiplier" dataDxfId="73">
+    <tableColumn id="8" uniqueName="Class_Multiplier" name="Class Multiplier" dataDxfId="72">
       <xmlColumnPr mapId="68" xpath="/Attacks/Attack/Class_Multiplier" xmlDataType="double"/>
     </tableColumn>
-    <tableColumn id="6" uniqueName="Stats_Low_Multiplier" name="Stats Low Multiplier" dataDxfId="72">
+    <tableColumn id="6" uniqueName="Stats_Low_Multiplier" name="Stats Low Multiplier" dataDxfId="71">
       <xmlColumnPr mapId="68" xpath="/Attacks/Attack/Stats_Low_Multiplier" xmlDataType="double"/>
     </tableColumn>
-    <tableColumn id="7" uniqueName="Stats_High_Multiplier" name="Stats High Multiplier" dataDxfId="71">
+    <tableColumn id="7" uniqueName="Stats_High_Multiplier" name="Stats High Multiplier" dataDxfId="70">
       <xmlColumnPr mapId="68" xpath="/Attacks/Attack/Stats_High_Multiplier" xmlDataType="double"/>
     </tableColumn>
-    <tableColumn id="2" uniqueName="HP_Damage" name="HP Damage" dataDxfId="70">
+    <tableColumn id="2" uniqueName="HP_Damage" name="HP Damage" dataDxfId="69">
       <xmlColumnPr mapId="68" xpath="/Attacks/Attack/HP_Damage" xmlDataType="double"/>
     </tableColumn>
-    <tableColumn id="3" uniqueName="Hit_Probability" name="Hit Probability" dataDxfId="69">
+    <tableColumn id="3" uniqueName="Hit_Probability" name="Hit Probability" dataDxfId="68">
       <xmlColumnPr mapId="68" xpath="/Attacks/Attack/Hit_Probability" xmlDataType="double"/>
     </tableColumn>
-    <tableColumn id="4" uniqueName="Effect" name="Effect" dataDxfId="68">
+    <tableColumn id="4" uniqueName="Effect" name="Effect" dataDxfId="67">
       <xmlColumnPr mapId="68" xpath="/Attacks/Attack/Effect" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="5" uniqueName="x" name="x" dataDxfId="67">
+    <tableColumn id="5" uniqueName="x" name="x" dataDxfId="66">
       <xmlColumnPr mapId="68" xpath="/Attacks/Attack/x" xmlDataType="double"/>
     </tableColumn>
   </tableColumns>
@@ -3832,46 +3832,46 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="A1:M13" tableType="xml" totalsRowShown="0" headerRowDxfId="66" dataDxfId="64" headerRowBorderDxfId="65" tableBorderDxfId="63" connectionId="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="A1:M13" tableType="xml" totalsRowShown="0" headerRowDxfId="65" dataDxfId="63" headerRowBorderDxfId="64" tableBorderDxfId="62" connectionId="21">
   <autoFilter ref="A1:M13"/>
   <tableColumns count="13">
-    <tableColumn id="1" uniqueName="Name" name="Name" dataDxfId="62">
+    <tableColumn id="1" uniqueName="Name" name="Name" dataDxfId="61">
       <xmlColumnPr mapId="71" xpath="/Monsters/Monster/Name" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="2" uniqueName="Level" name="Level" dataDxfId="61">
+    <tableColumn id="2" uniqueName="Level" name="Level" dataDxfId="60">
       <xmlColumnPr mapId="71" xpath="/Monsters/Monster/Level" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="14" uniqueName="Class_Multiplier" name="Class Multiplier" dataDxfId="60">
+    <tableColumn id="14" uniqueName="Class_Multiplier" name="Class Multiplier" dataDxfId="59">
       <xmlColumnPr mapId="71" xpath="/Monsters/Monster/Class_Multiplier" xmlDataType="double"/>
     </tableColumn>
-    <tableColumn id="10" uniqueName="Stats_Low_Multiplier" name="Stats Low Multiplier" dataDxfId="59">
+    <tableColumn id="10" uniqueName="Stats_Low_Multiplier" name="Stats Low Multiplier" dataDxfId="58">
       <xmlColumnPr mapId="71" xpath="/Monsters/Monster/Stats_Low_Multiplier" xmlDataType="double"/>
     </tableColumn>
-    <tableColumn id="13" uniqueName="Stats_High_Multiplier" name="Stats High Multiplier" dataDxfId="58">
+    <tableColumn id="13" uniqueName="Stats_High_Multiplier" name="Stats High Multiplier" dataDxfId="57">
       <xmlColumnPr mapId="71" xpath="/Monsters/Monster/Stats_High_Multiplier" xmlDataType="double"/>
     </tableColumn>
-    <tableColumn id="3" uniqueName="HP" name="HP" dataDxfId="57">
+    <tableColumn id="3" uniqueName="HP" name="HP" dataDxfId="56">
       <xmlColumnPr mapId="71" xpath="/Monsters/Monster/HP" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="4" uniqueName="Strength" name="Strength" dataDxfId="56">
+    <tableColumn id="4" uniqueName="Strength" name="Strength" dataDxfId="55">
       <xmlColumnPr mapId="71" xpath="/Monsters/Monster/Strength" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="5" uniqueName="Speed" name="Speed" dataDxfId="55">
+    <tableColumn id="5" uniqueName="Speed" name="Speed" dataDxfId="54">
       <xmlColumnPr mapId="71" xpath="/Monsters/Monster/Speed" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="6" uniqueName="Accuracy" name="Accuracy" dataDxfId="54">
+    <tableColumn id="6" uniqueName="Accuracy" name="Accuracy" dataDxfId="53">
       <xmlColumnPr mapId="71" xpath="/Monsters/Monster/Accuracy" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="7" uniqueName="Kill_Bonus_Type" name="Kill Bonus Type" dataDxfId="53">
+    <tableColumn id="7" uniqueName="Kill_Bonus_Type" name="Kill Bonus Type" dataDxfId="52">
       <xmlColumnPr mapId="71" xpath="/Monsters/Monster/Kill_Bonus_Type" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="8" uniqueName="Kill_Bonus_Low" name="Kill Bonus Low" dataDxfId="52">
+    <tableColumn id="8" uniqueName="Kill_Bonus_Low" name="Kill Bonus Low" dataDxfId="51">
       <xmlColumnPr mapId="71" xpath="/Monsters/Monster/Kill_Bonus_Low" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="9" uniqueName="Kill_Bonus_High" name="Kill Bonus High" dataDxfId="51">
+    <tableColumn id="9" uniqueName="Kill_Bonus_High" name="Kill Bonus High" dataDxfId="50">
       <xmlColumnPr mapId="71" xpath="/Monsters/Monster/Kill_Bonus_High" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="11" uniqueName="Image" name="Image" dataDxfId="50">
+    <tableColumn id="11" uniqueName="Image" name="Image" dataDxfId="49">
       <xmlColumnPr mapId="71" xpath="/Monsters/Monster/Image" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
@@ -3880,37 +3880,37 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:J16" tableType="xml" totalsRowShown="0" headerRowDxfId="49" dataDxfId="47" headerRowBorderDxfId="48" tableBorderDxfId="46" totalsRowBorderDxfId="45" connectionId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:J16" tableType="xml" totalsRowShown="0" headerRowDxfId="48" dataDxfId="46" headerRowBorderDxfId="47" tableBorderDxfId="45" totalsRowBorderDxfId="44" connectionId="3">
   <autoFilter ref="A1:J16"/>
   <tableColumns count="10">
-    <tableColumn id="1" uniqueName="Name" name="Name" dataDxfId="44">
+    <tableColumn id="1" uniqueName="Name" name="Name" dataDxfId="43">
       <xmlColumnPr mapId="74" xpath="/Armaments/Armament/Name" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="9" uniqueName="Item_Class" name="Item Class" dataDxfId="43">
+    <tableColumn id="9" uniqueName="Item_Class" name="Item Class" dataDxfId="42">
       <xmlColumnPr mapId="74" xpath="/Armaments/Armament/Item_Class" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="10" uniqueName="Class_Multiplier" name="Class Multiplier" dataDxfId="42">
+    <tableColumn id="10" uniqueName="Class_Multiplier" name="Class Multiplier" dataDxfId="41">
       <xmlColumnPr mapId="74" xpath="/Armaments/Armament/Class_Multiplier" xmlDataType="double"/>
     </tableColumn>
-    <tableColumn id="6" uniqueName="Stats_Low_Multiplier" name="Stats Low Multiplier" dataDxfId="41">
+    <tableColumn id="6" uniqueName="Stats_Low_Multiplier" name="Stats Low Multiplier" dataDxfId="40">
       <xmlColumnPr mapId="74" xpath="/Armaments/Armament/Stats_Low_Multiplier" xmlDataType="double"/>
     </tableColumn>
-    <tableColumn id="11" uniqueName="Stats_High_Multiplier" name="Stats High Multiplier" dataDxfId="40">
+    <tableColumn id="11" uniqueName="Stats_High_Multiplier" name="Stats High Multiplier" dataDxfId="39">
       <xmlColumnPr mapId="74" xpath="/Armaments/Armament/Stats_High_Multiplier" xmlDataType="double"/>
     </tableColumn>
-    <tableColumn id="2" uniqueName="Armor" name="Armor" dataDxfId="39">
+    <tableColumn id="2" uniqueName="Armor" name="Armor" dataDxfId="38">
       <xmlColumnPr mapId="74" xpath="/Armaments/Armament/Armor" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="3" uniqueName="Speed" name="Speed" dataDxfId="38">
+    <tableColumn id="3" uniqueName="Speed" name="Speed" dataDxfId="37">
       <xmlColumnPr mapId="74" xpath="/Armaments/Armament/Speed" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="4" uniqueName="Type" name="Type" dataDxfId="37">
+    <tableColumn id="4" uniqueName="Type" name="Type" dataDxfId="36">
       <xmlColumnPr mapId="74" xpath="/Armaments/Armament/Type" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="5" uniqueName="Bonus" name="Bonus" dataDxfId="36">
+    <tableColumn id="5" uniqueName="Bonus" name="Bonus" dataDxfId="35">
       <xmlColumnPr mapId="74" xpath="/Armaments/Armament/Bonus" xmlDataType="double"/>
     </tableColumn>
-    <tableColumn id="7" uniqueName="Image" name="Image" dataDxfId="35">
+    <tableColumn id="7" uniqueName="Image" name="Image" dataDxfId="34">
       <xmlColumnPr mapId="74" xpath="/Armaments/Armament/Image" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
@@ -3919,43 +3919,43 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:L11" tableType="xml" totalsRowShown="0" headerRowDxfId="34" dataDxfId="32" headerRowBorderDxfId="33" tableBorderDxfId="31" totalsRowBorderDxfId="30" connectionId="32">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:L11" tableType="xml" totalsRowShown="0" headerRowDxfId="33" dataDxfId="31" headerRowBorderDxfId="32" tableBorderDxfId="30" totalsRowBorderDxfId="29" connectionId="32">
   <autoFilter ref="A1:L11"/>
   <tableColumns count="12">
-    <tableColumn id="1" uniqueName="Name" name="Name" dataDxfId="29">
+    <tableColumn id="1" uniqueName="Name" name="Name" dataDxfId="28">
       <xmlColumnPr mapId="75" xpath="/Potions/Potion/Name" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="10" uniqueName="Item_Class" name="Item Class" dataDxfId="28">
+    <tableColumn id="10" uniqueName="Item_Class" name="Item Class" dataDxfId="27">
       <xmlColumnPr mapId="75" xpath="/Potions/Potion/Item_Class" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="11" uniqueName="Class_Multiplier" name="Class Multiplier" dataDxfId="27">
+    <tableColumn id="11" uniqueName="Class_Multiplier" name="Class Multiplier" dataDxfId="26">
       <xmlColumnPr mapId="75" xpath="/Potions/Potion/Class_Multiplier" xmlDataType="double"/>
     </tableColumn>
-    <tableColumn id="12" uniqueName="Stats_Low_Multiplier" name="Stats Low Multiplier" dataDxfId="26">
+    <tableColumn id="12" uniqueName="Stats_Low_Multiplier" name="Stats Low Multiplier" dataDxfId="25">
       <xmlColumnPr mapId="75" xpath="/Potions/Potion/Stats_Low_Multiplier" xmlDataType="double"/>
     </tableColumn>
-    <tableColumn id="13" uniqueName="Stats_High_Multiplier" name="Stats High Multiplier" dataDxfId="25">
+    <tableColumn id="13" uniqueName="Stats_High_Multiplier" name="Stats High Multiplier" dataDxfId="24">
       <xmlColumnPr mapId="75" xpath="/Potions/Potion/Stats_High_Multiplier" xmlDataType="double"/>
     </tableColumn>
-    <tableColumn id="2" uniqueName="Description" name="Description" dataDxfId="24">
+    <tableColumn id="2" uniqueName="Description" name="Description" dataDxfId="23">
       <xmlColumnPr mapId="75" xpath="/Potions/Potion/Description" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="3" uniqueName="Target" name="Target" dataDxfId="23">
+    <tableColumn id="3" uniqueName="Target" name="Target" dataDxfId="22">
       <xmlColumnPr mapId="75" xpath="/Potions/Potion/Target" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="4" uniqueName="Effect" name="Effect" dataDxfId="22">
+    <tableColumn id="4" uniqueName="Effect" name="Effect" dataDxfId="21">
       <xmlColumnPr mapId="75" xpath="/Potions/Potion/Effect" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="5" uniqueName="Mode" name="Mode" dataDxfId="21">
+    <tableColumn id="5" uniqueName="Mode" name="Mode" dataDxfId="20">
       <xmlColumnPr mapId="75" xpath="/Potions/Potion/Mode" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="6" uniqueName="x" name="x" dataDxfId="20">
+    <tableColumn id="6" uniqueName="x" name="x" dataDxfId="19">
       <xmlColumnPr mapId="75" xpath="/Potions/Potion/x" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="7" uniqueName="n" name="n" dataDxfId="19">
+    <tableColumn id="7" uniqueName="n" name="n" dataDxfId="18">
       <xmlColumnPr mapId="75" xpath="/Potions/Potion/n" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="8" uniqueName="Image" name="Image" dataDxfId="18">
+    <tableColumn id="8" uniqueName="Image" name="Image" dataDxfId="17">
       <xmlColumnPr mapId="75" xpath="/Potions/Potion/Image" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
@@ -3964,47 +3964,47 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:M9" tableType="xml" totalsRowShown="0" headerRowDxfId="17" dataDxfId="15" headerRowBorderDxfId="16" tableBorderDxfId="14" connectionId="57">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:M9" tableType="xml" totalsRowShown="0" headerRowDxfId="16" dataDxfId="14" headerRowBorderDxfId="15" tableBorderDxfId="13" connectionId="57">
   <autoFilter ref="A1:M9"/>
   <tableColumns count="13">
-    <tableColumn id="1" uniqueName="Name" name="Name" dataDxfId="13">
+    <tableColumn id="1" uniqueName="Name" name="Name" dataDxfId="12">
       <xmlColumnPr mapId="76" xpath="/Weapons/Weapon/Name" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="11" uniqueName="Item_Class" name="Item Class" dataDxfId="12">
+    <tableColumn id="11" uniqueName="Item_Class" name="Item Class" dataDxfId="11">
       <xmlColumnPr mapId="76" xpath="/Weapons/Weapon/Item_Class" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="12" uniqueName="Class_Multiplier" name="Class Multiplier" dataDxfId="11">
+    <tableColumn id="12" uniqueName="Class_Multiplier" name="Class Multiplier" dataDxfId="10">
       <xmlColumnPr mapId="76" xpath="/Weapons/Weapon/Class_Multiplier" xmlDataType="double"/>
     </tableColumn>
-    <tableColumn id="13" uniqueName="Stats_Low_Multiplier" name="Stats Low Multiplier" dataDxfId="10">
+    <tableColumn id="13" uniqueName="Stats_Low_Multiplier" name="Stats Low Multiplier" dataDxfId="9">
       <xmlColumnPr mapId="76" xpath="/Weapons/Weapon/Stats_Low_Multiplier" xmlDataType="double"/>
     </tableColumn>
-    <tableColumn id="14" uniqueName="Stats_High_Multiplier" name="Stats High Multiplier" dataDxfId="9">
+    <tableColumn id="14" uniqueName="Stats_High_Multiplier" name="Stats High Multiplier" dataDxfId="8">
       <xmlColumnPr mapId="76" xpath="/Weapons/Weapon/Stats_High_Multiplier" xmlDataType="double"/>
     </tableColumn>
-    <tableColumn id="2" uniqueName="Attack" name="Attack" dataDxfId="8">
+    <tableColumn id="2" uniqueName="Attack" name="Attack" dataDxfId="7">
       <xmlColumnPr mapId="76" xpath="/Weapons/Weapon/Attack" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="3" uniqueName="Speed" name="Speed" dataDxfId="7">
+    <tableColumn id="3" uniqueName="Speed" name="Speed" dataDxfId="6">
       <xmlColumnPr mapId="76" xpath="/Weapons/Weapon/Speed" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="4" uniqueName="Accuracy" name="Accuracy" dataDxfId="6">
+    <tableColumn id="4" uniqueName="Accuracy" name="Accuracy" dataDxfId="5">
       <xmlColumnPr mapId="76" xpath="/Weapons/Weapon/Accuracy" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="5" uniqueName="Defence" name="Defence" dataDxfId="5">
+    <tableColumn id="5" uniqueName="Defence" name="Defence" dataDxfId="4">
       <calculatedColumnFormula>"-"</calculatedColumnFormula>
       <xmlColumnPr mapId="76" xpath="/Weapons/Weapon/Defence" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="6" uniqueName="Slots" name="Slots" dataDxfId="4">
+    <tableColumn id="6" uniqueName="Slots" name="Slots" dataDxfId="3">
       <xmlColumnPr mapId="76" xpath="/Weapons/Weapon/Slots" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="7" uniqueName="Max" name="Max" dataDxfId="3">
+    <tableColumn id="7" uniqueName="Max" name="Max" dataDxfId="2">
       <xmlColumnPr mapId="76" xpath="/Weapons/Weapon/Max" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="8" uniqueName="Type" name="Type" dataDxfId="2">
+    <tableColumn id="8" uniqueName="Type" name="Type" dataDxfId="1">
       <xmlColumnPr mapId="76" xpath="/Weapons/Weapon/Type" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="9" uniqueName="Image" name="Image" dataDxfId="1">
+    <tableColumn id="9" uniqueName="Image" name="Image" dataDxfId="0">
       <xmlColumnPr mapId="76" xpath="/Weapons/Weapon/Image" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
@@ -4013,9 +4013,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa-Design">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Larissa">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -4053,7 +4053,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Larissa">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -4087,7 +4087,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -4122,10 +4121,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Larissa">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -4298,28 +4296,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
     </row>
   </sheetData>
@@ -4328,15 +4326,15 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:R26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="Q31" sqref="Q31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="31" style="21" customWidth="1"/>
     <col min="2" max="2" width="25.140625" style="21" bestFit="1" customWidth="1"/>
@@ -4358,17 +4356,17 @@
     <col min="18" max="18" width="28.5703125" style="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" ht="15.75" thickBot="1">
       <c r="A1" s="22"/>
       <c r="B1" s="22"/>
       <c r="C1" s="82" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="D1" s="83"/>
       <c r="E1" s="83"/>
       <c r="F1" s="84"/>
       <c r="G1" s="82" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="H1" s="83"/>
       <c r="I1" s="83"/>
@@ -4376,7 +4374,7 @@
       <c r="K1" s="79"/>
       <c r="L1" s="29"/>
       <c r="M1" s="86" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="N1" s="87"/>
       <c r="O1" s="87"/>
@@ -4384,68 +4382,68 @@
       <c r="Q1" s="36"/>
       <c r="R1" s="38"/>
     </row>
-    <row r="2" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" ht="15.75" thickBot="1">
       <c r="A2" s="23" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="B2" s="24" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="C2" s="25" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="D2" s="25" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="E2" s="25" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="F2" s="25" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="G2" s="25" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="H2" s="35" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="I2" s="35" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="J2" s="35" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="K2" s="78" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="L2" s="30" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="M2" s="32" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="N2" s="32" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="O2" s="32" t="s">
+        <v>139</v>
+      </c>
+      <c r="P2" s="32" t="s">
+        <v>140</v>
+      </c>
+      <c r="Q2" s="37" t="s">
         <v>148</v>
       </c>
-      <c r="P2" s="32" t="s">
-        <v>149</v>
-      </c>
-      <c r="Q2" s="37" t="s">
-        <v>157</v>
-      </c>
       <c r="R2" s="39" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18">
       <c r="A3" s="21" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="C3" s="26">
         <v>1</v>
@@ -4493,15 +4491,15 @@
         <v>3</v>
       </c>
       <c r="R3" s="21" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18">
       <c r="A4" s="21" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="C4" s="26">
         <v>1</v>
@@ -4549,15 +4547,15 @@
         <v>2</v>
       </c>
       <c r="R4" s="21" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18">
       <c r="A5" s="21" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="C5" s="26">
         <v>1</v>
@@ -4605,15 +4603,15 @@
         <v>2</v>
       </c>
       <c r="R5" s="21" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18">
       <c r="A6" s="21" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="C6" s="26">
         <v>1</v>
@@ -4661,15 +4659,15 @@
         <v>1</v>
       </c>
       <c r="R6" s="21" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18">
       <c r="A7" s="21" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="C7" s="26">
         <v>1</v>
@@ -4717,15 +4715,15 @@
         <v>1</v>
       </c>
       <c r="R7" s="21" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18">
       <c r="A8" s="21" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="B8" s="21" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="C8" s="26">
         <v>1</v>
@@ -4773,21 +4771,21 @@
         <v>5</v>
       </c>
       <c r="R8" s="21" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18">
       <c r="A10" s="21" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="C10" s="85" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="D10" s="85"/>
       <c r="E10" s="85"/>
       <c r="F10" s="85"/>
       <c r="G10" s="85" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="H10" s="85"/>
       <c r="I10" s="85"/>
@@ -4796,15 +4794,15 @@
       <c r="L10" s="31"/>
       <c r="M10" s="33"/>
       <c r="N10" s="85" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="O10" s="85"/>
       <c r="P10" s="85"/>
       <c r="Q10" s="33"/>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18">
       <c r="A11" s="21" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="G11" s="34"/>
       <c r="H11" s="34"/>
@@ -4818,12 +4816,12 @@
       <c r="P11" s="34"/>
       <c r="Q11" s="34"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18">
       <c r="A12" s="21" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="G12" s="34" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="H12" s="34"/>
       <c r="I12" s="34"/>
@@ -4832,15 +4830,15 @@
       <c r="L12" s="28"/>
       <c r="M12" s="34"/>
       <c r="N12" s="34" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="O12" s="34"/>
       <c r="P12" s="34"/>
       <c r="Q12" s="34"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18">
       <c r="A13" s="21" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="G13" s="34"/>
       <c r="H13" s="34"/>
@@ -4850,15 +4848,15 @@
       <c r="L13" s="28"/>
       <c r="M13" s="34"/>
       <c r="N13" s="34" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="O13" s="34"/>
       <c r="P13" s="34"/>
       <c r="Q13" s="34"/>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18">
       <c r="G14" s="85" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="H14" s="85"/>
       <c r="I14" s="85"/>
@@ -4871,12 +4869,12 @@
       <c r="P14" s="33"/>
       <c r="Q14" s="33"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18">
       <c r="A15" s="21" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="G15" s="85" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="H15" s="85"/>
       <c r="I15" s="85"/>
@@ -4889,9 +4887,9 @@
       <c r="P15" s="33"/>
       <c r="Q15" s="33"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18">
       <c r="G16" s="85" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="H16" s="85"/>
       <c r="I16" s="85"/>
@@ -4904,9 +4902,9 @@
       <c r="P16" s="33"/>
       <c r="Q16" s="33"/>
     </row>
-    <row r="17" spans="7:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="7:17">
       <c r="G17" s="85" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="H17" s="85"/>
       <c r="I17" s="85"/>
@@ -4919,9 +4917,9 @@
       <c r="P17" s="33"/>
       <c r="Q17" s="33"/>
     </row>
-    <row r="18" spans="7:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="7:17">
       <c r="G18" s="85" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="H18" s="85"/>
       <c r="I18" s="85"/>
@@ -4934,9 +4932,9 @@
       <c r="P18" s="33"/>
       <c r="Q18" s="33"/>
     </row>
-    <row r="20" spans="7:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="7:17">
       <c r="G20" s="85" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="H20" s="85"/>
       <c r="I20" s="85"/>
@@ -4949,9 +4947,9 @@
       <c r="P20" s="33"/>
       <c r="Q20" s="33"/>
     </row>
-    <row r="21" spans="7:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="7:17">
       <c r="G21" s="85" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="H21" s="85"/>
       <c r="I21" s="85"/>
@@ -4964,14 +4962,14 @@
       <c r="P21" s="33"/>
       <c r="Q21" s="33"/>
     </row>
-    <row r="23" spans="7:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="7:17">
       <c r="G23" s="26" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="24" spans="7:17" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="24" spans="7:17">
       <c r="G24" s="85" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="H24" s="85"/>
       <c r="I24" s="85"/>
@@ -4984,9 +4982,9 @@
       <c r="P24" s="33"/>
       <c r="Q24" s="33"/>
     </row>
-    <row r="25" spans="7:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="7:17">
       <c r="G25" s="85" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="H25" s="85"/>
       <c r="I25" s="85"/>
@@ -4999,9 +4997,9 @@
       <c r="P25" s="33"/>
       <c r="Q25" s="33"/>
     </row>
-    <row r="26" spans="7:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="7:17">
       <c r="G26" s="85" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="H26" s="85"/>
       <c r="I26" s="85"/>
@@ -5042,7 +5040,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5050,7 +5048,7 @@
       <selection pane="topRight" activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="21" customWidth="1"/>
     <col min="2" max="2" width="20" style="27" customWidth="1"/>
@@ -5062,24 +5060,24 @@
     <col min="8" max="8" width="5.85546875" style="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="15" customHeight="1" thickBot="1">
       <c r="A1" s="40" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="B1" s="42" t="s">
+        <v>141</v>
+      </c>
+      <c r="C1" s="42" t="s">
+        <v>149</v>
+      </c>
+      <c r="D1" s="42" t="s">
         <v>150</v>
       </c>
-      <c r="C1" s="42" t="s">
-        <v>158</v>
-      </c>
-      <c r="D1" s="42" t="s">
-        <v>159</v>
-      </c>
       <c r="E1" s="43" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="F1" s="43" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="G1" s="48" t="s">
         <v>16</v>
@@ -5088,9 +5086,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2" s="13" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="B2" s="44">
         <v>1</v>
@@ -5114,9 +5112,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="A3" s="14" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="B3" s="44">
         <v>1</v>
@@ -5140,9 +5138,9 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="A4" s="14" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="B4" s="44">
         <v>1</v>
@@ -5166,9 +5164,9 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="A5" s="15" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="B5" s="81">
         <v>1</v>
@@ -5192,9 +5190,9 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="A7" s="41" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="B7" s="28"/>
       <c r="C7" s="28"/>
@@ -5203,9 +5201,9 @@
       <c r="F7" s="28"/>
       <c r="G7" s="49"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8">
       <c r="A8" s="41" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="B8" s="28"/>
       <c r="C8" s="28"/>
@@ -5222,7 +5220,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5230,7 +5228,7 @@
       <selection pane="topRight" activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="17.28515625" style="21" customWidth="1"/>
     <col min="2" max="2" width="19.5703125" style="21" customWidth="1"/>
@@ -5247,24 +5245,24 @@
     <col min="13" max="13" width="34" style="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="15" customHeight="1" thickBot="1">
       <c r="A1" s="50" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="B1" s="51" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="C1" s="54" t="s">
+        <v>141</v>
+      </c>
+      <c r="D1" s="54" t="s">
+        <v>149</v>
+      </c>
+      <c r="E1" s="54" t="s">
         <v>150</v>
       </c>
-      <c r="D1" s="54" t="s">
-        <v>158</v>
-      </c>
-      <c r="E1" s="54" t="s">
-        <v>159</v>
-      </c>
       <c r="F1" s="57" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="G1" s="57" t="s">
         <v>22</v>
@@ -5276,24 +5274,24 @@
         <v>24</v>
       </c>
       <c r="J1" s="53" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="K1" s="61" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="L1" s="61" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="M1" s="50" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="15" customHeight="1">
       <c r="A2" s="18" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="C2" s="55">
         <v>1</v>
@@ -5326,15 +5324,15 @@
         <v>4</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="15" customHeight="1">
       <c r="A3" s="19" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="C3" s="55">
         <v>1</v>
@@ -5367,15 +5365,15 @@
         <v>2</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="15" customHeight="1">
       <c r="A4" s="19" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="C4" s="55">
         <v>1</v>
@@ -5408,15 +5406,15 @@
         <v>2</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="15" customHeight="1">
       <c r="A5" s="19" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="C5" s="55">
         <v>1</v>
@@ -5449,15 +5447,15 @@
         <v>2</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="15" customHeight="1">
       <c r="A6" s="19" t="s">
         <v>1</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="C6" s="55">
         <v>1</v>
@@ -5490,15 +5488,15 @@
         <v>2</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="15" customHeight="1">
       <c r="A7" s="19" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="C7" s="55">
         <v>1</v>
@@ -5531,15 +5529,15 @@
         <v>5</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="15" customHeight="1">
       <c r="A8" s="19" t="s">
         <v>3</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="C8" s="55">
         <v>1</v>
@@ -5572,15 +5570,15 @@
         <v>7</v>
       </c>
       <c r="M8" s="3" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="15" customHeight="1">
       <c r="A9" s="19" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="C9" s="55">
         <v>1</v>
@@ -5613,15 +5611,15 @@
         <v>5</v>
       </c>
       <c r="M9" s="3" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="15" customHeight="1">
       <c r="A10" s="19" t="s">
         <v>4</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="C10" s="55">
         <v>1</v>
@@ -5654,15 +5652,15 @@
         <v>10</v>
       </c>
       <c r="M10" s="3" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="15" customHeight="1">
       <c r="A11" s="19" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="C11" s="55">
         <v>1</v>
@@ -5695,15 +5693,15 @@
         <v>30</v>
       </c>
       <c r="M11" s="3" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="15" customHeight="1">
       <c r="A12" s="19" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="C12" s="55">
         <v>1</v>
@@ -5736,15 +5734,15 @@
         <v>30</v>
       </c>
       <c r="M12" s="3" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="15" customHeight="1">
       <c r="A13" s="20" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="C13" s="80">
         <v>1</v>
@@ -5777,37 +5775,37 @@
         <v>30</v>
       </c>
       <c r="M13" s="3" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
       <c r="A15" s="52" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="B15" s="52" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="C15" s="56"/>
       <c r="D15" s="56"/>
       <c r="E15" s="56"/>
     </row>
-    <row r="16" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="15" customHeight="1">
       <c r="A16" s="52" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="B16" s="52" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="C16" s="56"/>
       <c r="D16" s="56"/>
       <c r="E16" s="56"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5">
       <c r="A17" s="52" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="B17" s="52" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="C17" s="56"/>
       <c r="D17" s="56"/>
@@ -5823,7 +5821,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5831,7 +5829,7 @@
       <selection pane="topRight" activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20.7109375" style="21" customWidth="1"/>
     <col min="2" max="2" width="14.42578125" style="21" customWidth="1"/>
@@ -5845,44 +5843,44 @@
     <col min="10" max="10" width="55" style="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="15" customHeight="1" thickBot="1">
       <c r="A1" s="50" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="B1" s="50" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="C1" s="63" t="s">
+        <v>141</v>
+      </c>
+      <c r="D1" s="63" t="s">
+        <v>149</v>
+      </c>
+      <c r="E1" s="63" t="s">
         <v>150</v>
       </c>
-      <c r="D1" s="63" t="s">
-        <v>158</v>
-      </c>
-      <c r="E1" s="63" t="s">
-        <v>159</v>
-      </c>
       <c r="F1" s="57" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="G1" s="57" t="s">
         <v>23</v>
       </c>
       <c r="H1" s="51" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="I1" s="54" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="J1" s="50" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="15" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="C2" s="64">
         <v>1</v>
@@ -5902,21 +5900,21 @@
         <v>13.333333333333334</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="I2" s="64">
         <v>0.1</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="15" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="C3" s="65">
         <v>1</v>
@@ -5934,21 +5932,21 @@
         <v>20</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="I3" s="65">
         <v>0.1</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="15" customHeight="1">
       <c r="A4" s="1" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="C4" s="64">
         <v>1</v>
@@ -5968,21 +5966,21 @@
         <v>6.666666666666667</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="I4" s="65">
         <v>0.1</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="15" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="C5" s="65">
         <v>1</v>
@@ -6002,21 +6000,21 @@
         <v>10</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="I5" s="65">
         <v>0.1</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="15" customHeight="1">
       <c r="A6" s="1" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="C6" s="64">
         <v>1</v>
@@ -6036,21 +6034,21 @@
         <v>6.666666666666667</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="I6" s="65">
         <v>0.1</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="15" customHeight="1">
       <c r="A7" s="1" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="C7" s="65">
         <v>1</v>
@@ -6070,21 +6068,21 @@
         <v>16.666666666666668</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="I7" s="65">
         <v>0.15</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="15" customHeight="1">
       <c r="A8" s="1" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="C8" s="64">
         <v>1</v>
@@ -6102,21 +6100,21 @@
         <v>25</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="I8" s="65">
         <v>0.15</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="15" customHeight="1">
       <c r="A9" s="1" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="C9" s="65">
         <v>1</v>
@@ -6136,21 +6134,21 @@
         <v>8.3333333333333339</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="I9" s="65">
         <v>0.15</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="15" customHeight="1">
       <c r="A10" s="1" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="C10" s="64">
         <v>1</v>
@@ -6170,21 +6168,21 @@
         <v>12.5</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="I10" s="65">
         <v>0.15</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="15" customHeight="1">
       <c r="A11" s="1" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="C11" s="65">
         <v>1</v>
@@ -6204,21 +6202,21 @@
         <v>8.3333333333333339</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="I11" s="65">
         <v>0.15</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="15" customHeight="1">
       <c r="A12" s="1" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="C12" s="64">
         <v>1</v>
@@ -6238,21 +6236,21 @@
         <v>20</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="I12" s="65">
         <v>0.2</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="15" customHeight="1">
       <c r="A13" s="1" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="C13" s="65">
         <v>1</v>
@@ -6270,21 +6268,21 @@
         <v>30</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="I13" s="65">
         <v>0.2</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="15" customHeight="1">
       <c r="A14" s="1" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="C14" s="64">
         <v>1</v>
@@ -6304,21 +6302,21 @@
         <v>10</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="I14" s="65">
         <v>0.2</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="15" customHeight="1">
       <c r="A15" s="1" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="C15" s="65">
         <v>1</v>
@@ -6338,21 +6336,21 @@
         <v>15</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="I15" s="65">
         <v>0.2</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="15" customHeight="1">
       <c r="A16" s="4" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="C16" s="64">
         <v>1</v>
@@ -6372,21 +6370,21 @@
         <v>10</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="I16" s="66">
         <v>0.2</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="18" spans="3:7">
       <c r="C18" s="27" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="G18" s="26" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -6399,15 +6397,15 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F19" sqref="F19"/>
+      <selection pane="topRight" activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="16.7109375" style="21" customWidth="1"/>
     <col min="2" max="2" width="14.7109375" style="21" customWidth="1"/>
@@ -6423,24 +6421,24 @@
     <col min="12" max="12" width="54.85546875" style="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="15" customHeight="1" thickBot="1">
       <c r="A1" s="50" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="B1" s="50" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="C1" s="63" t="s">
+        <v>141</v>
+      </c>
+      <c r="D1" s="63" t="s">
+        <v>149</v>
+      </c>
+      <c r="E1" s="63" t="s">
         <v>150</v>
       </c>
-      <c r="D1" s="63" t="s">
-        <v>158</v>
-      </c>
-      <c r="E1" s="63" t="s">
-        <v>159</v>
-      </c>
       <c r="F1" s="70" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="G1" s="70" t="s">
         <v>17</v>
@@ -6458,15 +6456,15 @@
         <v>6</v>
       </c>
       <c r="L1" s="50" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="C2" s="64">
         <v>1</v>
@@ -6478,7 +6476,7 @@
         <v>1.2</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>29</v>
+        <v>201</v>
       </c>
       <c r="G2" s="5" t="s">
         <v>8</v>
@@ -6497,15 +6495,15 @@
         <v>1</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="C3" s="65">
         <v>1</v>
@@ -6517,7 +6515,7 @@
         <v>1.2</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>30</v>
+        <v>202</v>
       </c>
       <c r="G3" s="6" t="s">
         <v>8</v>
@@ -6536,15 +6534,15 @@
         <v>5</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="C4" s="64">
         <v>1</v>
@@ -6556,7 +6554,7 @@
         <v>1.2</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G4" s="6" t="s">
         <v>8</v>
@@ -6574,15 +6572,15 @@
         <v>1</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
       <c r="A5" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="C5" s="65">
         <v>1</v>
@@ -6594,7 +6592,7 @@
         <v>1.2</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>32</v>
+        <v>203</v>
       </c>
       <c r="G5" s="6" t="s">
         <v>8</v>
@@ -6612,15 +6610,15 @@
         <v>5</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
       <c r="A6" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="C6" s="64">
         <v>1</v>
@@ -6632,7 +6630,7 @@
         <v>1.2</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>33</v>
+        <v>204</v>
       </c>
       <c r="G6" s="6" t="s">
         <v>8</v>
@@ -6650,15 +6648,15 @@
         <v>5</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
       <c r="A7" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="C7" s="65">
         <v>1</v>
@@ -6670,7 +6668,7 @@
         <v>1.2</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>34</v>
+        <v>205</v>
       </c>
       <c r="G7" s="6" t="s">
         <v>8</v>
@@ -6688,15 +6686,15 @@
         <v>5</v>
       </c>
       <c r="L7" s="3" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
       <c r="A8" s="7" t="s">
         <v>25</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="C8" s="64">
         <v>1</v>
@@ -6708,7 +6706,7 @@
         <v>1.2</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>35</v>
+        <v>206</v>
       </c>
       <c r="G8" s="6" t="s">
         <v>9</v>
@@ -6726,15 +6724,15 @@
         <v>5</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
       <c r="A9" s="7" t="s">
         <v>28</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="C9" s="65">
         <v>1</v>
@@ -6746,7 +6744,7 @@
         <v>1.2</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>36</v>
+        <v>207</v>
       </c>
       <c r="G9" s="6" t="s">
         <v>9</v>
@@ -6764,15 +6762,15 @@
         <v>5</v>
       </c>
       <c r="L9" s="3" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
       <c r="A10" s="7" t="s">
         <v>27</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="C10" s="64">
         <v>1</v>
@@ -6784,7 +6782,7 @@
         <v>1.2</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>37</v>
+        <v>208</v>
       </c>
       <c r="G10" s="6" t="s">
         <v>9</v>
@@ -6803,15 +6801,15 @@
         <v>5</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
       <c r="A11" s="8" t="s">
         <v>26</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="C11" s="65">
         <v>1</v>
@@ -6823,7 +6821,7 @@
         <v>1.2</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>38</v>
+        <v>209</v>
       </c>
       <c r="G11" s="9" t="s">
         <v>9</v>
@@ -6841,12 +6839,12 @@
         <v>5</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
       <c r="C13" s="27" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -6858,7 +6856,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6866,7 +6864,7 @@
       <selection pane="topRight" activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.85546875" style="21" customWidth="1"/>
     <col min="2" max="2" width="16.7109375" style="21" customWidth="1"/>
@@ -6881,24 +6879,24 @@
     <col min="13" max="13" width="55.42578125" style="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="15" customHeight="1" thickBot="1">
       <c r="A1" s="23" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="B1" s="23" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="C1" s="30" t="s">
+        <v>141</v>
+      </c>
+      <c r="D1" s="30" t="s">
+        <v>149</v>
+      </c>
+      <c r="E1" s="30" t="s">
         <v>150</v>
       </c>
-      <c r="D1" s="30" t="s">
-        <v>158</v>
-      </c>
-      <c r="E1" s="30" t="s">
-        <v>159</v>
-      </c>
       <c r="F1" s="35" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="G1" s="35" t="s">
         <v>23</v>
@@ -6907,24 +6905,24 @@
         <v>24</v>
       </c>
       <c r="I1" s="35" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="J1" s="35" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="K1" s="35" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="L1" s="76" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="M1" s="23" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
       <c r="A2" s="2" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>7</v>
@@ -6957,18 +6955,18 @@
         <v>2</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
       <c r="A3" s="1" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="C3" s="64">
         <v>1</v>
@@ -6998,18 +6996,18 @@
         <v>2</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="C4" s="64">
         <v>1</v>
@@ -7039,18 +7037,18 @@
         <v>2</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
       <c r="A5" s="1" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="C5" s="64">
         <v>1</v>
@@ -7080,18 +7078,18 @@
         <v>2</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
       <c r="A6" s="1" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="C6" s="64">
         <v>1</v>
@@ -7121,18 +7119,18 @@
         <v>1</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
       <c r="A7" s="1" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="C7" s="64">
         <v>1</v>
@@ -7162,18 +7160,18 @@
         <v>2</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
       <c r="A8" s="1" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="C8" s="64">
         <v>1</v>
@@ -7203,18 +7201,18 @@
         <v>1</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="M8" s="3" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
       <c r="A9" s="4" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="C9" s="64">
         <v>1</v>
@@ -7244,15 +7242,15 @@
         <v>1</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="M9" s="3" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
       <c r="C11" s="27" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>

</xml_diff>